<commit_message>
add statistics to view, modify and find new way to scrap blibli since the security mechanism has changed and previous method was not able to penerate the security layer
</commit_message>
<xml_diff>
--- a/ui_data/blibli.xlsx
+++ b/ui_data/blibli.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Product Data" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Product Data" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -432,13 +432,13 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="17" customWidth="1" min="1" max="1"/>
-    <col width="33" customWidth="1" min="2" max="2"/>
+    <col width="27" customWidth="1" min="2" max="2"/>
     <col width="58.33333333333334" customWidth="1" min="3" max="3"/>
-    <col width="97" customWidth="1" min="4" max="4"/>
+    <col width="147" customWidth="1" min="4" max="4"/>
     <col width="10" customWidth="1" min="5" max="5"/>
-    <col width="224" customWidth="1" min="6" max="6"/>
+    <col width="276" customWidth="1" min="6" max="6"/>
     <col width="8" customWidth="1" min="7" max="7"/>
-    <col width="559" customWidth="1" min="8" max="8"/>
+    <col width="582" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -486,7 +486,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>BLW-60022-01270</t>
+          <t>VAM-60047-00028</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -496,12 +496,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>BLYTHE</t>
+          <t>VAYA</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>BLYTHE Karet Rambut Pack Isi 5 pcs Karet Rambut Elastis Korea Cantik VCA Alhambra - Multi Color</t>
+          <t>Vaya Celana Dalam Wanita Art 105</t>
         </is>
       </c>
       <c r="E2" t="n">
@@ -509,60 +509,60 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/MTA-102263832/blythe_blythe_karet_rambut_pack_isi_5_pcs_karet_rambut_elastis_korea_cantik_vca_alhambra_-_multi_color_full02_pirek09q.jpeg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium//113/MTA-7946897/vaya_vaya_celana_dalam_wanita_art_105_full07_tsegjxpc.jpg</t>
         </is>
       </c>
       <c r="G2" t="n">
-        <v>5</v>
+        <v>4.8</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/blythe-karet-rambut-pack-isi-5-pcs-karet-rambut-elastis-korea-cantik-vca-alhambra-multi-color/ps--BLW-60022-01270?ds=BLW-60022-01270-00001&amp;source=SEARCH&amp;sid=1629777a4a0387e4&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC0ry844Ce9aEHITmMYpiMq+T2r7fOYNS0fn24lYkspaBl5vfrmHU5Q8bT/ocNrObpFesavfRnEsmWNUn9y9IGTPNbQv3e9jt8aL3d1v2xu9DKSzHz/PIkE4dvMq7nfYD/A+bVy57sPYICbagrfTX85ws4+rWZ7zCXM6RAaC0DCw0MKQ9PlM/Q98GUugQJNGaO371+Fx1GV9QkiSnx+YzhKM=&amp;cnc=false&amp;pickupPointCode=PP-3047949&amp;pid1=BLW-60022-01270</t>
+          <t>https://www.blibli.com/p/vaya-celana-dalam-wanita-art-105/ps--VAM-60047-00028?ds=VAM-60047-00028-00022&amp;source=SEARCH&amp;sid=eb3344a674df186d&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC0ry844Ce9aEHITmMYpiMq+T2r7fOYNS0fn24lYkspaBOiFJzBdj5bpigceDw0uA91esavfRnEsmWNUn9y9IGTPNbQv3e9jt8aL3d1v2xu9DKSzHz/PIkE4dvMq7nfYD/HuiZ47Lpn6Wymqd3CV70A8s4+rWZ7zCXM6RAaC0DCw0e2Pllk5UNg4gE0pn1fUaDcWA2XVscKi/tVwIPhWxnEMPPjVhhyLHi3omjt/pcgmB&amp;cnc=false&amp;pickupPointCode=PP-3191339&amp;pid1=VAM-60047-00028</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>NEB-60027-01137</t>
+          <t>INS-28338-00021</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Olahraga &amp; Aktivitas Luar Ruang</t>
+          <t>Fashion Pria</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>New Balance</t>
+          <t>Muscle Fit</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>New Balance Men Running Impact Run 5 Inch Short Celana Olahraga Pria [NEWAMS21268N]</t>
+          <t>Muscle Fit MFBX-110 Boxer Celana Dalam Pria - Hitam [3 Pcs]</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>390000</v>
+        <v>74307</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/MTA-96602598/new_balance_new_balance_men_running_impact_run_5_inch_short_celana_olahraga_pria_-newams21268n-_full02_sxuehwox.png</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium//109/MTA-15939099/muscle_fit_muscle_fit_mfbx-110_boxer_celana_dalam_pria_-_hitam_-3_pcs-_full04_b2eqjl6u.jpg</t>
         </is>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>4.6</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/new-balance-men-running-impact-run-5-inch-short-celana-olahraga-pria-newams21268n/ps--NEB-60027-01137?ds=NEB-60027-01137-00003&amp;source=SEARCH&amp;sid=1629777a4a0387e4&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC8ABEbUv77oGEmdGsuoM438H5hXXWkF0dKfPGTdZQcdlwOuwn8PMdUs21zBM0LtaAlesavfRnEsmWNUn9y9IGTPNbQv3e9jt8aL3d1v2xu9DKSzHz/PIkE4dvMq7nfYD/A+bVy57sPYICbagrfTX85wkO/esjvqoogVKmoFC5IfolouBECXZJM5fw2H9lFaTDkaTmXM5ymgQU76aQtitcsKDEC3cLXX0wtGQFaK7Z8yP&amp;cnc=false&amp;pickupPointCode=PP-3526013&amp;pid1=NEB-60027-01137</t>
+          <t>https://www.blibli.com/p/muscle-fit-mfbx-110-boxer-celana-dalam-pria-hitam-3-pcs/ps--INS-28338-00021?ds=INS-28338-00021-00005&amp;source=SEARCH&amp;sid=eb3344a674df186d&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC6+ofzQPca16/hNKbnSDAJ7iA6KyoMcwEkeRG65oyOFiCGlgPeK8rUlktyavu3C5T2lLxoLaHsRAJv8lj0ZJ+KKWyiBVV+ZSlXxNvPz9a8MHT9B348TZH4FhxuSDbhHbW94ZoZgYUZh/bnPUJo2NrB1YDqIYcOPQIbVM7pUbxxlrUYgNp1+TEJCf8Aed76MVhhAzI+1iWJG3a3RJebe09mkKDBhcJWU7Wh6Q+zs/xW9UK75dCgVySnSnFnHvJRwecg==&amp;cnc=false&amp;pickupPointCode=PP-3004512&amp;pid1=INS-28338-00021</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>FLM-22188-00903</t>
+          <t>EVO-70024-00184</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -572,35 +572,35 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Flyman</t>
+          <t>EVERNEXT</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Flyman Celana Dalam Pria Katun CD Briefs laki segitiga 1 Pcs FM 3378</t>
+          <t>EVERNEXT - CELANA BOXER CAVERO PRIA CELANA PENDEK SANTAI PRIA CELANA JOGGING RUNNING PRIA CELANA OLAHRAGA DDISTRO PRIA</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>30500</v>
+        <v>28000</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium//catalog-image/MTA-47588965/flyman_flyman_celana_dalam_pria_katun_cd_briefs_laki_segitiga_1_pcs_fm_3378_full01_jlj77yur.jpg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/MTA-78904222/evernext_evernext_-_celana_boxer_cavero_pria_celana_pendek_santai_pria_celana_jogging_running_pria_celana_olahraga_ddistro_pria_full01_f2j2m289.jpeg</t>
         </is>
       </c>
       <c r="G4" t="n">
-        <v>4.9</v>
+        <v>3.1</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/flyman-celana-dalam-pria-katun-cd-briefs-laki-segitiga-1-pcs-fm-3378/ps--FLM-22188-00903?ds=FLM-22188-00903-00001&amp;source=SEARCH&amp;sid=1629777a4a0387e4&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC+G4LZi2pi3YNLiDQiX+7EO/HAkxoVke7cxJ4LyInlLe6L7IRaSZ3iwh0M268aXvN1X6YqNL/N38iJlYkQlI2HD9cnB7A9Br96VNOoae/H1+UvM5rYQ2b7sWjAIjInNGfymSid4UzDSJt9ecE9c7PeUrDNQbMrsAMmfYB7gn+SuipPH0QkIWnpynVxqg5n9k7czb4iFkMm3ZXxtmElZqnPw=&amp;cnc=false&amp;pickupPointCode=FLM-22188-001&amp;pid1=FLM-22188-00903</t>
+          <t>https://www.blibli.com/p/evernext-celana-boxer-cavero-pria-celana-pendek-santai-pria-celana-jogging-running-pria-celana-olahraga-ddistro-pria/ps--EVO-70024-00184?ds=EVO-70024-00184-00001&amp;source=SEARCH&amp;sid=eb3344a674df186d&amp;metaData=SnHZRCX7NPLsJ+ExPEFNCxhotWbalOJK1bAKb4JrdH6T2r7fOYNS0fn24lYkspaB4MPWdDoQWfSgMTYkozeBy1esavfRnEsmWNUn9y9IGTPNbQv3e9jt8aL3d1v2xu9DKSzHz/PIkE4dvMq7nfYD/HuiZ47Lpn6Wymqd3CV70A+/lyaCEV2cLuob29BhL/vaXkpaMig9WMN+9MyN3AaEzqoZ4Vvz6LpzbeNJ0g0IKxs=&amp;cnc=false&amp;pickupPointCode=PP-3357698&amp;pid1=EVO-70024-00184</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>FLM-22188-00917</t>
+          <t>LIF-60029-00060</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -610,58 +610,58 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Flyman</t>
+          <t>LOKKAL</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Flyman Celana Dalam Boxer Sport Cool Mesh Pria Clana Dalem CD Bokser Cowok 1 PCS FM 3385</t>
+          <t>Basic Boxer Unisex - Blue</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>35600</v>
+        <v>39000</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium//catalog-image/MTA-61498611/flyman_flyman_celana_dalam_boxer_sport_cool_mesh_pria_clana_dalem_cd_bokser_cowok_1_pcs_fm_3385_full01_qcjo6rko.jpg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/MTA-74315404/lokkal_basic_boxer_unisex_-_blue_full06_uo8fe0j7.jpeg</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>4.8</v>
+        <v>5</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/flyman-celana-dalam-boxer-sport-cool-mesh-pria-clana-dalem-cd-bokser-cowok-1-pcs-fm-3385/ps--FLM-22188-00917?ds=FLM-22188-00917-00009&amp;source=SEARCH&amp;sid=1629777a4a0387e4&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC7uWdf8oWYVqFa8kN7IOdiFnh6wQ6PEr8y5kW/jpBoqaAXvRQdB/K7sS63OLVknJIJbKIFVX5lKVfE28/P1rwwdP0HfjxNkfgWHG5INuEdtb3hmhmBhRmH9uc9QmjY2sHdREAk1W9SMQMEM8jORiHHlRiA2nX5MQkJ/wB53voxWGEDMj7WJYkbdrdEl5t7T2aQoMGFwlZTtaHpD7Oz/Fb1Qrvl0KBXJKdKcWce8lHB5y&amp;cnc=false&amp;pickupPointCode=FLM-22188-001&amp;pid1=FLM-22188-00917</t>
+          <t>https://www.blibli.com/p/basic-boxer-unisex-blue/ps--LIF-60029-00060?ds=LIF-60029-00060-00002&amp;source=SEARCH&amp;sid=eb3344a674df186d&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC8ABEbUv77oGEmdGsuoM43+T2r7fOYNS0fn24lYkspaB+FOpWmW16LNrO62Nx2PgulesavfRnEsmWNUn9y9IGTPNbQv3e9jt8aL3d1v2xu9D3zP/3jXSVAsNO6CVkKiBbHhwvx3ifXg1BsOX37zBUHL9sb/8qEo2WC/FC2pJ0cgq9PvGCTEFtDAoi9ApC7l/76GluLHL7sh8udwFskycmSs=&amp;cnc=false&amp;pickupPointCode=PP-3519937&amp;pid1=LIF-60029-00060</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>GUC-70082-00023</t>
+          <t>INP-60076-00116</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Fashion Pria</t>
+          <t>Mainan, Buku &amp; Stationery</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Guten Inc</t>
+          <t>Hobby Boss</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Guten Inc - Celana Pendek Thin Boxer Black</t>
+          <t>Hobby Boss 83405 USS Boxer LHD-4 Model Kit [1:700]</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>26500</v>
+        <v>513000</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/107/MTA-159506880/guten_inc_guten_inc_-_celana_pendek_thin_boxer_black_full05_m9nwmh8g.jpg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium//105/MTA-29995610/hobby-boss_hobby-boss-uss-boxer-lhd-4--1-700--83405_full02.jpg</t>
         </is>
       </c>
       <c r="G6" t="n">
@@ -669,90 +669,90 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/guten-inc-celana-pendek-thin-boxer-black/ps--GUC-70082-00023?ds=GUC-70082-00023-00001&amp;source=SEARCH&amp;sid=1629777a4a0387e4&amp;metaData=SnHZRCX7NPLsJ+ExPEFNCwR0bgev9saiJ9QpuPsgXPy/HAkxoVke7cxJ4LyInlLelIueRS9s/tGUhVEdqo5+5VesavfRnEsmWNUn9y9IGTPNbQv3e9jt8aL3d1v2xu9DKSzHz/PIkE4dvMq7nfYD/A+bVy57sPYICbagrfTX85y/lyaCEV2cLuob29BhL/vaPnDwMFHBNkZD96z2eBGIU/0PfvP+DsPv5wKBaYVD+nM=&amp;cnc=false&amp;pickupPointCode=PP-3522123&amp;pid1=GUC-70082-00023</t>
+          <t>https://www.blibli.com/p/hobby-boss-83405-uss-boxer-lhd-4-model-kit-1-700/ps--INP-60076-00116?ds=INP-60076-00116-00001&amp;source=SEARCH&amp;sid=eb3344a674df186d&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC/zjMYmgLdOqahjgDqbPvascL69AJjeZ+MXw+OZq4PdaU+qNVzNAHCfEDldNFubAdFesavfRnEsmWNUn9y9IGTPNbQv3e9jt8aL3d1v2xu9D3zP/3jXSVAsNO6CVkKiBbHhwvx3ifXg1BsOX37zBUHK76SVnWEJx+v2C4ypfwXRNKLEGimk7iYf456duVuew0UVxsVtt1u7+lViZLq4OWe0=&amp;cnc=false&amp;pickupPointCode=PP-3380297&amp;pid1=INP-60076-00116</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>GUC-70082-00021</t>
+          <t>INP-60076-02694</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Fashion Pria</t>
+          <t>Mainan, Buku &amp; Stationery</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Guten Inc</t>
+          <t>Hobby Boss</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Guten Inc - Celana Underwear Pria Pendek Alan GREY</t>
+          <t>Hobby Boss 83405 USS Boxer LHD-4 Model Kit [1:700]</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>35000</v>
+        <v>399000</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/104/MTA-159506662/guten_inc_guten_inc_-_celana_underwear_pria_pendek_alan_grey_full01_mcecwt3g.jpg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/105/MTA-159533844/hobby-boss_hobby-boss-uss-boxer-lhd-4--1-700--83405_full02.jpg</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/guten-inc-celana-underwear-pria-pendek-alan-grey/ps--GUC-70082-00021?ds=GUC-70082-00021-00001&amp;source=SEARCH&amp;sid=1629777a4a0387e4&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC7uWdf8oWYVqFa8kN7IOdiGT2r7fOYNS0fn24lYkspaBEg3X3jytsJx+M8M3Wz5HMejqrM/mjls6JQDzIHvTluMiB4zoBbkTKkiVxxU6hr74Axnpn5uUjYeSavSjwxFyeYHMulcALaTPcKQsPMie104BLn0jdNeGBFFsHx5DkZbeFIFHBTh0UcYxsAONNaWLB2YMGu7X5WeWbqQCCLU+XnM=&amp;cnc=false&amp;pickupPointCode=PP-3522123&amp;pid1=GUC-70082-00021</t>
+          <t>https://www.blibli.com/p/hobby-boss-83405-uss-boxer-lhd-4-model-kit-1-700/ps--INP-60076-02694?ds=INP-60076-02694-00001&amp;source=SEARCH&amp;sid=eb3344a674df186d&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC8ABEbUv77oGEmdGsuoM43+GkIqt3bNpbYK+L444UhhhU+qNVzNAHCfEDldNFubAdFesavfRnEsmWNUn9y9IGTPNbQv3e9jt8aL3d1v2xu9D3zP/3jXSVAsNO6CVkKiBbHhwvx3ifXg1BsOX37zBUHK76SVnWEJx+v2C4ypfwXRNKLEGimk7iYf456duVuew0UVxsVtt1u7+lViZLq4OWe0=&amp;cnc=false&amp;pickupPointCode=PP-3380297&amp;pid1=INP-60076-02694</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>OFI-70005-00087</t>
+          <t>INP-60076-01480</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Ibu &amp; Anak</t>
+          <t>Mainan, Buku &amp; Stationery</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Offspring</t>
+          <t>Aurora</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Offspring Popok Bayi Diaper SAP Bebas Klorin - Triple Pack Celana L36 x3</t>
+          <t>Aurora World Anjing Boxer Dog XXL Plush Toy Boneka Anak XXL-2</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>356333</v>
+        <v>216000</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium//catalog-image/95/MTA-141213848/offspring_triple_pack_offspring_fashion_diapers_pants_popok_bayi_celana_bebas_klorin_-_l_-108pcs-_full01_hw4pewuy.jpg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium//111/MTA-58188882/aurora_aurora_world_anjing_boxer_dog_xxl_plush_toy_boneka_anak__xxl-2_full01_rd9mjwde.jpg</t>
         </is>
       </c>
       <c r="G8" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/offspring-popok-bayi-diaper-sap-bebas-klorin-triple-pack-celana-l36-x3/ps--OFI-70005-00087?ds=OFI-70005-00087-00001&amp;source=SEARCH&amp;sid=1629777a4a0387e4&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC7uWdf8oWYVqFa8kN7IOdiHD0Ph7y4AQIxNTJ6MlP49q1jjHdHUy2ZlC0z6akf4iE+Wk7L/WjZW4V3T1+QzDEpiZTqX+08YMFPt67oXduO/veDye5g4cJG51p5fjAlqNKhFRUDY7LArWqkV+AxOUq3WAegSItxabBVc/56PQyMrgankehYe5gM2XTsam362Zd9Q99NxEe4jU/YNHa8ykRiZbpBQB0IqoKZalbuEoFFziZxxZARbp9ORhpBOmAaQtRQ==&amp;cnc=false&amp;pickupPointCode=PP-3454732&amp;pid1=OFI-70005-00087</t>
+          <t>https://www.blibli.com/p/aurora-world-anjing-boxer-dog-xxl-plush-toy-boneka-anak-xxl-2/ps--INP-60076-01480?ds=INP-60076-01480-00001&amp;source=SEARCH&amp;sid=eb3344a674df186d&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC+OZu5yoAs+ZwOIEQgV7goIJcaEJLcqsH3r6UABTq0TLU+qNVzNAHCfEDldNFubAdFesavfRnEsmWNUn9y9IGTPNbQv3e9jt8aL3d1v2xu9D3zP/3jXSVAsNO6CVkKiBbHhwvx3ifXg1BsOX37zBUHK76SVnWEJx+v2C4ypfwXRNmx4cAQvCFu40hbphYlPEe4TodBPeru5IipRxn8umZ90=&amp;cnc=false&amp;pickupPointCode=PP-3380297&amp;pid1=INP-60076-01480</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>HUP-60027-02994</t>
+          <t>INS-28338-00494</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -762,35 +762,35 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Hush Puppies</t>
+          <t>Muscle Fit</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Hush Puppies Rum 3 Terry Jogger Pants Pria 01</t>
+          <t>Celana dalam Boxer Anak Cowok - 1 pcs</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>293020</v>
+        <v>15900</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium//catalog-image/99/MTA-112702877/hush_puppies_hush_puppies_rum_3_terry_jogger_pants_pria_01_full01_f4kx679b.jpg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium//105/MTA-35638737/muscle_fit_celana_dalam_boxer_anak_cowok_-_1_pcs_full01_tjg0ghi3.jpg</t>
         </is>
       </c>
       <c r="G9" t="n">
-        <v>5</v>
+        <v>4.6</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/hush-puppies-rum-3-terry-jogger-pants-pria-01/ps--HUP-60027-02994?ds=HUP-60027-02994-00005&amp;source=SEARCH&amp;sid=1629777a4a0387e4&amp;metaData=SnHZRCX7NPLsJ+ExPEFNCwIcYjJhUkfzuki5iW9SKA+DepsSX6NPsAnT86Kcx4IUMt/3c2rmpbvxfTWQ1SJQeFesavfRnEsmWNUn9y9IGTPNbQv3e9jt8aL3d1v2xu9DKSzHz/PIkE4dvMq7nfYD/A+bVy57sPYICbagrfTX85y/lyaCEV2cLuob29BhL/vaXkpaMig9WMN+9MyN3AaEzjfGE4yVZ/ypRJ/1UooaqOY=&amp;cnc=false&amp;pickupPointCode=PP-3095796&amp;pid1=HUP-60027-02994</t>
+          <t>https://www.blibli.com/p/celana-dalam-boxer-anak-cowok-1-pcs/ps--INS-28338-00494?ds=INS-28338-00494-00005&amp;source=SEARCH&amp;sid=eb3344a674df186d&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC9tiwxYVs41tNENObWAga5GIIGmm33viDj/+hYQaGlpdJpxUsLAohHVwJa3vwtOUsujqrM/mjls6JQDzIHvTluMiB4zoBbkTKkiVxxU6hr74PdxTHKZBV9wukrN4w82/yWp5HoWHuYDNl07Gpt+tmXfEjjW01Qnp2OSK0iQtfojJf8tZrf2s64VqZXfbnwqrhtlkcl11OleYOCUgny6Mmrc=&amp;cnc=false&amp;pickupPointCode=PP-3004512&amp;pid1=INS-28338-00494&amp;tag=new</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>GUC-70082-00509</t>
+          <t>BLG-70029-03629</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -800,20 +800,20 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Guten Inc</t>
+          <t>no brand</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Guteninc - Strap Sandal YELLOW BLACK Sendal Pria Slipper</t>
+          <t>Go Celana Dalam Pria Disposable - White</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>86500</v>
+        <v>29000</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/100/MTA-160690814/brd-28051_guteninc-strap-sandal-yellow-black-sendal-pria-slipper_full03-44f8736f.jpg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/MTA-95317676/no_brand_celana_dalam_pria_disposable_white_full04_okqua4k5.jpeg</t>
         </is>
       </c>
       <c r="G10" t="n">
@@ -821,37 +821,37 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/guteninc-strap-sandal-yellow-black-sendal-pria-slipper/ps--GUC-70082-00509?ds=GUC-70082-00509-00001&amp;source=SEARCH&amp;sid=1629777a4a0387e4&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC7cMd/CdFKsQOTiElOFgtVS/HAkxoVke7cxJ4LyInlLeEg3X3jytsJx+M8M3Wz5HMejqrM/mjls6JQDzIHvTluMiB4zoBbkTKkiVxxU6hr74Axnpn5uUjYeSavSjwxFyeYHMulcALaTPcKQsPMie104BLn0jdNeGBFFsHx5DkZbetmindxAjsrBzvXL0TzEINNJBzoPbzcvGyeutJypmYTc=&amp;cnc=false&amp;pickupPointCode=PP-3522123&amp;pid1=GUC-70082-00509</t>
+          <t>https://www.blibli.com/p/go-celana-dalam-pria-disposable-white/ps--BLG-70029-03629?ds=BLG-70029-03629-00001&amp;source=SEARCH&amp;sid=eb3344a674df186d&amp;metaData=SnHZRCX7NPLsJ+ExPEFNCwIcYjJhUkfzuki5iW9SKA+T2r7fOYNS0fn24lYkspaBeDjUvNSdi2pMgvjOUAWtGlesavfRnEsmWNUn9y9IGTPNbQv3e9jt8aL3d1v2xu9D3zP/3jXSVAsNO6CVkKiBbHhwvx3ifXg1BsOX37zBUHL9sb/8qEo2WC/FC2pJ0cgq9PvGCTEFtDAoi9ApC7l/76GluLHL7sh8udwFskycmSs=&amp;cnc=false&amp;pickupPointCode=PP-3526957&amp;pid1=BLG-70029-03629</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>SCY-70003-00016</t>
+          <t>LIF-60029-00055</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Fashion Wanita</t>
+          <t>Fashion Pria</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Scomfy</t>
+          <t>LOKKAL</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Scomfy Hannah Pants Celana Wanita - Olive</t>
+          <t>Basic Boxer Unisex - Checkered Blue</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>50000</v>
+        <v>39000</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/MTA-40662221/scomfy_scomfy_wide_leg_pants__celana_wanita_-_olive_full02_ccf2kh11.jpeg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/MTA-74309952/lokkal_basic_boxer_unisex_-_checkered_blue_full09_luvblje0.jpeg</t>
         </is>
       </c>
       <c r="G11" t="n">
@@ -859,37 +859,37 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/scomfy-hannah-pants-celana-wanita-olive/ps--SCY-70003-00016?ds=SCY-70003-00016-00001&amp;source=SEARCH&amp;sid=1629777a4a0387e4&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC7H99hTZSOJNePuhl5sgJ5OT2r7fOYNS0fn24lYkspaBH6O7uYSEzakzVw5tVcdvv1esavfRnEsmWNUn9y9IGTPNbQv3e9jt8aL3d1v2xu9D3zP/3jXSVAsNO6CVkKiBbHhwvx3ifXg1BsOX37zBUHKRossEAoUMZC/Ol+lg8c+HU2ZEeIuBn14TxfdO6++3xlRvUANPiMrWsA04si+GB3y0XBPM8Ib69hRyb0y0TLR/&amp;cnc=false&amp;pickupPointCode=PP-3415535&amp;pid1=SCY-70003-00016</t>
+          <t>https://www.blibli.com/p/basic-boxer-unisex-checkered-blue/ps--LIF-60029-00055?ds=LIF-60029-00055-00001&amp;source=SEARCH&amp;sid=eb3344a674df186d&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC8ABEbUv77oGEmdGsuoM43+T2r7fOYNS0fn24lYkspaBJpxUsLAohHVwJa3vwtOUsujqrM/mjls6JQDzIHvTluMiB4zoBbkTKkiVxxU6hr74PdxTHKZBV9wukrN4w82/yWp5HoWHuYDNl07Gpt+tmXfEjjW01Qnp2OSK0iQtfojJf8tZrf2s64VqZXfbnwqrhtlkcl11OleYOCUgny6Mmrc=&amp;cnc=false&amp;pickupPointCode=PP-3526302&amp;pid1=LIF-60029-00055</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>OTD-70015-00027</t>
+          <t>BLI-15014-19548</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Bliblimart</t>
+          <t>Ibu &amp; Anak</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Oto</t>
+          <t>Velvet Junior</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Oto Adult Pants Popok Celana Dewasa Size M [5 pcs]</t>
+          <t>Velvet Junior Girl Boxer AOP 2 - [3pcs/pack]</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>36000</v>
+        <v>96895</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/MTA-112159395/oto_oto_adult_pants_popok_celana_dewasa_size_m_-5_pcs-_full02_s9tc4ozw.jpeg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium//91/MTA-28301066/velvet-junior_velvet-junior_full01.jpg</t>
         </is>
       </c>
       <c r="G12" t="n">
@@ -897,90 +897,90 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/oto-adult-pants-popok-celana-dewasa-size-m-5-pcs/ps--OTD-70015-00027?ds=OTD-70015-00027-00001&amp;source=SEARCH&amp;sid=1629777a4a0387e4&amp;metaData=SnHZRCX7NPLsJ+ExPEFNCzL10t6deH8IJLci3UQaGCGT2r7fOYNS0fn24lYkspaBBdU+DX/zi5ZcJnSvGHVgcFesavfRnEsmWNUn9y9IGTPNbQv3e9jt8aL3d1v2xu9D3zP/3jXSVAsNO6CVkKiBbHhwvx3ifXg1BsOX37zBUHId8q/CTKnimReTmKzpYHZnoThlFy2kzD3CtMxiZ12p+UZRSYItc+S7ThhBJv21jGa0XBPM8Ib69hRyb0y0TLR/&amp;cnc=false&amp;pickupPointCode=PP-3482728&amp;pid1=OTD-70015-00027</t>
+          <t>https://www.blibli.com/p/velvet-junior-girl-boxer-aop-2-3pcs-pack/ps--BLI-15014-19548?ds=BLI-15014-19548-00003&amp;source=SEARCH&amp;sid=eb3344a674df186d&amp;metaData=SnHZRCX7NPLsJ+ExPEFNCxrRKGh9Gzd1bEF4U1oZrL48vkblbwv0+E1QlSs7EtdUJpxUsLAohHVwJa3vwtOUsujqrM/mjls6JQDzIHvTluMiB4zoBbkTKkiVxxU6hr74PdxTHKZBV9wukrN4w82/yWp5HoWHuYDNl07Gpt+tmXfE8Fq3Y7FQDm7GSllvB0EzwRUapLx/yCmHBm+F6S9MPxAR75Szd5AvP5iOPg1fnThfyUcjpfQtbDHqJqFsTE07&amp;cnc=false&amp;pickupPointCode=PP-3523009&amp;pid1=BLI-15014-19548</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>OTD-70015-00018</t>
+          <t>LIF-60029-00062</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Bliblimart</t>
+          <t>Fashion Pria</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Oto</t>
+          <t>LOKKAL</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Oto Adult Pants Popok Celana Dewasa Size M [Karton/12 x 8 pcs]</t>
+          <t>Basic Boxer Unisex - Tosca</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>718500</v>
+        <v>39000</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/MTA-112143309/oto_oto_adult_pants_popok_celana_dewasa_size_m_-karton-12_x_8_pcs-_full02_2fnalqv.jpeg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/MTA-74315901/lokkal_basic_boxer_unisex_-_tosca_full05_h7wg6kdj.jpeg</t>
         </is>
       </c>
       <c r="G13" t="n">
-        <v>5</v>
+        <v>4.8</v>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/oto-adult-pants-popok-celana-dewasa-size-m-karton-12-x-8-pcs/ps--OTD-70015-00018?ds=OTD-70015-00018-00001&amp;source=SEARCH&amp;sid=1629777a4a0387e4&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC6RXpYt557pWi7AhEmIfSHVk2WJGJ23OQq5oDpk4nsrgwOuwn8PMdUs21zBM0LtaAlesavfRnEsmWNUn9y9IGTPNbQv3e9jt8aL3d1v2xu9D3zP/3jXSVAsNO6CVkKiBbHhwvx3ifXg1BsOX37zBUHId8q/CTKnimReTmKzpYHZnoThlFy2kzD3CtMxiZ12p+UZRSYItc+S7ThhBJv21jGa0XBPM8Ib69hRyb0y0TLR/&amp;cnc=false&amp;pickupPointCode=PP-3482728&amp;pid1=OTD-70015-00018</t>
+          <t>https://www.blibli.com/p/basic-boxer-unisex-tosca/ps--LIF-60029-00062?ds=LIF-60029-00062-00001&amp;source=SEARCH&amp;sid=eb3344a674df186d&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC8ABEbUv77oGEmdGsuoM43+T2r7fOYNS0fn24lYkspaBJpxUsLAohHVwJa3vwtOUsujqrM/mjls6JQDzIHvTluMiB4zoBbkTKkiVxxU6hr74PdxTHKZBV9wukrN4w82/yWp5HoWHuYDNl07Gpt+tmXfEjjW01Qnp2OSK0iQtfojJf8tZrf2s64VqZXfbnwqrhtlkcl11OleYOCUgny6Mmrc=&amp;cnc=false&amp;pickupPointCode=PP-3526302&amp;pid1=LIF-60029-00062</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>OTD-70015-00035</t>
+          <t>LIF-60029-00064</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Bliblimart</t>
+          <t>Fashion Pria</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Oto</t>
+          <t>LOKKAL</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Oto Adult Pants Popok Celana Dewasa Size L [Karton/6 x 16 pcs]</t>
+          <t>Basic Boxer Unisex - Bundle Checkered</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>724600</v>
+        <v>50000</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/MTA-112178817/oto_oto_adult_pants_popok_celana_dewasa_size_l_-karton-6_x_16_pcs-_full02_ogo9m985.jpeg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/MTA-74359562/lokkal_basic_boxer_unisex_-_bundle_checkered_full08_jqdfdnyt.jpeg</t>
         </is>
       </c>
       <c r="G14" t="n">
-        <v>5</v>
+        <v>4.8</v>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/oto-adult-pants-popok-celana-dewasa-size-l-karton-6-x-16-pcs/ps--OTD-70015-00035?ds=OTD-70015-00035-00001&amp;source=SEARCH&amp;sid=1629777a4a0387e4&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC3Rpfx4BeUxhHN8ir7wH+Lxg65eTsQZO+TcmnPZYkc0ZMt/3c2rmpbvxfTWQ1SJQeFesavfRnEsmWNUn9y9IGTPNbQv3e9jt8aL3d1v2xu9D3zP/3jXSVAsNO6CVkKiBbHhwvx3ifXg1BsOX37zBUHId8q/CTKnimReTmKzpYHZnoThlFy2kzD3CtMxiZ12p+UZRSYItc+S7ThhBJv21jGa0XBPM8Ib69hRyb0y0TLR/&amp;cnc=false&amp;pickupPointCode=PP-3482728&amp;pid1=OTD-70015-00035</t>
+          <t>https://www.blibli.com/p/basic-boxer-unisex-bundle-checkered/ps--LIF-60029-00064?ds=LIF-60029-00064-00001&amp;source=SEARCH&amp;sid=eb3344a674df186d&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC7H99hTZSOJNePuhl5sgJ5OT2r7fOYNS0fn24lYkspaBJpxUsLAohHVwJa3vwtOUsujqrM/mjls6JQDzIHvTluMiB4zoBbkTKkiVxxU6hr74PdxTHKZBV9wukrN4w82/yWp5HoWHuYDNl07Gpt+tmXfEjjW01Qnp2OSK0iQtfojJf8tZrf2s64VqZXfbnwqrhtlkcl11OleYOCUgny6Mmrc=&amp;cnc=false&amp;pickupPointCode=PP-3526302&amp;pid1=LIF-60029-00064</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>ZWL-70001-00013</t>
+          <t>LIF-60029-00058</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -990,210 +990,210 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Zweckout</t>
+          <t>LOKKAL</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>ZWECKOUT - Celana Jeans Pria Panjang Hitam Pekat Slim Fit Skiny</t>
+          <t>Basic Boxer Unisex - Dusty Pink</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>149000</v>
+        <v>39000</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium//100/MTA-57214738/zweckout_zweckout_-_celana_jeans_pria_panjang_hitam_pekat_slim_fit_skiny_full03_egu3f5ja.jpg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/MTA-74311918/lokkal_basic_boxer_unisex_-_dusty_pink_full05_gmuzh68c.jpeg</t>
         </is>
       </c>
       <c r="G15" t="n">
-        <v>4.7</v>
+        <v>4.8</v>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/zweckout-celana-jeans-pria-panjang-hitam-pekat-slim-fit-skiny/ps--ZWL-70001-00013?ds=ZWL-70001-00013-00003&amp;source=SEARCH&amp;sid=1629777a4a0387e4&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC5ve/n9i6faHZpUkF2NushKGkIqt3bNpbYK+L444UhhhCAfbybkMLU8HnJV96GDkOlX6YqNL/N38iJlYkQlI2HD9cnB7A9Br96VNOoae/H1+BSFd02BuHmZWh0L7R6dhksB+tPNv9ITp+8ttAFmGt52Np6XO8WKdHoYeMogok9fdMVdPPWazoH8NOe2rYSlzZRL77KPe7oWrAYbeKNJa1ek=&amp;cnc=false&amp;pickupPointCode=PP-3372711&amp;pid1=ZWL-70001-00013</t>
+          <t>https://www.blibli.com/p/basic-boxer-unisex-dusty-pink/ps--LIF-60029-00058?ds=LIF-60029-00058-00002&amp;source=SEARCH&amp;sid=eb3344a674df186d&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC8ABEbUv77oGEmdGsuoM43+T2r7fOYNS0fn24lYkspaBJpxUsLAohHVwJa3vwtOUsujqrM/mjls6JQDzIHvTluMiB4zoBbkTKkiVxxU6hr74PdxTHKZBV9wukrN4w82/yWp5HoWHuYDNl07Gpt+tmXfEjjW01Qnp2OSK0iQtfojJf8tZrf2s64VqZXfbnwqrhtlkcl11OleYOCUgny6Mmrc=&amp;cnc=false&amp;pickupPointCode=PP-3519937&amp;pid1=LIF-60029-00058</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>SWS-70058-00065</t>
+          <t>BOD-70081-00004</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Bliblimart</t>
+          <t>Fashion Pria</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Sweety</t>
+          <t>boxr_id</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Surabaya - Sweety Bronze Dry X-Pert Pants Popok Bayi M 32s</t>
+          <t>Boxr_id Celana Dalam Pria Boxer Vibb Premium isi 3 pcs</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>50000</v>
+        <v>62099</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/MTA-158294709/sweety_surabaya_-_sweety_bronze_dry_x-pert_pants_popok_bayi_m_32s_full06_g4shwtz5.png</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/98/MTA-169225063/boxr-id_boxr-id_celana_dalam_pria_boxer_vibb_isi_3_pcs_full01_osa0kw18.jpg</t>
         </is>
       </c>
       <c r="G16" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/surabaya-sweety-bronze-dry-x-pert-pants-popok-bayi-m-32s/ps--SWS-70058-00065?ds=SWS-70058-00065-00001&amp;source=SEARCH&amp;sid=1629777a4a0387e4&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC7H99hTZSOJNePuhl5sgJ5OT2r7fOYNS0fn24lYkspaBpDKqaGEX00yummo0TbuMJlesavfRnEsmWNUn9y9IGTPNbQv3e9jt8aL3d1v2xu9D3zP/3jXSVAsNO6CVkKiBbHhwvx3ifXg1BsOX37zBUHIrv2uRgEqoWSOjr4iVZ2UqQnwkUoFArHrsuBTMpULV2HurS6AB/A5le/nF9k9GOQM=&amp;cnc=false&amp;pickupPointCode=PP-3528240&amp;pid1=SWS-70058-00065</t>
+          <t>https://www.blibli.com/p/boxr-id-celana-dalam-pria-boxer-vibb-premium-isi-3-pcs/ps--BOD-70081-00004?ds=BOD-70081-00004-00003&amp;source=SEARCH&amp;sid=eb3344a674df186d&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC9lYjsoWJEyQX0Th4y0Bu9Wjb5Ww3NVCPhuzfFnOG2I2JpxUsLAohHVwJa3vwtOUsujqrM/mjls6JQDzIHvTluMiB4zoBbkTKkiVxxU6hr74PdxTHKZBV9wukrN4w82/yWp5HoWHuYDNl07Gpt+tmXfEjjW01Qnp2OSK0iQtfojJf8tZrf2s64VqZXfbnwqrhtlkcl11OleYOCUgny6Mmrc=&amp;cnc=false&amp;pickupPointCode=PP-3532932&amp;pid1=BOD-70081-00004&amp;tag=new</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>SWS-70058-00007</t>
+          <t>BOD-70081-00001</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Bliblimart</t>
+          <t>Fashion Pria</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Sweety</t>
+          <t>no brand</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Surabaya - Sweety Silver Pants Popok Bayi L 28 Pcs x 3 Pack</t>
+          <t>Boxr_id Celana Dalam Pria Boxer Vibb Premium</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>157700</v>
+        <v>68999</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium//catalog-image/104/MTA-121967077/sweety_surabaya_-_sweety_silver_pants_popok_bayi_l_28_pcs_x_3_pack_full05_cmsr1wfz.jpg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/100/MTA-168553503/no_brand_boxr-id_celana_dalam_boxer_pria_vibb_premium_3_pcs_full01_em8sv0s2.jpg</t>
         </is>
       </c>
       <c r="G17" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/surabaya-sweety-silver-pants-popok-bayi-l-28-pcs-x-3-pack/ps--SWS-70058-00007?ds=SWS-70058-00007-00001&amp;source=SEARCH&amp;sid=1629777a4a0387e4&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC9tiwxYVs41tNENObWAga5FOSLm5WQ5rKmNtQadKtSabk2EJMN8VbdeaOfoDxq6aRFX6YqNL/N38iJlYkQlI2HD9cnB7A9Br96VNOoae/H1+BSFd02BuHmZWh0L7R6dhksB+tPNv9ITp+8ttAFmGt50F+DpLndLhhyOgRHezlp9aMvr1jaPBGR1Dff4JpGI+sYg1DCagL+VwGISeGTKUZdPkJ+go0SyaO5+o9d2cyg+S74S3wwI6k8I7omGYAl+u5o+WiGxwQPrk3UJlQOsxrERiB8ZtKTtsFLe2XdLeEKDs&amp;cnc=false&amp;pickupPointCode=PP-3528240&amp;pid1=SWS-70058-00007</t>
+          <t>https://www.blibli.com/p/boxr-id-celana-dalam-pria-boxer-vibb-premium/ps--BOD-70081-00001?ds=BOD-70081-00001-00001&amp;source=SEARCH&amp;sid=eb3344a674df186d&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC4tTCBijc70K03wpOh0TemHOlHF/k5IdSxwaVC2xTLFWJpxUsLAohHVwJa3vwtOUsujqrM/mjls6JQDzIHvTluMiB4zoBbkTKkiVxxU6hr74PdxTHKZBV9wukrN4w82/yWp5HoWHuYDNl07Gpt+tmXfEjjW01Qnp2OSK0iQtfojJf8tZrf2s64VqZXfbnwqrhtlkcl11OleYOCUgny6Mmrc=&amp;cnc=false&amp;pickupPointCode=PP-3532932&amp;pid1=BOD-70081-00001&amp;tag=new</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>SWS-70058-00013</t>
+          <t>TAU-60025-01767</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Bliblimart</t>
+          <t>Ibu &amp; Anak</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Sweety</t>
+          <t>Tally</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Surabaya - Sweety Silver Pants Boys Popok Bayi XL 26 Pcs x 3 Pack</t>
+          <t>TALLY Celana Dalam Hamil Bahan Katun Bambu Fit to L -XL Muat Kehamilan 0 - 9 Bulan Celana Maternity CD Wanita High Waist Pakaian Dalam Lembut</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>167700</v>
+        <v>39999</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium//catalog-image/96/MTA-121983414/sweety_sweety_silver_pants_boys_popok_bayi_-size_xl-_3_x_26_pcs-_full03_qwo3b033.jpg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/112/MTA-169583269/tally_tally_celana_dalam_hamil_bahan_katun_bambu_fit_to_l_-xl_muat_kehamilan_0_-_9_bulan_celana_maternity_cd_wanita_high_waist_pakaian_dalam_lembut_full01_lcxibazp.jpg</t>
         </is>
       </c>
       <c r="G18" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/surabaya-sweety-silver-pants-boys-popok-bayi-xl-26-pcs-x-3-pack/ps--SWS-70058-00013?ds=SWS-70058-00013-00001&amp;source=SEARCH&amp;sid=1629777a4a0387e4&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC7Icmq1gsSXLUq8ZinzLw7tOSLm5WQ5rKmNtQadKtSabCAfbybkMLU8HnJV96GDkOlX6YqNL/N38iJlYkQlI2HD9cnB7A9Br96VNOoae/H1+BSFd02BuHmZWh0L7R6dhksB+tPNv9ITp+8ttAFmGt50F+DpLndLhhyOgRHezlp9aMvr1jaPBGR1Dff4JpGI+sYg1DCagL+VwGISeGTKUZdPkJ+go0SyaO5+o9d2cyg+S74S3wwI6k8I7omGYAl+u5o+WiGxwQPrk3UJlQOsxrERiB8ZtKTtsFLe2XdLeEKDs&amp;cnc=false&amp;pickupPointCode=PP-3528240&amp;pid1=SWS-70058-00013</t>
+          <t>https://www.blibli.com/p/tally-celana-dalam-hamil-bahan-katun-bambu-fit-to-l-xl-muat-kehamilan-0-9-bulan-celana-maternity-cd-wanita-high-waist-pakaian-dalam-lembut/ps--TAU-60025-01767?ds=TAU-60025-01767-00001&amp;source=SEARCH&amp;sid=eb3344a674df186d&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC8ABEbUv77oGEmdGsuoM43/OlHF/k5IdSxwaVC2xTLFWJpxUsLAohHVwJa3vwtOUsujqrM/mjls6JQDzIHvTluMiB4zoBbkTKkiVxxU6hr74PdxTHKZBV9wukrN4w82/yWp5HoWHuYDNl07Gpt+tmXdtbUEB2KN2y84saGW8FURoFNpMZjfoNazsAekWU+LFfRtd5JisA+krezcArUVhBa3TrWgM/WffSFIKvZxBffSZ&amp;cnc=false&amp;pickupPointCode=PP-3085543&amp;pid1=TAU-60025-01767&amp;tag=new</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>SWS-70058-00014</t>
+          <t>TAU-60025-01774</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Bliblimart</t>
+          <t>Fashion Wanita</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Sweety</t>
+          <t>Tally</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Surabaya - Sweety Silver Pants Boys Popok Bayi L 28 Pcs x 3 Pack</t>
+          <t>TALLY Celana Dalam Wanita Bahan Katun Bambu fit to L - XL Cd Wanita Basic Super Lembut Pakaian Dalam Wanita Stretchable CD 1260</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>177000</v>
+        <v>25999</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium//catalog-image/106/MTA-121983919/sweety_sweety_silver_pants_boys_popok_bayi_-size_l-_3_x_28_pcs-_full03_h1cxoo8a.jpg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/100/MTA-169623181/tally_tally_celana_dalam_wanita_bahan_katun_bambu_fit_to_l_-_xl_cd_wanita_basic_super_lembut_pakaian_dalam_wanita_stretchable_cd_1260_full06_hyjkadze.jpg</t>
         </is>
       </c>
       <c r="G19" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/surabaya-sweety-silver-pants-boys-popok-bayi-l-28-pcs-x-3-pack/ps--SWS-70058-00014?ds=SWS-70058-00014-00001&amp;source=SEARCH&amp;sid=1629777a4a0387e4&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC1ifcoeXCfsl309abOwHy+V484ig9GGZ2RzcsQTFZUtmzzZ/8U3KjGLexZ+hPeKg01esavfRnEsmWNUn9y9IGTPNbQv3e9jt8aL3d1v2xu9D3zP/3jXSVAsNO6CVkKiBbHhwvx3ifXg1BsOX37zBUHIrv2uRgEqoWSOjr4iVZ2UqQnwkUoFArHrsuBTMpULV2LnIWRkU0YcQeCzMai3vt1gpf2IWziHLx7iDlUWZO4axleBsKjDSYYdNagV5MxwYWqZm5qTnquY9priXX1YScNPo0XRS9ppfUuESnkztTN78&amp;cnc=false&amp;pickupPointCode=PP-3528240&amp;pid1=SWS-70058-00014</t>
+          <t>https://www.blibli.com/p/tally-celana-dalam-wanita-bahan-katun-bambu-fit-to-l-xl-cd-wanita-basic-super-lembut-pakaian-dalam-wanita-stretchable-cd-1260/ps--TAU-60025-01774?ds=TAU-60025-01774-00001&amp;source=SEARCH&amp;sid=eb3344a674df186d&amp;metaData=SnHZRCX7NPLsJ+ExPEFNCzO4NENA+D3a2b160XD/ATDOlHF/k5IdSxwaVC2xTLFWJpxUsLAohHVwJa3vwtOUsujqrM/mjls6JQDzIHvTluMiB4zoBbkTKkiVxxU6hr74PdxTHKZBV9wukrN4w82/yWp5HoWHuYDNl07Gpt+tmXfO/kFtVj4porywlY2UWbf6VMqwppbx5Qk9+27gygWs9lk0gjRbIbx9mhzaC4fFgmtfyUcjpfQtbDHqJqFsTE07&amp;cnc=false&amp;pickupPointCode=PP-3085543&amp;pid1=TAU-60025-01774&amp;tag=new</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>SWS-70058-00012</t>
+          <t>HOO-10808-00428</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Bliblimart</t>
+          <t>Fashion Pria</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Sweety</t>
+          <t>Rider</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Surabaya - Sweety Silver Pants Boys Popok Bayi XXL 24 Pcs x 3 Pack</t>
+          <t>Rider Boxer Sport Men's Underwear R763B (1 pcs)</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>177500</v>
+        <v>38635</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium//catalog-image/96/MTA-121983062/sweety_sweety_silver_pants_boys_popok_bayi_-size_xxl-_3_x_24_sheets-_full02_pplq6ai3.jpg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium//113/MTA-75269858/rider_rider_boxer_sport_men-s_underwear_r763b_-1_pcs-_full07_u9c3l9nv.jpg</t>
         </is>
       </c>
       <c r="G20" t="n">
@@ -1201,52 +1201,52 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/surabaya-sweety-silver-pants-boys-popok-bayi-xxl-24-pcs-x-3-pack/ps--SWS-70058-00012?ds=SWS-70058-00012-00001&amp;source=SEARCH&amp;sid=1629777a4a0387e4&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC1ifcoeXCfsl309abOwHy+Upz6Oltu5mExkNdyvoaObo1REXguDUy1GVQkblUMrMyVX6YqNL/N38iJlYkQlI2HD9cnB7A9Br96VNOoae/H1+BSFd02BuHmZWh0L7R6dhksB+tPNv9ITp+8ttAFmGt50F+DpLndLhhyOgRHezlp9aMvr1jaPBGR1Dff4JpGI+sYg1DCagL+VwGISeGTKUZdPkJ+go0SyaO5+o9d2cyg+S74S3wwI6k8I7omGYAl+u5o+WiGxwQPrk3UJlQOsxrERiB8ZtKTtsFLe2XdLeEKDs&amp;cnc=false&amp;pickupPointCode=PP-3528240&amp;pid1=SWS-70058-00012</t>
+          <t>https://www.blibli.com/p/rider-boxer-sport-men-s-underwear-r763b-1-pcs/ps--HOO-10808-00428?ds=HOO-10808-00428-00012&amp;source=SEARCH&amp;sid=eb3344a674df186d&amp;metaData=SnHZRCX7NPLsJ+ExPEFNCzrqhn2WeenYl70j0tMOsyi3gbHx1BRMw4TcnojR/1dYtSexjj4b6RjEfICBcSNGe1X6YqNL/N38iJlYkQlI2HD9cnB7A9Br96VNOoae/H1+BSFd02BuHmZWh0L7R6dhksB+tPNv9ITp+8ttAFmGt50fyHCRn0/K8xKS6bnBZOgsceqJBE8+DUjBwsxdmjWQn2ghvZVulURit5M328K8mmU=&amp;cnc=false&amp;pickupPointCode=HOO-10808-002&amp;pid1=HOO-10808-00428</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>SWS-70058-00008</t>
+          <t>SYU-60023-00446</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Bliblimart</t>
+          <t>Ibu &amp; Anak</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Sweety</t>
+          <t>no brand</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Surabaya - Sweety Silver Pants Girl Popok Bayi XXL 24 Pcs x 3 Pack</t>
+          <t>Celana dalam anak ternyaman laki laki perempuan motif random</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>177500</v>
+        <v>16000</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium//catalog-image/105/MTA-121968852/sweety_sweety_silver_pants_girl_popok_bayi_-size_xxl-_24_pcs-_3_pack-_full02_tfy1kxol.jpg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/120/MTA-168838986/no-brand_celana-dalam-anak-ternyaman-laki-laki-perempuan-motif-random_full01.jpg</t>
         </is>
       </c>
       <c r="G21" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/surabaya-sweety-silver-pants-girl-popok-bayi-xxl-24-pcs-x-3-pack/ps--SWS-70058-00008?ds=SWS-70058-00008-00001&amp;source=SEARCH&amp;sid=1629777a4a0387e4&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC1ifcoeXCfsl309abOwHy+Upz6Oltu5mExkNdyvoaOboS2t0M8S3eAMOX0byvli/HFX6YqNL/N38iJlYkQlI2HD9cnB7A9Br96VNOoae/H1+BSFd02BuHmZWh0L7R6dhksB+tPNv9ITp+8ttAFmGt50F+DpLndLhhyOgRHezlp9aMvr1jaPBGR1Dff4JpGI+sYg1DCagL+VwGISeGTKUZdPkJ+go0SyaO5+o9d2cyg+S74S3wwI6k8I7omGYAl+u5o+WiGxwQPrk3UJlQOsxrERiB8ZtKTtsFLe2XdLeEKDs&amp;cnc=false&amp;pickupPointCode=PP-3528240&amp;pid1=SWS-70058-00008</t>
+          <t>https://www.blibli.com/p/celana-dalam-anak-ternyaman-laki-laki-perempuan-motif-random/ps--SYU-60023-00446?ds=SYU-60023-00446-00002&amp;source=SEARCH&amp;sid=eb3344a674df186d&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC7Icmq1gsSXLUq8ZinzLw7uT2r7fOYNS0fn24lYkspaBJpxUsLAohHVwJa3vwtOUsujqrM/mjls6JQDzIHvTluMiB4zoBbkTKkiVxxU6hr74PdxTHKZBV9wukrN4w82/yWp5HoWHuYDNl07Gpt+tmXfE8Fq3Y7FQDm7GSllvB0EzwRUapLx/yCmHBm+F6S9MPxAR75Szd5AvP5iOPg1fnThfyUcjpfQtbDHqJqFsTE07&amp;cnc=false&amp;pickupPointCode=PP-3124847&amp;pid1=SYU-60023-00446&amp;tag=new</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>THP-70006-00066</t>
+          <t>YOH-60025-00664</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -1256,210 +1256,210 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Sorex</t>
+          <t>Young Hearts</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Sorex art. 15227 CD Kancut Remaja Cewek / Celana Dalam Basic Wanita Fit to L Bahan Katun</t>
+          <t>Young Hearts Panty (Celana Dalam) Marshmallow Kiss, Hipster Y27-000680</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>10000</v>
+        <v>72000</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium//99/MTA-43900936/sorex_sorex_art-_15227_cd_kancut_remaja_cewek_-_celana_dalam_basic_wanita_fit_to_l_bahan_katun_full01_gz6ffmkh.jpg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/116/MTA-168869726/br-m036969-10134_young-hearts-panty-celana-dalam-marshmallow-kiss-hipster-y27-000680_full09-cff1eaac.jpg</t>
         </is>
       </c>
       <c r="G22" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/sorex-art-15227-cd-kancut-remaja-cewek-celana-dalam-basic-wanita-fit-to-l-bahan-katun/ps--THP-70006-00066?ds=THP-70006-00066-00001&amp;source=SEARCH&amp;sid=1629777a4a0387e4&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC0ry844Ce9aEHITmMYpiMq+T2r7fOYNS0fn24lYkspaBgTJ8MrOe6rxqTJ0SPzMiflX6YqNL/N38iJlYkQlI2HD9cnB7A9Br96VNOoae/H1+UvM5rYQ2b7sWjAIjInNGfymSid4UzDSJt9ecE9c7PeUrriCFOI5lmHqdKNgbp4eEVx4J/1iDNX0HaLHD3yW7Hb46duIZxGbk9mK36HGAl/uFLV40DCFINHOsYP0JA4zA&amp;cnc=false&amp;pickupPointCode=PP-3146962&amp;pid1=THP-70006-00066</t>
+          <t>https://www.blibli.com/p/young-hearts-panty-celana-dalam-marshmallow-kiss-hipster-y27-000680/ps--YOH-60025-00664?ds=YOH-60025-00664-00002&amp;source=SEARCH&amp;sid=eb3344a674df186d&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC3Rpfx4BeUxhHN8ir7wH+LyT2r7fOYNS0fn24lYkspaBJpxUsLAohHVwJa3vwtOUsujqrM/mjls6JQDzIHvTluMiB4zoBbkTKkiVxxU6hr74PdxTHKZBV9wukrN4w82/yWp5HoWHuYDNl07Gpt+tmXfO/kFtVj4porywlY2UWbf6VMqwppbx5Qk9+27gygWs9lk0gjRbIbx9mhzaC4fFgmtfyUcjpfQtbDHqJqFsTE07&amp;cnc=false&amp;pickupPointCode=PP-3054594&amp;pid1=YOH-60025-00664&amp;tag=new</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>GBM-70000-00056</t>
+          <t>TAU-60025-01769</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Bliblimart</t>
+          <t>Fashion Wanita</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>MamyPoko</t>
+          <t>Tally</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>MamyPoko Royal Soft Pant L34 Boy</t>
+          <t>TALLY Celana Korset Wanita Extra Shapping Ada Kait Bahan Rajut Fit to M/L - 3X/4XL Corset Elastis Lembut dan Nyaman Pakaian Dalam Wanita CST 1251</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>79200</v>
+        <v>89999</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium//99/MTA-18075067/mamypoko_mamypoko_royal_soft_pant_l34_boy_full01_bhppemm5.jpg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/106/MTA-169586152/tally_tally_celana_korset_wanita_extra_shapping_ada_kait_bahan_rajut_fit_to_m-l_-_3x-4xl_corset_elastis_lembut_dan_nyaman_pakaian_dalam_wanita_cst_1251_full11_u0lqnc0c.jpg</t>
         </is>
       </c>
       <c r="G23" t="n">
-        <v>4.9</v>
+        <v>0</v>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/mamypoko-royal-soft-pant-l34-boy/ps--GBM-70000-00056?ds=GBM-70000-00056-00001&amp;source=SEARCH&amp;sid=1629777a4a0387e4&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC+lwajEQMliso6x+S1dlY1HG7ZKryzxMhLfm5+J6+v8bO/vnA5t9K0Dl2QdZxqhd3lX6YqNL/N38iJlYkQlI2HD9cnB7A9Br96VNOoae/H1+UvM5rYQ2b7sWjAIjInNGfymSid4UzDSJt9ecE9c7PeV2gNMGFcfbof284avA3NXEQWjeZmb5HX82xAuernonhApLuJFId0/bnznE+dmC5y/pqZ4sYT5Dw65c9NjlZBD0GU6+X7Ca5v+MvVLTl6vIgMl1mgM4oDgEVStdMbvQNTM5zgFtHclGUARQ9ELsjSKFK75dCgVySnSnFnHvJRwecg==&amp;cnc=false&amp;pickupPointCode=PP-3182874&amp;pid1=GBM-70000-00056</t>
+          <t>https://www.blibli.com/p/tally-celana-korset-wanita-extra-shapping-ada-kait-bahan-rajut-fit-to-m-l-3x-4xl-corset-elastis-lembut-dan-nyaman-pakaian-dalam-wanita-cst-1251/ps--TAU-60025-01769?ds=TAU-60025-01769-00002&amp;source=SEARCH&amp;sid=eb3344a674df186d&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC9XGAMfrhUMip/eqTpDTn+vOlHF/k5IdSxwaVC2xTLFWJpxUsLAohHVwJa3vwtOUsujqrM/mjls6JQDzIHvTluMiB4zoBbkTKkiVxxU6hr74PdxTHKZBV9wukrN4w82/yWp5HoWHuYDNl07Gpt+tmXfO/kFtVj4porywlY2UWbf6VMqwppbx5Qk9+27gygWs9pbvmWihN1rLv6WEwT2nrqFfyUcjpfQtbDHqJqFsTE07&amp;cnc=false&amp;pickupPointCode=PP-3085543&amp;pid1=TAU-60025-01769&amp;tag=new</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>GBM-70000-00054</t>
+          <t>BLI-60043-01827</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Bliblimart</t>
+          <t>Fashion Pria</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Baby Happy</t>
+          <t>Bloods</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Baby Happy XXL24</t>
+          <t>Bloods Series Boxer Signals Black</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>46700</v>
+        <v>139000</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/MTA-10488055/baby_happy_baby_happy_xxl24_full01_kll2frq6.jpg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/105/MTA-168861047/brd-09186_bloods-series-boxer-signals-black_full01-a1b60144.jpg</t>
         </is>
       </c>
       <c r="G24" t="n">
-        <v>4.9</v>
+        <v>0</v>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/baby-happy-xxl24/ps--GBM-70000-00054?ds=GBM-70000-00054-00001&amp;source=SEARCH&amp;sid=1629777a4a0387e4&amp;metaData=SnHZRCX7NPLsJ+ExPEFNCxMBO06F3DG/I/RxYUVI14udEXuxqXaNFOM6xK9miVb8jXK5lZ8k4OWZwl0EVYR8zZbKIFVX5lKVfE28/P1rwwdP0HfjxNkfgWHG5INuEdtb3hmhmBhRmH9uc9QmjY2sHdREAk1W9SMQMEM8jORiHHnxkaTwRuRc1M87T35afQYSIY8zCUZTQMImZcXrQqatmMlXVzCnW+9h51z9RDvnHdUrvl0KBXJKdKcWce8lHB5y&amp;cnc=false&amp;pickupPointCode=PP-3182874&amp;pid1=GBM-70000-00054</t>
+          <t>https://www.blibli.com/p/bloods-series-boxer-signals-black/ps--BLI-60043-01827?ds=BLI-60043-01827-00001&amp;source=SEARCH&amp;sid=eb3344a674df186d&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC1cGXwSFpLJsXh2noxRjCIuGkIqt3bNpbYK+L444UhhhU+qNVzNAHCfEDldNFubAdFesavfRnEsmWNUn9y9IGTPNbQv3e9jt8aL3d1v2xu9D3zP/3jXSVAsNO6CVkKiBbHhwvx3ifXg1BsOX37zBUHL9sb/8qEo2WC/FC2pJ0cgq9PvGCTEFtDAoi9ApC7l/76GluLHL7sh8udwFskycmSs=&amp;cnc=false&amp;pickupPointCode=PP-3521786&amp;pid1=BLI-60043-01827&amp;tag=new</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>SCY-70003-00017</t>
+          <t>BLI-60043-01824</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Fashion Wanita</t>
+          <t>Fashion Pria</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Scomfy</t>
+          <t>Bloods</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Scomfy Hannah Pants Celana Wanita - Light Grey</t>
+          <t>Bloods Series Boxer Taked Black</t>
         </is>
       </c>
       <c r="E25" t="n">
-        <v>59700</v>
+        <v>139000</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/MTA-40662223/scomfy_scomfy_wide_leg_pants__celana_wanita_-_light_grey_full02_lwd5lv4p.jpeg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/102/MTA-168861044/brd-09186_bloods-series-boxer-taked-black_full01-20f1bf18.jpg</t>
         </is>
       </c>
       <c r="G25" t="n">
-        <v>4.7</v>
+        <v>0</v>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/scomfy-hannah-pants-celana-wanita-light-grey/ps--SCY-70003-00017?ds=SCY-70003-00017-00001&amp;source=SEARCH&amp;sid=1629777a4a0387e4&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC5ZM94ezkueJan8UnJr3rVmdEXuxqXaNFOM6xK9miVb8BI+SgwT0bjuIBd7LA3Wgh1esavfRnEsmWNUn9y9IGTPNbQv3e9jt8aL3d1v2xu9D3zP/3jXSVAsNO6CVkKiBbHhwvx3ifXg1BsOX37zBUHKRossEAoUMZC/Ol+lg8c+HU2ZEeIuBn14TxfdO6++3xlRvUANPiMrWsA04si+GB3y0XBPM8Ib69hRyb0y0TLR/&amp;cnc=false&amp;pickupPointCode=PP-3415535&amp;pid1=SCY-70003-00017</t>
+          <t>https://www.blibli.com/p/bloods-series-boxer-taked-black/ps--BLI-60043-01824?ds=BLI-60043-01824-00003&amp;source=SEARCH&amp;sid=eb3344a674df186d&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC1cGXwSFpLJsXh2noxRjCIuGkIqt3bNpbYK+L444UhhhU+qNVzNAHCfEDldNFubAdFesavfRnEsmWNUn9y9IGTPNbQv3e9jt8aL3d1v2xu9D3zP/3jXSVAsNO6CVkKiBbHhwvx3ifXg1BsOX37zBUHL9sb/8qEo2WC/FC2pJ0cgq9PvGCTEFtDAoi9ApC7l/76GluLHL7sh8udwFskycmSs=&amp;cnc=false&amp;pickupPointCode=PP-3521786&amp;pid1=BLI-60043-01824&amp;tag=new</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>DIT-60030-00407</t>
+          <t>BLI-60043-01821</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Olahraga &amp; Aktivitas Luar Ruang</t>
+          <t>Fashion Pria</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Diadora</t>
+          <t>Bloods</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Diadora Women Training Tights Ganis Legging Fitness Wanita [DIAPN230101B]</t>
+          <t>Bloods Series Boxer Wonde White</t>
         </is>
       </c>
       <c r="E26" t="n">
-        <v>225000</v>
+        <v>139000</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/MTA-99225419/diadora_diadora_women_training_tights_ganis_legging_fitness_wanita_-diapn230101b-_full05_hyhazkl9.jpeg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/104/MTA-168855224/brd-09186_bloods-series-boxer-wonde-white_full01-6a76e226.jpg</t>
         </is>
       </c>
       <c r="G26" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/diadora-women-training-tights-ganis-legging-fitness-wanita-diapn230101b/ps--DIT-60030-00407?ds=DIT-60030-00407-00001&amp;source=SEARCH&amp;sid=1629777a4a0387e4&amp;metaData=SnHZRCX7NPLsJ+ExPEFNCzcTLm2yJwfE+vqixRWQ5q80wn7+82bYRdE+2sGGRS84T/uxVTkHJrdC+NFZb+f6u1X6YqNL/N38iJlYkQlI2HD9cnB7A9Br96VNOoae/H1+BSFd02BuHmZWh0L7R6dhksB+tPNv9ITp+8ttAFmGt53gqhxMcK8WFN2S236B9Kw9dczJ2dZl0GF+fKX+a5i6arCqKzRr8lLllAusTqHk6aA=&amp;cnc=false&amp;pickupPointCode=PP-3526146&amp;pid1=DIT-60030-00407</t>
+          <t>https://www.blibli.com/p/bloods-series-boxer-wonde-white/ps--BLI-60043-01821?ds=BLI-60043-01821-00003&amp;source=SEARCH&amp;sid=eb3344a674df186d&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC1cGXwSFpLJsXh2noxRjCIuGkIqt3bNpbYK+L444UhhhU+qNVzNAHCfEDldNFubAdFesavfRnEsmWNUn9y9IGTPNbQv3e9jt8aL3d1v2xu9D3zP/3jXSVAsNO6CVkKiBbHhwvx3ifXg1BsOX37zBUHL9sb/8qEo2WC/FC2pJ0cgq9PvGCTEFtDAoi9ApC7l/76GluLHL7sh8udwFskycmSs=&amp;cnc=false&amp;pickupPointCode=PP-3521786&amp;pid1=BLI-60043-01821&amp;tag=new</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>OTD-70015-00031</t>
+          <t>BLI-60043-01822</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Bliblimart</t>
+          <t>Fashion Pria</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Oto</t>
+          <t>Bloods</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Oto Adult Pants Popok Celana Dewasa Size XL [3 pcs]</t>
+          <t>Bloods Series Boxer Hatred Black</t>
         </is>
       </c>
       <c r="E27" t="n">
-        <v>29300</v>
+        <v>139000</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/MTA-112175387/oto_oto_adult_pants_popok_celana_dewasa_size_xl_-3_pcs-_full02_iamaeq0r.jpeg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/99/MTA-168861041/brd-09186_bloods-series-boxer-hatred-black_full01-88dd0211.jpg</t>
         </is>
       </c>
       <c r="G27" t="n">
@@ -1467,37 +1467,37 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/oto-adult-pants-popok-celana-dewasa-size-xl-3-pcs/ps--OTD-70015-00031?ds=OTD-70015-00031-00001&amp;source=SEARCH&amp;sid=1629777a4a0387e4&amp;metaData=SnHZRCX7NPLsJ+ExPEFNCwIcYjJhUkfzuki5iW9SKA8PkCU6Vf0gJqVxNGwMfC4mZ8ko3/0ZpJ68wdWEBuKJXVesavfRnEsmWNUn9y9IGTPNbQv3e9jt8aL3d1v2xu9D3zP/3jXSVAsNO6CVkKiBbHhwvx3ifXg1BsOX37zBUHId8q/CTKnimReTmKzpYHZnoThlFy2kzD3CtMxiZ12p+UZRSYItc+S7ThhBJv21jGa0XBPM8Ib69hRyb0y0TLR/&amp;cnc=false&amp;pickupPointCode=PP-3482728&amp;pid1=OTD-70015-00031</t>
+          <t>https://www.blibli.com/p/bloods-series-boxer-hatred-black/ps--BLI-60043-01822?ds=BLI-60043-01822-00001&amp;source=SEARCH&amp;sid=eb3344a674df186d&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC1cGXwSFpLJsXh2noxRjCIuGkIqt3bNpbYK+L444UhhhU+qNVzNAHCfEDldNFubAdFesavfRnEsmWNUn9y9IGTPNbQv3e9jt8aL3d1v2xu9D3zP/3jXSVAsNO6CVkKiBbHhwvx3ifXg1BsOX37zBUHL9sb/8qEo2WC/FC2pJ0cgq9PvGCTEFtDAoi9ApC7l/76GluLHL7sh8udwFskycmSs=&amp;cnc=false&amp;pickupPointCode=PP-3521786&amp;pid1=BLI-60043-01822&amp;tag=new</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>OTD-70015-00022</t>
+          <t>BLI-60043-01823</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Bliblimart</t>
+          <t>Fashion Pria</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Oto</t>
+          <t>Bloods</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Oto Adult Pants Popok Celana Dewasa Size XL [Karton/12 x 8 pcs]</t>
+          <t>Bloods Series Boxer Cheydo Black</t>
         </is>
       </c>
       <c r="E28" t="n">
-        <v>750800</v>
+        <v>139000</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/MTA-112159326/oto_oto_adult_pants_popok_celana_dewasa_size_xl_-karton-12_x_8_pcs-_full02_jv5z8dbl.jpeg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/100/MTA-168861042/brd-09186_bloods-series-boxer-cheydo-black_full01-f6d15114.jpg</t>
         </is>
       </c>
       <c r="G28" t="n">
@@ -1505,37 +1505,37 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/oto-adult-pants-popok-celana-dewasa-size-xl-karton-12-x-8-pcs/ps--OTD-70015-00022?ds=OTD-70015-00022-00001&amp;source=SEARCH&amp;sid=1629777a4a0387e4&amp;metaData=SnHZRCX7NPLsJ+ExPEFNCycpTyS3V4Bt86XaxsYSf79UK3Q12Gibu3N0BIMtAAAGzzZ/8U3KjGLexZ+hPeKg01esavfRnEsmWNUn9y9IGTPNbQv3e9jt8aL3d1v2xu9D3zP/3jXSVAsNO6CVkKiBbHhwvx3ifXg1BsOX37zBUHId8q/CTKnimReTmKzpYHZnoThlFy2kzD3CtMxiZ12p+UZRSYItc+S7ThhBJv21jGa0XBPM8Ib69hRyb0y0TLR/&amp;cnc=false&amp;pickupPointCode=PP-3482728&amp;pid1=OTD-70015-00022</t>
+          <t>https://www.blibli.com/p/bloods-series-boxer-cheydo-black/ps--BLI-60043-01823?ds=BLI-60043-01823-00003&amp;source=SEARCH&amp;sid=eb3344a674df186d&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC1cGXwSFpLJsXh2noxRjCIuGkIqt3bNpbYK+L444UhhhU+qNVzNAHCfEDldNFubAdFesavfRnEsmWNUn9y9IGTPNbQv3e9jt8aL3d1v2xu9D3zP/3jXSVAsNO6CVkKiBbHhwvx3ifXg1BsOX37zBUHL9sb/8qEo2WC/FC2pJ0cgq9PvGCTEFtDAoi9ApC7l/76GluLHL7sh8udwFskycmSs=&amp;cnc=false&amp;pickupPointCode=PP-3521786&amp;pid1=BLI-60043-01823&amp;tag=new</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>OTD-70015-00020</t>
+          <t>BLI-60043-01826</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Bliblimart</t>
+          <t>Fashion Pria</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Oto</t>
+          <t>Bloods</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Oto Adult Pants Popok Celana Dewasa Size L [Karton/12 x 8 pcs]</t>
+          <t>Bloods Series Boxer Bitan Black</t>
         </is>
       </c>
       <c r="E29" t="n">
-        <v>790900</v>
+        <v>139000</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/MTA-112143344/oto_oto_adult_pants_popok_celana_dewasa_size_l_-karton-12_x_8_pcs-_full02_pc9sj99v.jpeg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/104/MTA-168861046/brd-09186_bloods-series-boxer-bitan-black_full01-79adfa97.jpg</t>
         </is>
       </c>
       <c r="G29" t="n">
@@ -1543,463 +1543,463 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/oto-adult-pants-popok-celana-dewasa-size-l-karton-12-x-8-pcs/ps--OTD-70015-00020?ds=OTD-70015-00020-00001&amp;source=SEARCH&amp;sid=1629777a4a0387e4&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC+lwajEQMliso6x+S1dlY1EH3qS6KEp2/0vyLR+xTfJHU+qNVzNAHCfEDldNFubAdFesavfRnEsmWNUn9y9IGTPNbQv3e9jt8aL3d1v2xu9D3zP/3jXSVAsNO6CVkKiBbHhwvx3ifXg1BsOX37zBUHId8q/CTKnimReTmKzpYHZnoThlFy2kzD3CtMxiZ12p+UZRSYItc+S7ThhBJv21jGa0XBPM8Ib69hRyb0y0TLR/&amp;cnc=false&amp;pickupPointCode=PP-3482728&amp;pid1=OTD-70015-00020</t>
+          <t>https://www.blibli.com/p/bloods-series-boxer-bitan-black/ps--BLI-60043-01826?ds=BLI-60043-01826-00002&amp;source=SEARCH&amp;sid=eb3344a674df186d&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC1cGXwSFpLJsXh2noxRjCIuGkIqt3bNpbYK+L444UhhhU+qNVzNAHCfEDldNFubAdFesavfRnEsmWNUn9y9IGTPNbQv3e9jt8aL3d1v2xu9D3zP/3jXSVAsNO6CVkKiBbHhwvx3ifXg1BsOX37zBUHL9sb/8qEo2WC/FC2pJ0cgq9PvGCTEFtDAoi9ApC7l/76GluLHL7sh8udwFskycmSs=&amp;cnc=false&amp;pickupPointCode=PP-3521786&amp;pid1=BLI-60043-01826&amp;tag=new</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>BLG-70029-07204</t>
+          <t>BLI-60043-01809</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Bliblimart</t>
+          <t>Fashion Pria</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Fitti</t>
+          <t>Bloods</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Fitti Pants Popok Celana XL-40</t>
+          <t>Bloods Pants Boardshort Boxer Testuo Series</t>
         </is>
       </c>
       <c r="E30" t="n">
-        <v>82100</v>
+        <v>175000</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium//catalog-image/104/MTA-145691059/fitti_fitti_pants_xl-40_popok_celana_full01_syl4whp.jpg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/107/MTA-168852581/brd-09186_bloods-pants-boardshort-boxer-testuo-series_full02-5b7bb777.jpg</t>
         </is>
       </c>
       <c r="G30" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/fitti-pants-popok-celana-xl-40/ps--BLG-70029-07204?ds=BLG-70029-07204-00001&amp;source=SEARCH&amp;sid=1629777a4a0387e4&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC8tpUbp7kIfoUBwX3mSt48UmbE/LLJy7W3VwRB8pUx8xb5r2p5qDtWVXqVc7GY1hBFesavfRnEsmWNUn9y9IGTPNbQv3e9jt8aL3d1v2xu9D3zP/3jXSVAsNO6CVkKiBbHhwvx3ifXg1BsOX37zBUHIrv2uRgEqoWSOjr4iVZ2UqQnwkUoFArHrsuBTMpULV2HurS6AB/A5le/nF9k9GOQM=&amp;cnc=false&amp;pickupPointCode=PP-3526957&amp;pid1=BLG-70029-07204</t>
+          <t>https://www.blibli.com/p/bloods-pants-boardshort-boxer-testuo-series/ps--BLI-60043-01809?ds=BLI-60043-01809-00006&amp;source=SEARCH&amp;sid=eb3344a674df186d&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC1ifcoeXCfsl309abOwHy+U0wn7+82bYRdE+2sGGRS84U+qNVzNAHCfEDldNFubAdFesavfRnEsmWNUn9y9IGTPNbQv3e9jt8aL3d1v2xu9D3zP/3jXSVAsNO6CVkKiBbHhwvx3ifXg1BsOX37zBUHLzpIPdxAyKrk/S8s/bCYGWSTkAjo33L6F9xnpFG8B7gmdsB5KTRJ+AvjEIVvrsQdY=&amp;cnc=false&amp;pickupPointCode=PP-3521786&amp;pid1=BLI-60043-01809&amp;tag=new</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>BLI-60051-00153</t>
+          <t>BLI-60043-01819</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Bliblimart</t>
+          <t>Fashion Pria</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Fitti</t>
+          <t>Bloods</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Fitti Pants M-32 Popok Celana</t>
+          <t>Bloods Series Boxer Barbed 02 Black</t>
         </is>
       </c>
       <c r="E31" t="n">
-        <v>43500</v>
+        <v>129000</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium//113/MTA-66772859/fitti_fitti_pants_m-32_popok_celana_full01_lc0aaueq.jpg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/101/MTA-168854230/brd-09186_bloods-series-boxer-barbed-02-black_full01-b74725a5.jpg</t>
         </is>
       </c>
       <c r="G31" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/fitti-pants-m-32-popok-celana/ps--BLI-60051-00153?ds=BLI-60051-00153-00001&amp;source=SEARCH&amp;sid=1629777a4a0387e4&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC7D5EnLGW/JufRUomLn7UXW/HAkxoVke7cxJ4LyInlLextyGfwhgQK76PRFevbPZllotyG7K9fuf6GhuhBg1qx5fpZP/HlAo0kBDTb857XQHO00wcIcM43S5kDh1UxrTh35uVJiiuCPRdlV4aliGvlC4/N0ykXdPBQ+Zmpzx07ptbgsUlSAp08Shy7kn+K2jxfTqqqGcrvj1CCDxi0R3X7jevLXBnmN3FEqYdm+HSwzK&amp;cnc=false&amp;pickupPointCode=PP-3137074&amp;pid1=BLI-60051-00153</t>
+          <t>https://www.blibli.com/p/bloods-series-boxer-barbed-02-black/ps--BLI-60043-01819?ds=BLI-60043-01819-00001&amp;source=SEARCH&amp;sid=eb3344a674df186d&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC2QNmx+r+f1ujpt2oEeckeCGkIqt3bNpbYK+L444UhhhU+qNVzNAHCfEDldNFubAdFesavfRnEsmWNUn9y9IGTPNbQv3e9jt8aL3d1v2xu9D3zP/3jXSVAsNO6CVkKiBbHhwvx3ifXg1BsOX37zBUHL9sb/8qEo2WC/FC2pJ0cgq9PvGCTEFtDAoi9ApC7l/76GluLHL7sh8udwFskycmSs=&amp;cnc=false&amp;pickupPointCode=PP-3521786&amp;pid1=BLI-60043-01819&amp;tag=new</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>BLS-60079-00384</t>
+          <t>BLI-60043-01820</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Bliblimart</t>
+          <t>Fashion Pria</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Confidence</t>
+          <t>Bloods</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Confidence Popok Celana XXL 10</t>
+          <t>Bloods Series Boxer Barbed 02 Black</t>
         </is>
       </c>
       <c r="E32" t="n">
-        <v>172900</v>
+        <v>129000</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium//103/MTA-87371076/confidence_confidence_premium_pants_xxl_10s_full01_kje6iw2v.jpg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/101/MTA-168854231/brd-09186_bloods-series-boxer-barbed-02-black_full01-bf2e3fbb.jpg</t>
         </is>
       </c>
       <c r="G32" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/confidence-popok-celana-xxl-10/ps--BLS-60079-00384?ds=BLS-60079-00384-00001&amp;source=SEARCH&amp;sid=1629777a4a0387e4&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC1ifcoeXCfsl309abOwHy+UYK73rVv9KyKDdReFaYxbBFT6wOPPQz1WLVq0UoKjafJbKIFVX5lKVfE28/P1rwwdP0HfjxNkfgWHG5INuEdtbni/RfXtjO+mLEBi1JvU4oOf9OamnFrvil6IltQoJVV59D3SjmueOfuYI/9W6zNJ4IDdMZLWnhXStRTEeVO4x1AuyDCwvEqOrKbGk02DOZSDwuJ0N+bwReUSR+pQh3lm5HHD7YxzuYdR4OGGpazCTKM5vVH7BzxqFyIibOEPK4xWeNw9uVSuVU2SAe4f07oEPZ2wHkpNEn4C+MQhW+uxB1g==&amp;cnc=false&amp;pickupPointCode=PP-3131546&amp;pid1=BLS-60079-00384</t>
+          <t>https://www.blibli.com/p/bloods-series-boxer-barbed-02-black/ps--BLI-60043-01820?ds=BLI-60043-01820-00001&amp;source=SEARCH&amp;sid=eb3344a674df186d&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC2QNmx+r+f1ujpt2oEeckeCGkIqt3bNpbYK+L444UhhhU+qNVzNAHCfEDldNFubAdFesavfRnEsmWNUn9y9IGTPNbQv3e9jt8aL3d1v2xu9D3zP/3jXSVAsNO6CVkKiBbHhwvx3ifXg1BsOX37zBUHL9sb/8qEo2WC/FC2pJ0cgq9PvGCTEFtDAoi9ApC7l/76GluLHL7sh8udwFskycmSs=&amp;cnc=false&amp;pickupPointCode=PP-3521786&amp;pid1=BLI-60043-01820&amp;tag=new</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>SOT-70038-00019</t>
+          <t>BLI-60043-01825</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Fashion Wanita</t>
+          <t>Fashion Pria</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Sovlo</t>
+          <t>Bloods</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Sovlo Sada Pants Celana Wanita  - Classic</t>
+          <t>Bloods Series Boxer Paper White Black</t>
         </is>
       </c>
       <c r="E33" t="n">
-        <v>139600</v>
+        <v>139000</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/MTA-38242854/sovlo_sovlo_sada_pants_celana_wanita__-_classic_full02_gv4cq690.jpeg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/103/MTA-168861045/brd-09186_bloods-series-boxer-paper-white-black_full01-f50caff3.jpg</t>
         </is>
       </c>
       <c r="G33" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/sovlo-sada-pants-celana-wanita-classic/ps--SOT-70038-00019?ds=SOT-70038-00019-00001&amp;source=SEARCH&amp;sid=1629777a4a0387e4&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC1cGXwSFpLJsXh2noxRjCItJfcCJiE9DzJp296UAYGk/DHoqKmYsTFC9Iv89Ei/0YlX6YqNL/N38iJlYkQlI2HD9cnB7A9Br96VNOoae/H1+BSFd02BuHmZWh0L7R6dhksB+tPNv9ITp+8ttAFmGt52x3MY/P1JCPR+VkZon1oF3vi6tL37cibBqpyoQOG6RAO1AbP/grvbJLIA0ySMLKu2DEC3cLXX0wtGQFaK7Z8yP&amp;cnc=false&amp;pickupPointCode=PP-3521260&amp;pid1=SOT-70038-00019</t>
+          <t>https://www.blibli.com/p/bloods-series-boxer-paper-white-black/ps--BLI-60043-01825?ds=BLI-60043-01825-00002&amp;source=SEARCH&amp;sid=eb3344a674df186d&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC1cGXwSFpLJsXh2noxRjCIuGkIqt3bNpbYK+L444UhhhU+qNVzNAHCfEDldNFubAdFesavfRnEsmWNUn9y9IGTPNbQv3e9jt8aL3d1v2xu9D3zP/3jXSVAsNO6CVkKiBbHhwvx3ifXg1BsOX37zBUHL9sb/8qEo2WC/FC2pJ0cgq9PvGCTEFtDAoi9ApC7l/76GluLHL7sh8udwFskycmSs=&amp;cnc=false&amp;pickupPointCode=PP-3521786&amp;pid1=BLI-60043-01825&amp;tag=new</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>BLI-60051-00152</t>
+          <t>BLI-60043-01818</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Bliblimart</t>
+          <t>Fashion Pria</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Fitti</t>
+          <t>Bloods</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Fitti Pants Popok Celana S-40</t>
+          <t>Bloods Series Boxer Barbed 01 Grey</t>
         </is>
       </c>
       <c r="E34" t="n">
-        <v>43500</v>
+        <v>129000</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium//105/MTA-66771546/fitti_fitti_pants_s-40_popok_celana_full01_bnpzc0pn.jpg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/107/MTA-168854228/brd-09186_bloods-series-boxer-barbed-01-grey_full01-33f3f2cb.jpg</t>
         </is>
       </c>
       <c r="G34" t="n">
-        <v>4.9</v>
+        <v>0</v>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/fitti-pants-popok-celana-s-40/ps--BLI-60051-00152?ds=BLI-60051-00152-00001&amp;source=SEARCH&amp;sid=1629777a4a0387e4&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC7D5EnLGW/JufRUomLn7UXW/HAkxoVke7cxJ4LyInlLe0NB2shiGJwkqZeuan2yTXVotyG7K9fuf6GhuhBg1qx5fpZP/HlAo0kBDTb857XQHO00wcIcM43S5kDh1UxrTh35uVJiiuCPRdlV4aliGvlC4/N0ykXdPBQ+Zmpzx07ptbgsUlSAp08Shy7kn+K2jxfTqqqGcrvj1CCDxi0R3X7jevLXBnmN3FEqYdm+HSwzK&amp;cnc=false&amp;pickupPointCode=PP-3137074&amp;pid1=BLI-60051-00152</t>
+          <t>https://www.blibli.com/p/bloods-series-boxer-barbed-01-grey/ps--BLI-60043-01818?ds=BLI-60043-01818-00001&amp;source=SEARCH&amp;sid=eb3344a674df186d&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC2QNmx+r+f1ujpt2oEeckeCGkIqt3bNpbYK+L444UhhhU+qNVzNAHCfEDldNFubAdFesavfRnEsmWNUn9y9IGTPNbQv3e9jt8aL3d1v2xu9D3zP/3jXSVAsNO6CVkKiBbHhwvx3ifXg1BsOX37zBUHL9sb/8qEo2WC/FC2pJ0cgq9PvGCTEFtDAoi9ApC7l/76GluLHL7sh8udwFskycmSs=&amp;cnc=false&amp;pickupPointCode=PP-3521786&amp;pid1=BLI-60043-01818&amp;tag=new</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>BLI-60051-00143</t>
+          <t>BLI-60043-01810</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Bliblimart</t>
+          <t>Fashion Pria</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Fitti</t>
+          <t>Bloods</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Fitti Pants Popok Celana XL-40</t>
+          <t>Bloods Pants Boardshort Boxer Testuo 01 Black</t>
         </is>
       </c>
       <c r="E35" t="n">
-        <v>62400</v>
+        <v>175000</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium//100/MTA-43492951/fitti_fitti_pants_xl-40_popok_celana_full01_syl4whp.jpg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/113/MTA-168852587/brd-09186_bloods-pants-boardshort-boxer-testuo-01-black_full01-7292e1e4.jpg</t>
         </is>
       </c>
       <c r="G35" t="n">
-        <v>4.9</v>
+        <v>0</v>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/fitti-pants-popok-celana-xl-40/ps--BLI-60051-00143?ds=BLI-60051-00143-00001&amp;source=SEARCH&amp;sid=1629777a4a0387e4&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC9lYjsoWJEyQX0Th4y0Bu9WX0LAHVJZ7EB+ox4oiZlNa6IImyrG79Dj2ct38qAiaJlotyG7K9fuf6GhuhBg1qx5fpZP/HlAo0kBDTb857XQHO00wcIcM43S5kDh1UxrTh35uVJiiuCPRdlV4aliGvlC4/N0ykXdPBQ+Zmpzx07ptbgsUlSAp08Shy7kn+K2jxfTqqqGcrvj1CCDxi0R3X7hTjBkITjtP4HiCHcESGOu9XpzEDZeRtkXgJo9qBPLejiQ5jyPy/a+1FRux7LeZEfwciMB3crEVshwW5gB3OxwZXrw/kjQPLGoA/IvdC3F8cA==&amp;cnc=false&amp;pickupPointCode=PP-3137074&amp;pid1=BLI-60051-00143</t>
+          <t>https://www.blibli.com/p/bloods-pants-boardshort-boxer-testuo-01-black/ps--BLI-60043-01810?ds=BLI-60043-01810-00003&amp;source=SEARCH&amp;sid=eb3344a674df186d&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC1ifcoeXCfsl309abOwHy+U0wn7+82bYRdE+2sGGRS84U+qNVzNAHCfEDldNFubAdFesavfRnEsmWNUn9y9IGTPNbQv3e9jt8aL3d1v2xu9D3zP/3jXSVAsNO6CVkKiBbHhwvx3ifXg1BsOX37zBUHL9sb/8qEo2WC/FC2pJ0cgq9PvGCTEFtDAoi9ApC7l/76GluLHL7sh8udwFskycmSs=&amp;cnc=false&amp;pickupPointCode=PP-3521786&amp;pid1=BLI-60043-01810&amp;tag=new</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>BLG-70029-00910</t>
+          <t>BLI-60043-01816</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Bliblimart</t>
+          <t>Fashion Pria</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>MamyPoko</t>
+          <t>Bloods</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Mamypoko Pants Skin Comfort Popok Celana [L-28]</t>
+          <t>Bloods Series Pants Boardshort Boxer Waish 01 Black</t>
         </is>
       </c>
       <c r="E36" t="n">
-        <v>73400</v>
+        <v>175000</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/MTA-50827042/mamypoko_mamypoko_pants_skin_comfort_l-28_popok_celana_full02_gsyk5yl4.jpeg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/103/MTA-168854016/brd-09186_bloods-series-pants-boardshort-boxer-waish-01-black_full01-31623d62.jpg</t>
         </is>
       </c>
       <c r="G36" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/mamypoko-pants-skin-comfort-popok-celana-l-28/ps--BLG-70029-00910?ds=BLG-70029-00910-00001&amp;source=SEARCH&amp;sid=1629777a4a0387e4&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC9nxsCWE66IToY6H/3TEJYiX0LAHVJZ7EB+ox4oiZlNafZP/GG3kitIJQ18VZrlDPVX6YqNL/N38iJlYkQlI2HD9cnB7A9Br96VNOoae/H1+BSFd02BuHmZWh0L7R6dhksB+tPNv9ITp+8ttAFmGt50F+DpLndLhhyOgRHezlp9aMvr1jaPBGR1Dff4JpGI+sYg1DCagL+VwGISeGTKUZdPkJ+go0SyaO5+o9d2cyg+S74S3wwI6k8I7omGYAl+u5o+WiGxwQPrk3UJlQOsxrERiB8ZtKTtsFLe2XdLeEKDs&amp;cnc=false&amp;pickupPointCode=PP-3329095&amp;pid1=BLG-70029-00910</t>
+          <t>https://www.blibli.com/p/bloods-series-pants-boardshort-boxer-waish-01-black/ps--BLI-60043-01816?ds=BLI-60043-01816-00001&amp;source=SEARCH&amp;sid=eb3344a674df186d&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC1ifcoeXCfsl309abOwHy+U0wn7+82bYRdE+2sGGRS84U+qNVzNAHCfEDldNFubAdFesavfRnEsmWNUn9y9IGTPNbQv3e9jt8aL3d1v2xu9D3zP/3jXSVAsNO6CVkKiBbHhwvx3ifXg1BsOX37zBUHLzpIPdxAyKrk/S8s/bCYGWSTkAjo33L6F9xnpFG8B7gmdsB5KTRJ+AvjEIVvrsQdY=&amp;cnc=false&amp;pickupPointCode=PP-3521786&amp;pid1=BLI-60043-01816&amp;tag=new</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>BLI-60051-00141</t>
+          <t>BLI-60043-01815</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Bliblimart</t>
+          <t>Fashion Pria</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Fitti</t>
+          <t>Bloods</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>Fitti Pants Popok Celana L-46</t>
+          <t>Bloods Series Pants Boardshort Boxer Waish 02 Navy</t>
         </is>
       </c>
       <c r="E37" t="n">
-        <v>62400</v>
+        <v>175000</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium//101/MTA-43492673/fitti_fitti_pants_l-46_popok_celana_full01_y5xrnyo.jpg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/102/MTA-168854015/brd-09186_bloods-series-pants-boardshort-boxer-waish-02-navy_full01-3c1cda22.jpg</t>
         </is>
       </c>
       <c r="G37" t="n">
-        <v>4.9</v>
+        <v>0</v>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/fitti-pants-popok-celana-l-46/ps--BLI-60051-00141?ds=BLI-60051-00141-00001&amp;source=SEARCH&amp;sid=1629777a4a0387e4&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC9lYjsoWJEyQX0Th4y0Bu9WX0LAHVJZ7EB+ox4oiZlNazpZF87QAsrFpzqYTQqEjKJbKIFVX5lKVfE28/P1rwwdP0HfjxNkfgWHG5INuEdtbni/RfXtjO+mLEBi1JvU4oOf9OamnFrvil6IltQoJVV6RJE4ryhs06fLidM+cAquoHfBjEULBfnPoMmI29KfUcrnWWHSsHM025lxc3a63JKE0YV6u4r6FHicjbNcfVIc5L8CuvvxNJQ0/xyIPqlVvyWd6dXDOQsttc82GbzPziJcxsCd03D4eBZi5acWIGP6X&amp;cnc=false&amp;pickupPointCode=PP-3137074&amp;pid1=BLI-60051-00141</t>
+          <t>https://www.blibli.com/p/bloods-series-pants-boardshort-boxer-waish-02-navy/ps--BLI-60043-01815?ds=BLI-60043-01815-00003&amp;source=SEARCH&amp;sid=eb3344a674df186d&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC1ifcoeXCfsl309abOwHy+U0wn7+82bYRdE+2sGGRS84U+qNVzNAHCfEDldNFubAdFesavfRnEsmWNUn9y9IGTPNbQv3e9jt8aL3d1v2xu9D3zP/3jXSVAsNO6CVkKiBbHhwvx3ifXg1BsOX37zBUHLzpIPdxAyKrk/S8s/bCYGWSTkAjo33L6F9xnpFG8B7gmdsB5KTRJ+AvjEIVvrsQdY=&amp;cnc=false&amp;pickupPointCode=PP-3521786&amp;pid1=BLI-60043-01815&amp;tag=new</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>BLI-60051-00155</t>
+          <t>BLI-60043-01813</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Bliblimart</t>
+          <t>Fashion Pria</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Fitti</t>
+          <t>Bloods</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Fitti Pants L-28 Popok Celana</t>
+          <t>Bloods Series Pants Boardshort Boxer Gramce 03 Black</t>
         </is>
       </c>
       <c r="E38" t="n">
-        <v>43500</v>
+        <v>175000</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium//108/MTA-66774528/fitti_fitti_pants_l-28_popok_celana_full01_la2csv61.jpg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/109/MTA-168853915/brd-09186_bloods-series-pants-boardshort-boxer-gramce-03-black_full03-e55b3e15.jpg</t>
         </is>
       </c>
       <c r="G38" t="n">
-        <v>4.9</v>
+        <v>0</v>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/fitti-pants-l-28-popok-celana/ps--BLI-60051-00155?ds=BLI-60051-00155-00001&amp;source=SEARCH&amp;sid=1629777a4a0387e4&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC7D5EnLGW/JufRUomLn7UXW/HAkxoVke7cxJ4LyInlLe+A636cuMmlSWwRxmlI+9F1otyG7K9fuf6GhuhBg1qx5fpZP/HlAo0kBDTb857XQHO00wcIcM43S5kDh1UxrTh35uVJiiuCPRdlV4aliGvlC4/N0ykXdPBQ+Zmpzx07ptbgsUlSAp08Shy7kn+K2jxfTqqqGcrvj1CCDxi0R3X7jevLXBnmN3FEqYdm+HSwzK&amp;cnc=false&amp;pickupPointCode=PP-3137074&amp;pid1=BLI-60051-00155</t>
+          <t>https://www.blibli.com/p/bloods-series-pants-boardshort-boxer-gramce-03-black/ps--BLI-60043-01813?ds=BLI-60043-01813-00003&amp;source=SEARCH&amp;sid=eb3344a674df186d&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC1ifcoeXCfsl309abOwHy+U0wn7+82bYRdE+2sGGRS84U+qNVzNAHCfEDldNFubAdFesavfRnEsmWNUn9y9IGTPNbQv3e9jt8aL3d1v2xu9D3zP/3jXSVAsNO6CVkKiBbHhwvx3ifXg1BsOX37zBUHL9sb/8qEo2WC/FC2pJ0cgq9PvGCTEFtDAoi9ApC7l/76GluLHL7sh8udwFskycmSs=&amp;cnc=false&amp;pickupPointCode=PP-3521786&amp;pid1=BLI-60043-01813&amp;tag=new</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>BLI-60051-00157</t>
+          <t>BLI-60043-01811</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Bliblimart</t>
+          <t>Fashion Pria</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Fitti</t>
+          <t>Bloods</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Fitti Pants Popok Celana XL-26</t>
+          <t>Bloods Series Pants Boardshort Boxer Gramce 02 Misty</t>
         </is>
       </c>
       <c r="E39" t="n">
-        <v>49200</v>
+        <v>175000</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium//115/MTA-66776479/fitti_fitti_pants_xl-26_popok_celana_full01_em7mpap2.jpg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/105/MTA-168853911/brd-09186_bloods-series-pants-boardshort-boxer-gramce-02-misty_full01-7e08c04b.jpg</t>
         </is>
       </c>
       <c r="G39" t="n">
-        <v>4.9</v>
+        <v>0</v>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/fitti-pants-popok-celana-xl-26/ps--BLI-60051-00157?ds=BLI-60051-00157-00001&amp;source=SEARCH&amp;sid=1629777a4a0387e4&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC+p/AVA0mwbANsVpLR+XCRnG7ZKryzxMhLfm5+J6+v8bIScvAZZWbsACaRFot3j/AlotyG7K9fuf6GhuhBg1qx5fpZP/HlAo0kBDTb857XQHO00wcIcM43S5kDh1UxrTh35uVJiiuCPRdlV4aliGvlC4/N0ykXdPBQ+Zmpzx07ptbgsUlSAp08Shy7kn+K2jxfTqqqGcrvj1CCDxi0R3X7jevLXBnmN3FEqYdm+HSwzK&amp;cnc=false&amp;pickupPointCode=PP-3137074&amp;pid1=BLI-60051-00157</t>
+          <t>https://www.blibli.com/p/bloods-series-pants-boardshort-boxer-gramce-02-misty/ps--BLI-60043-01811?ds=BLI-60043-01811-00001&amp;source=SEARCH&amp;sid=eb3344a674df186d&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC1ifcoeXCfsl309abOwHy+U0wn7+82bYRdE+2sGGRS84U+qNVzNAHCfEDldNFubAdFesavfRnEsmWNUn9y9IGTPNbQv3e9jt8aL3d1v2xu9D3zP/3jXSVAsNO6CVkKiBbHhwvx3ifXg1BsOX37zBUHLzpIPdxAyKrk/S8s/bCYGWSTkAjo33L6F9xnpFG8B7gmdsB5KTRJ+AvjEIVvrsQdY=&amp;cnc=false&amp;pickupPointCode=PP-3521786&amp;pid1=BLI-60043-01811&amp;tag=new</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>BLI-60051-00154</t>
+          <t>BLI-60043-01812</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Bliblimart</t>
+          <t>Fashion Pria</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Fitti</t>
+          <t>Bloods</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Fitti Pants M-32 Popok Celana - 3 Packs</t>
+          <t>Bloods Series Pants Boardshort Boxer Gramce 01 Navy</t>
         </is>
       </c>
       <c r="E40" t="n">
-        <v>130700</v>
+        <v>175000</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium//111/MTA-66773649/fitti_fitti_pants_m-32_popok_celana_-_3_packs_full01_ck3cs7y8.jpg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/107/MTA-168853913/brd-09186_bloods-series-pants-boardshort-boxer-gramce-01-navy_full01-552792fa.jpg</t>
         </is>
       </c>
       <c r="G40" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/fitti-pants-m-32-popok-celana-3-packs/ps--BLI-60051-00154?ds=BLI-60051-00154-00001&amp;source=SEARCH&amp;sid=1629777a4a0387e4&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC1cGXwSFpLJsXh2noxRjCIvC3B+deCLZjcmojlYJayMnmp8jZiT09CnDGiL5QFb0F+Wk7L/WjZW4V3T1+QzDEpiZTqX+08YMFPt67oXduO/veDye5g4cJG51p5fjAlqNKr3Qa6Aw9nJN8ZS3vPJl9087KBj1oW91VVdgmsyeMwxA1ZBkU0NcX4uiXe/YPsHDKqnA5D4DcAHjNP9dlSC5zDcBe4P5AIu+eFkdqNkTRIAr&amp;cnc=false&amp;pickupPointCode=PP-3137074&amp;pid1=BLI-60051-00154</t>
+          <t>https://www.blibli.com/p/bloods-series-pants-boardshort-boxer-gramce-01-navy/ps--BLI-60043-01812?ds=BLI-60043-01812-00001&amp;source=SEARCH&amp;sid=eb3344a674df186d&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC1ifcoeXCfsl309abOwHy+U0wn7+82bYRdE+2sGGRS84U+qNVzNAHCfEDldNFubAdFesavfRnEsmWNUn9y9IGTPNbQv3e9jt8aL3d1v2xu9D3zP/3jXSVAsNO6CVkKiBbHhwvx3ifXg1BsOX37zBUHL9sb/8qEo2WC/FC2pJ0cgq9PvGCTEFtDAoi9ApC7l/76GluLHL7sh8udwFskycmSs=&amp;cnc=false&amp;pickupPointCode=PP-3521786&amp;pid1=BLI-60043-01812&amp;tag=new</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>BLI-60051-00140</t>
+          <t>BLI-60043-01817</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Bliblimart</t>
+          <t>Fashion Pria</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Fitti</t>
+          <t>Bloods</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Fitti Pants M-52 Popok Celana - 4 Packs</t>
+          <t>Bloods Series Pants Boardshort Boxer Waish 03 Dark Grey</t>
         </is>
       </c>
       <c r="E41" t="n">
-        <v>259700</v>
+        <v>175000</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium//97/MTA-43492516/fitti_fitti_pants_m-52_popok_celana_-_4_packs_full01_iuwxylzh.jpg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/108/MTA-168854039/brd-09186_bloods-series-pants-boardshort-boxer-waish-03-dark-grey_full01-056e9377.jpg</t>
         </is>
       </c>
       <c r="G41" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/fitti-pants-m-52-popok-celana-4-packs/ps--BLI-60051-00140?ds=BLI-60051-00140-00001&amp;source=SEARCH&amp;sid=1629777a4a0387e4&amp;metaData=SnHZRCX7NPLsJ+ExPEFNCzO4NENA+D3a2b160XD/ATD26SWwN3NVPmUUl3LL6fRhM0NJV/28Uln3kFK/gRH/wOWk7L/WjZW4V3T1+QzDEpiZTqX+08YMFPt67oXduO/veDye5g4cJG51p5fjAlqNKr3Qa6Aw9nJN8ZS3vPJl9087KBj1oW91VVdgmsyeMwxA1ZBkU0NcX4uiXe/YPsHDKqnA5D4DcAHjNP9dlSC5zDcBe4P5AIu+eFkdqNkTRIAr&amp;cnc=false&amp;pickupPointCode=PP-3137074&amp;pid1=BLI-60051-00140</t>
+          <t>https://www.blibli.com/p/bloods-series-pants-boardshort-boxer-waish-03-dark-grey/ps--BLI-60043-01817?ds=BLI-60043-01817-00002&amp;source=SEARCH&amp;sid=eb3344a674df186d&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC1ifcoeXCfsl309abOwHy+U0wn7+82bYRdE+2sGGRS84U+qNVzNAHCfEDldNFubAdFesavfRnEsmWNUn9y9IGTPNbQv3e9jt8aL3d1v2xu9D3zP/3jXSVAsNO6CVkKiBbHhwvx3ifXg1BsOX37zBUHLzpIPdxAyKrk/S8s/bCYGWSTkAjo33L6F9xnpFG8B7gmdsB5KTRJ+AvjEIVvrsQdY=&amp;cnc=false&amp;pickupPointCode=PP-3521786&amp;pid1=BLI-60043-01817&amp;tag=new</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
add to cart functionality and loading progress with percentage
</commit_message>
<xml_diff>
--- a/ui_data/blibli.xlsx
+++ b/ui_data/blibli.xlsx
@@ -432,13 +432,13 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="17" customWidth="1" min="1" max="1"/>
-    <col width="24" customWidth="1" min="2" max="2"/>
+    <col width="16" customWidth="1" min="2" max="2"/>
     <col width="58.33333333333334" customWidth="1" min="3" max="3"/>
-    <col width="98" customWidth="1" min="4" max="4"/>
+    <col width="93" customWidth="1" min="4" max="4"/>
     <col width="10" customWidth="1" min="5" max="5"/>
-    <col width="228" customWidth="1" min="6" max="6"/>
+    <col width="214" customWidth="1" min="6" max="6"/>
     <col width="8" customWidth="1" min="7" max="7"/>
-    <col width="597" customWidth="1" min="8" max="8"/>
+    <col width="531" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -486,107 +486,106 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>BLI-60060-00017</t>
+          <t>SOO-60051-01043</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Bliblimart</t>
+          <t>Fashion Wanita</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>S-26</t>
+          <t>Sorex</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t xml:space="preserve">S-26 Promise Tahap 4 Susu Formula [1400 g x 3 pcs] 
-</t>
+          <t>Sorex Bra Seamless Tanpa Kawat Kait 2 Cup A-B Busa Tipis BH 65004</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>840000</v>
+        <v>61600</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium//100/MTA-6816178/S26_S26_Promise_Tahap_4_Susu_Formula_-1400_g-_x_3_Pcs_full01_n2gaw9ux.jpg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/101/MTA-159825520/sorex_sorex_bra_seamless_tanpa_kawat_kait_2_cup_a-b_busa_tipis_bh_65004_full02_ds94bo75.jpg</t>
         </is>
       </c>
       <c r="G2" t="n">
-        <v>4.9</v>
+        <v>5</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/s-26-promise-tahap-4-susu-formula-1400-g-x-3-pcs/ps--BLI-60060-00017?ds=BLI-60060-00017-00001&amp;source=SEARCH&amp;sid=e132f3cdc0f57c22&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC+9KgQwIVJt8z/dR363VuzwH5hXXWkF0dKfPGTdZQcdl+cGcreNGPDrmTP7Ktv5yJNldH9pXtqj8cRFTERUal3Bpz33rJJwAjBRbAFmAxRYrR2JC8yefRRKTBapN1Wd/InPP1hTAELZMPkG2ugw4qQC9MlocLc/g5WkcBM2SJQmdEBnb9qyL5HQbNMV2/+3IhSDwF+P/lDvyT3bjUeeQy534fdprL2an9+zGt6lCF7URnQgdYn7q211GPDma9F6OBOnmGXFanEBshpSoYFwZaF8Gy7v8OIeE3eVAfqXOI+h1X8lHI6X0LWwx6iahbExNOw==&amp;cnc=false&amp;pickupPointCode=PP-3162573&amp;pid1=BLI-60060-00017</t>
+          <t>https://www.blibli.com/p/sorex-bra-seamless-tanpa-kawat-kait-2-cup-a-b-busa-tipis-bh-65004/ps--SOO-60051-01043?ds=SOO-60051-01043-00007&amp;source=SEARCH&amp;sid=6250e0eb050ab5a0&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC8wDol3ZkqhTHXjds9fEyH5nh6wQ6PEr8y5kW/jpBoqaJpxUsLAohHVwJa3vwtOUsujqrM/mjls6JQDzIHvTluMiB4zoBbkTKkiVxxU6hr74PdxTHKZBV9wukrN4w82/yWp5HoWHuYDNl07Gpt+tmXfO/kFtVj4porywlY2UWbf6VMqwppbx5Qk9+27gygWs9sZi4HFMNt1hNudy6hVQGo9fyUcjpfQtbDHqJqFsTE07&amp;cnc=false&amp;pickupPointCode=PP-3126072&amp;pid1=SOO-60051-01043</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>BLI-60054-00163</t>
+          <t>SOO-60051-00995</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Bliblimart</t>
+          <t>Fashion Pria</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>SGM</t>
+          <t>Sorex</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>SGM Ananda 2 (6-12 Bulan) Susu Formula [600 g]</t>
+          <t>(2 PCS) Sorex Man Lifetyle Boxer Pria Celana Dalam Cowo Adem Trunk LK 38285</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>58200</v>
+        <v>69000</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/MTA-6338547/sgm_sgm_ananda_2_-6-12_bulan-_susu_formula_-600_g-_full13_bkwj7928.jpeg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium//catalog-image/103/MTA-147676135/sorex_-2_pcs-_sorex_man_lifetyle_boxer_pria_celana_dalam_cowo_adem_trunk_lk_38285_full04_futs8yik.jpg</t>
         </is>
       </c>
       <c r="G3" t="n">
-        <v>4.9</v>
+        <v>5</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/sgm-ananda-2-6-12-bulan-susu-formula-600-g/ps--BLI-60054-00163?ds=BLI-60054-00163-00001&amp;source=SEARCH&amp;sid=e132f3cdc0f57c22&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC0Io8iY7bS3QFgUrrRjl8b/G7ZKryzxMhLfm5+J6+v8b1a+8iQty2s7WQ/5m9moOdZbKIFVX5lKVfE28/P1rwwdP0HfjxNkfgWHG5INuEdtbni/RfXtjO+mLEBi1JvU4oOf9OamnFrvil6IltQoJVV6RJE4ryhs06fLidM+cAquoweejFuSR+ejFuz0MPHOoPqeae2Mr7kUSCRhQl4RITCZjUqFP11h9zlqNWNkuhtN0vavFjQW+Hi0U1g5VsfADeL+0KlWZP9TCw01G7E1sRkY=&amp;cnc=false&amp;pickupPointCode=PP-3137092&amp;pid1=BLI-60054-00163</t>
+          <t>https://www.blibli.com/p/2-pcs-sorex-man-lifetyle-boxer-pria-celana-dalam-cowo-adem-trunk-lk-38285/ps--SOO-60051-00995?ds=SOO-60051-00995-00001&amp;source=SEARCH&amp;sid=6250e0eb050ab5a0&amp;metaData=SnHZRCX7NPLsJ+ExPEFNCwNduFYwfvFwnmds8RU/70OT2r7fOYNS0fn24lYkspaBA+hoPN7IuiYgrYrEmVR4uujqrM/mjls6JQDzIHvTluMiB4zoBbkTKkiVxxU6hr74PdxTHKZBV9wukrN4w82/yWp5HoWHuYDNl07Gpt+tmXfEjjW01Qnp2OSK0iQtfojJf8tZrf2s64VqZXfbnwqrhtlkcl11OleYOCUgny6Mmrc=&amp;cnc=false&amp;pickupPointCode=PP-3126072&amp;pid1=SOO-60051-00995</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>MA9-60026-00512</t>
+          <t>SOO-60051-00913</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Bliblimart</t>
+          <t>Ibu &amp; Anak</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Diamond</t>
+          <t>Sorex</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Diamond Full Cream Susu UHT 1000 mL</t>
+          <t>Sorex Young Miniset Anak Remaja Step 1 Tanpa Kawat Visha Y 1013</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>16990</v>
+        <v>25800</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium//99/MTA-59116824/diamond_diamond_uht_1_liter_full01_f750ec45.jpg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium//catalog-image/97/MTA-136183074/sorex_sorex_young_miniset_anak_remaja_step_1_tanpa_kawat_visha_y_1013_full02_ummhstw2.jpg</t>
         </is>
       </c>
       <c r="G4" t="n">
@@ -594,37 +593,37 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/diamond-full-cream-susu-uht-1000-ml/ps--MA9-60026-00512?ds=MA9-60026-00512-00001&amp;source=SEARCH&amp;sid=e132f3cdc0f57c22&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC7Icmq1gsSXLUq8ZinzLw7v+oLJqLy/XvDHMcpKt+HY66c5Rv2pwKiFp//o451F+FJbKIFVX5lKVfE28/P1rwwdP0HfjxNkfgWHG5INuEdtbni/RfXtjO+mLEBi1JvU4oOf9OamnFrvil6IltQoJVV7gVFzNUgTsVxnEJaAi206QylkZHer+F/DmhPZJvYm9VGEkj8u/5h4Kyn3dAqlMr+Xi4YSCsa/SsFeuwwC/3BZ9vavFjQW+Hi0U1g5VsfADeL+0KlWZP9TCw01G7E1sRkY=&amp;cnc=false&amp;pickupPointCode=PP-3525762&amp;pid1=MA9-60026-00512</t>
+          <t>https://www.blibli.com/p/sorex-young-miniset-anak-remaja-step-1-tanpa-kawat-visha-y-1013/ps--SOO-60051-00913?ds=SOO-60051-00913-00002&amp;source=SEARCH&amp;sid=6250e0eb050ab5a0&amp;metaData=SnHZRCX7NPLsJ+ExPEFNCzO4NENA+D3a2b160XD/ATBl2MnZWZ1TwAwuODpbBDUV/judXluBkrGQbYL5wQ1heujqrM/mjls6JQDzIHvTluMiB4zoBbkTKkiVxxU6hr74PdxTHKZBV9wukrN4w82/yWp5HoWHuYDNl07Gpt+tmXfE8Fq3Y7FQDm7GSllvB0EzwRUapLx/yCmHBm+F6S9MPxAR75Szd5AvP5iOPg1fnThfyUcjpfQtbDHqJqFsTE07&amp;cnc=false&amp;pickupPointCode=PP-3126072&amp;pid1=SOO-60051-00913</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>BLG-70029-06124</t>
+          <t>SOO-60051-00861</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Bliblimart</t>
+          <t>Fashion Wanita</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Ultra Jaya</t>
+          <t>Sorex</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Clearance - Ultra Milk Low Fat Chocolate Susu UHT [1000ml]</t>
+          <t>Sorex Celana Dalam Katun Basic Cutting Midi Polos Shape Up CD 9075</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>19200</v>
+        <v>36800</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium//catalog-image/106/MTA-134387079/ultra_jaya_ultra_milk_low_fat_chocolate_100ml_full05_vb5kqszl.jpg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/MTA-112996396/sorex_sorex_celana_dalam_katun_basic_cutting_midi_polos_shape_up_cd_9075_full02_kdz4sy7w.jpg</t>
         </is>
       </c>
       <c r="G5" t="n">
@@ -632,151 +631,151 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/clearance-ultra-milk-low-fat-chocolate-susu-uht-1000ml/ps--BLG-70029-06124?ds=BLG-70029-06124-00001&amp;source=SEARCH&amp;sid=e132f3cdc0f57c22&amp;metaData=SnHZRCX7NPLsJ+ExPEFNCyyDdutSjnAKjW/qtRSWe1LG7ZKryzxMhLfm5+J6+v8bT4SwC3dPYQxOfUGC+4Sn7VesavfRnEsmWNUn9y9IGTPNbQv3e9jt8aL3d1v2xu9D3zP/3jXSVAsNO6CVkKiBbHhwvx3ifXg1BsOX37zBUHIopPuOXO3ZPFXx1Ozq+hxbn0t+Z31N/tG70rzxf062H4Scv7qvXlsLo00FBKrsBre0XBPM8Ib69hRyb0y0TLR/&amp;cnc=false&amp;pickupPointCode=PP-3526957&amp;pid1=BLG-70029-06124</t>
+          <t>https://www.blibli.com/p/sorex-celana-dalam-katun-basic-cutting-midi-polos-shape-up-cd-9075/ps--SOO-60051-00861?ds=SOO-60051-00861-00001&amp;source=SEARCH&amp;sid=6250e0eb050ab5a0&amp;metaData=SnHZRCX7NPLsJ+ExPEFNCzL10t6deH8IJLci3UQaGCFl2MnZWZ1TwAwuODpbBDUVJpxUsLAohHVwJa3vwtOUsujqrM/mjls6JQDzIHvTluMiB4zoBbkTKkiVxxU6hr74PdxTHKZBV9wukrN4w82/yWp5HoWHuYDNl07Gpt+tmXfO/kFtVj4porywlY2UWbf6VMqwppbx5Qk9+27gygWs9lk0gjRbIbx9mhzaC4fFgmtfyUcjpfQtbDHqJqFsTE07&amp;cnc=false&amp;pickupPointCode=PP-3126072&amp;pid1=SOO-60051-00861</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>BLG-70029-00032</t>
+          <t>SOO-60051-00829</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Bliblimart</t>
+          <t>Fashion Wanita</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Indomilk</t>
+          <t>Sorex</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Indomilk Full Cream Plain Susu UHT [950 mL] - D</t>
+          <t>Sorex Celana Dalam Wanita Hamil Midi Maternity Panty Freesize CD 1145</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>17000</v>
+        <v>33075</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium//99/MTA-42236388/indomilk_indomilk_full_cream_plain_susu_uht_-950_ml-_full05_c9ijxfq.jpg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/MTA-70479327/sorex_sorex_celana_dalam_wanita_hamil_midi_maternity_panty_freesize_cd_1145_full02_hb7mng6q.jpeg</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>4.9</v>
+        <v>5</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/indomilk-full-cream-plain-susu-uht-950-ml-d/ps--BLG-70029-00032?ds=BLG-70029-00032-00001&amp;source=SEARCH&amp;sid=e132f3cdc0f57c22&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC1ifcoeXCfsl309abOwHy+WT2r7fOYNS0fn24lYkspaBvQ+zpQtxgrRypwW88+WUuFX6YqNL/N38iJlYkQlI2HD9cnB7A9Br96VNOoae/H1+BSFd02BuHmZWh0L7R6dhksB+tPNv9ITp+8ttAFmGt53nU4Dp3uhlwixflscAf8XVNd9Qdrb3QWYxenklePSJm24qiwzrO6nWnHsxgeryKb/ltUNk96VTdqdjG4caO5Q1wCaCWmOutPc0eIowrS/xtbSlp5iaPRa3auHKDapyNXA=&amp;cnc=false&amp;pickupPointCode=PP-3526957&amp;pid1=BLG-70029-00032</t>
+          <t>https://www.blibli.com/p/sorex-celana-dalam-wanita-hamil-midi-maternity-panty-freesize-cd-1145/ps--SOO-60051-00829?ds=SOO-60051-00829-00001&amp;source=SEARCH&amp;sid=6250e0eb050ab5a0&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC8ZIN0KweYTfTnX/ul7fF5HqWD619BPrHnoq4EdKnykUJpxUsLAohHVwJa3vwtOUsujqrM/mjls6JQDzIHvTluMiB4zoBbkTKkiVxxU6hr74PdxTHKZBV9wukrN4w82/yWp5HoWHuYDNl07Gpt+tmXfO/kFtVj4porywlY2UWbf6VMqwppbx5Qk9+27gygWs9lk0gjRbIbx9mhzaC4fFgmtfyUcjpfQtbDHqJqFsTE07&amp;cnc=false&amp;pickupPointCode=PP-3126072&amp;pid1=SOO-60051-00829</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>RAM-70107-01154</t>
+          <t>SOO-60051-00769</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Bliblimart</t>
+          <t>Ibu &amp; Anak</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Greenfields</t>
+          <t>Sorex</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Greenfields uht full cream 1lt tta</t>
+          <t>Sorex Celana Dalam Wanita Hamil Midi Maternity Panty Fit To L-XXL CD 1148</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>18500</v>
+        <v>41895</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium//96/MTA-21517269/greenfields_greenfields_uht_full_cream___1lt_tta_full01_kzb8pgtf.jpg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/MTA-46523947/sorex_sorex_celana_dalam_wanita_hamil_midi_maternity_panty_fit_to_l-xxl_cd_1148_full01_r4vls97f.jpg</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>4.9</v>
+        <v>5</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/greenfields-uht-full-cream-1lt-tta/ps--RAM-70107-01154?ds=RAM-70107-01154-00001&amp;source=SEARCH&amp;sid=e132f3cdc0f57c22&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC83UCraFZ0P7NET872xC0wi/HAkxoVke7cxJ4LyInlLe47tJ7v5exg+yWovfFoMw1ZbKIFVX5lKVfE28/P1rwwdP0HfjxNkfgWHG5INuEdtbni/RfXtjO+mLEBi1JvU4oOf9OamnFrvil6IltQoJVV7gVFzNUgTsVxnEJaAi206QylkZHer+F/DmhPZJvYm9VGEkj8u/5h4Kyn3dAqlMr+Xi4YSCsa/SsFeuwwC/3BZ9vavFjQW+Hi0U1g5VsfADeL+0KlWZP9TCw01G7E1sRkY=&amp;cnc=false&amp;pickupPointCode=PP-3507456&amp;pid1=RAM-70107-01154</t>
+          <t>https://www.blibli.com/p/sorex-celana-dalam-wanita-hamil-midi-maternity-panty-fit-to-l-xxl-cd-1148/ps--SOO-60051-00769?ds=SOO-60051-00769-00001&amp;source=SEARCH&amp;sid=6250e0eb050ab5a0&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC5nGzsCVntCT1sSfFwqgrxg8vkblbwv0+E1QlSs7EtdUJpxUsLAohHVwJa3vwtOUsujqrM/mjls6JQDzIHvTluMiB4zoBbkTKkiVxxU6hr74PdxTHKZBV9wukrN4w82/yWp5HoWHuYDNl07Gpt+tmXdtbUEB2KN2y84saGW8FURoFNpMZjfoNazsAekWU+LFfRtd5JisA+krezcArUVhBa3TrWgM/WffSFIKvZxBffSZ&amp;cnc=false&amp;pickupPointCode=PP-3126072&amp;pid1=SOO-60051-00769</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>MIU-60036-00152</t>
+          <t>SOO-60051-00471</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Bliblimart</t>
+          <t>Fashion Wanita</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>MilkLife</t>
+          <t>Sorex</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>MilkLife UHT Chocolate Milk 1000 mL</t>
+          <t>Sorex 17232 Casual Style Bra - Cup B</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>19200</v>
+        <v>39004</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium//catalog-image/MTA-96886606/milklife_milklife_uht_chocolate_milk_-_susu_cokelat_-1000_ml-_full01_mfw3cdmh.jpeg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium//103/MTA-12493876/sorex_sorex_bra_busa_tanpa_kawat_kait_2_setara_cup_b_bh_harian_casual_style_bra_17232_full01_rx5utll6.jpg</t>
         </is>
       </c>
       <c r="G8" t="n">
-        <v>4.9</v>
+        <v>5</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/milklife-uht-chocolate-milk-1000-ml/ps--MIU-60036-00152?ds=MIU-60036-00152-00001&amp;source=SEARCH&amp;sid=e132f3cdc0f57c22&amp;metaData=SnHZRCX7NPLsJ+ExPEFNCyyDdutSjnAKjW/qtRSWe1LG7ZKryzxMhLfm5+J6+v8b4PQDwO5jLIz1mN9xTajwh1otyG7K9fuf6GhuhBg1qx5fpZP/HlAo0kBDTb857XQHO00wcIcM43S5kDh1UxrTh35uVJiiuCPRdlV4aliGvlC4/N0ykXdPBQ+Zmpzx07ptbgsUlSAp08Shy7kn+K2jxU/1fLwUXvMEGcJP8vYHs+i70aAZfLEhItHKJnBRk5mOXfqn7ztN/d1UPKnyy4npw4ALYVsVJ0CULUmRipV0cZnFS2Bs6MqaweAs0BMvmAIOK75dCgVySnSnFnHvJRwecg==&amp;cnc=false&amp;pickupPointCode=PP-3243836&amp;pid1=MIU-60036-00152</t>
+          <t>https://www.blibli.com/p/sorex-17232-casual-style-bra-cup-b/ps--SOO-60051-00471?ds=SOO-60051-00471-00008&amp;source=SEARCH&amp;sid=6250e0eb050ab5a0&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC8ABEbUv77oGEmdGsuoM43/eggqgMiupqXxacM5eGPWfJpxUsLAohHVwJa3vwtOUsujqrM/mjls6JQDzIHvTluMiB4zoBbkTKkiVxxU6hr74PdxTHKZBV9wukrN4w82/yWp5HoWHuYDNl07Gpt+tmXfO/kFtVj4porywlY2UWbf6VMqwppbx5Qk9+27gygWs9sZi4HFMNt1hNudy6hVQGo9fyUcjpfQtbDHqJqFsTE07&amp;cnc=false&amp;pickupPointCode=PP-3126072&amp;pid1=SOO-60051-00471</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>BLD-60037-00350</t>
+          <t>SOO-60051-00552</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Bliblimart</t>
+          <t>Fashion Wanita</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Frisian Flag</t>
+          <t>Sorex</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>WHS - Frisian Flag Purefarm Susu UHT Sereal Cokelat [225 mL]</t>
+          <t>Sorex CD wanita Midi Super Soft Adem Lembut CD 15232</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>4400</v>
+        <v>20580</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium//catalog-image/92/MTA-128028214/frisian_flag_frisian_flag_purefarm_susu_uht_sereal_cokelat_-225_ml-_full01_dgqxv6tx.jpg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/MTA-20762030/sorex_sorex_cd_wanita_midi_super_soft_adem_lembut_cd_15232_full02_rfcio72k.jpeg</t>
         </is>
       </c>
       <c r="G9" t="n">
@@ -784,37 +783,37 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/whs-frisian-flag-purefarm-susu-uht-sereal-cokelat-225-ml/ps--BLD-60037-00350?ds=BLD-60037-00350-00001&amp;source=SEARCH&amp;sid=e132f3cdc0f57c22&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC/yWWkfvbmGmkfSwUzmXNKO3VQ2WlzHp9deWrxqynfgSKG/XOj6f7+guuhEd6Le9MOjqrM/mjls6JQDzIHvTluMiB4zoBbkTKkiVxxU6hr74PdxTHKZBV9wukrN4w82/yWp5HoWHuYDNl07Gpt+tmXeDioWrdqW2jVDexSAU462NTDhvU2dGTHXFRrWe7cayKOxVR1NKRIdNH5nx1LcA2EBgK3eW+Zh5x4g6PLMg3Mki3xH6A1SDCPhEv9COJBZsutoKTrVSRDI+tQZ6wB+l2Bk=&amp;cnc=false&amp;pickupPointCode=PP-3098866&amp;pid1=BLD-60037-00350</t>
+          <t>https://www.blibli.com/p/sorex-cd-wanita-midi-super-soft-adem-lembut-cd-15232/ps--SOO-60051-00552?ds=SOO-60051-00552-00001&amp;source=SEARCH&amp;sid=6250e0eb050ab5a0&amp;metaData=SnHZRCX7NPLsJ+ExPEFNCxzohPZzaxyiJv5ug5c6gt2aqponFxzbpAb1YzoA8RzrJpxUsLAohHVwJa3vwtOUsujqrM/mjls6JQDzIHvTluMiB4zoBbkTKkiVxxU6hr74PdxTHKZBV9wukrN4w82/yWp5HoWHuYDNl07Gpt+tmXfO/kFtVj4porywlY2UWbf6VMqwppbx5Qk9+27gygWs9lk0gjRbIbx9mhzaC4fFgmtfyUcjpfQtbDHqJqFsTE07&amp;cnc=false&amp;pickupPointCode=PP-3126072&amp;pid1=SOO-60051-00552</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>BLG-70029-06975</t>
+          <t>SOO-60051-00012</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Bliblimart</t>
+          <t>Fashion Wanita</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Indomilk</t>
+          <t>Sorex</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Indomilk Strawberry Susu UHT 115 mL</t>
+          <t>Sorex CD Basic Maxi Super Light Celana Dalam Wanita Extra Size Jumbo 1249</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>2600</v>
+        <v>37044</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium//catalog-image/98/MTA-145643138/indomilk_indomilk_strawberry_susu_uht_-115_ml-_full07_bsx9t01i.jpg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/MTA-7709188/sorex_sorex_cd_basic_maxi_super_light_celana_dalam_wanita_extra_size_jumbo_1249_full02_m8u3eoep.jpg</t>
         </is>
       </c>
       <c r="G10" t="n">
@@ -822,37 +821,37 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/indomilk-strawberry-susu-uht-115-ml/ps--BLG-70029-06975?ds=BLG-70029-06975-00001&amp;source=SEARCH&amp;sid=e132f3cdc0f57c22&amp;metaData=SnHZRCX7NPLsJ+ExPEFNCwR0bgev9saiJ9QpuPsgXPy3VQ2WlzHp9deWrxqynfgSxHz9g6yXVsVL9UZIHPpNiFesavfRnEsmWNUn9y9IGTPNbQv3e9jt8aL3d1v2xu9D3zP/3jXSVAsNO6CVkKiBbHhwvx3ifXg1BsOX37zBUHIopPuOXO3ZPFXx1Ozq+hxbn0t+Z31N/tG70rzxf062H4Scv7qvXlsLo00FBKrsBre0XBPM8Ib69hRyb0y0TLR/&amp;cnc=false&amp;pickupPointCode=PP-3329095&amp;pid1=BLG-70029-06975</t>
+          <t>https://www.blibli.com/p/sorex-cd-basic-maxi-super-light-celana-dalam-wanita-extra-size-jumbo-1249/ps--SOO-60051-00012?ds=SOO-60051-00012-00002&amp;source=SEARCH&amp;sid=6250e0eb050ab5a0&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC/uzJZ4qiKCUsLXY6fa2mZsQHMYoO9/9ygcijfF65PUOJpxUsLAohHVwJa3vwtOUsujqrM/mjls6JQDzIHvTluMiB4zoBbkTKkiVxxU6hr74PdxTHKZBV9wukrN4w82/yWp5HoWHuYDNl07Gpt+tmXfO/kFtVj4porywlY2UWbf6VMqwppbx5Qk9+27gygWs9lk0gjRbIbx9mhzaC4fFgmtfyUcjpfQtbDHqJqFsTE07&amp;cnc=false&amp;pickupPointCode=PP-3126072&amp;pid1=SOO-60051-00012</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>BLG-70029-03091</t>
+          <t>SOO-60051-00362</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Bliblimart</t>
+          <t>Ibu &amp; Anak</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Indomilk</t>
+          <t>Sorex</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Indomilk Vanila Susu UHT [115 mL]</t>
+          <t>Sorex Celana Dalam Wanita Ibu Hamil Maxi Katun Maternity Panty Freesize CD 1138</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>2600</v>
+        <v>36260</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium//94/MTA-90082451/indomilk_indomilk_vanila_susu_uht_-115_ml-_full07_el00nnve.jpg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/MTA-10651111/sorex_sorex_celana_dalam_wanita_ibu_hamil_maxi_katun_maternity_panty_freesize_cd_1138_full02_ptla6keg.jpg</t>
         </is>
       </c>
       <c r="G11" t="n">
@@ -860,37 +859,37 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/indomilk-vanila-susu-uht-115-ml/ps--BLG-70029-03091?ds=BLG-70029-03091-00001&amp;source=SEARCH&amp;sid=e132f3cdc0f57c22&amp;metaData=SnHZRCX7NPLsJ+ExPEFNCwR0bgev9saiJ9QpuPsgXPy3VQ2WlzHp9deWrxqynfgSUOva+erg1zhRP8ORuqdB0Fa8f1JvScJ6DrHwqmhDSmJ38pLvQtrJkjvO7Vji06N5Y/z3GNGYn0VDwoIIPnDgZ5AnoLYwmKE1R7OS9+9VGfqViJT0I/qzo1dSRzxYbUZ/ex2pbIx4kQWkh1axBx2JSth7xMW6cmCR+WDrARSDFb7+rUtXImUPAV3D58kpwIYQ3+aoZiWtW16AA4AzyHvVpdxcinYBStTbM0E99KPslfQaUy5QgCcBieU0mQhMExcU&amp;cnc=false&amp;pickupPointCode=PP-3528098&amp;pid1=BLG-70029-03091</t>
+          <t>https://www.blibli.com/p/sorex-celana-dalam-wanita-ibu-hamil-maxi-katun-maternity-panty-freesize-cd-1138/ps--SOO-60051-00362?ds=SOO-60051-00362-00001&amp;source=SEARCH&amp;sid=6250e0eb050ab5a0&amp;metaData=SnHZRCX7NPLsJ+ExPEFNCzL10t6deH8IJLci3UQaGCFdn+zDqrhLdjITE3plPTXXJpxUsLAohHVwJa3vwtOUsujqrM/mjls6JQDzIHvTluMiB4zoBbkTKkiVxxU6hr74PdxTHKZBV9wukrN4w82/yWp5HoWHuYDNl07Gpt+tmXdtbUEB2KN2y84saGW8FURoFNpMZjfoNazsAekWU+LFfRtd5JisA+krezcArUVhBa3TrWgM/WffSFIKvZxBffSZ&amp;cnc=false&amp;pickupPointCode=PP-3126072&amp;pid1=SOO-60051-00362</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>BLG-70029-08747</t>
+          <t>SOO-60051-00061</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Bliblimart</t>
+          <t>Ibu &amp; Anak</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>MilkLife</t>
+          <t>Sorex</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Clearance - MilkLife UHT Teens Tetra Slim Leaf Coklat 200 ml</t>
+          <t>Sorex Celana Dalam Hamil Motif Katun Lembut Maternity Panty CD 1140</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>3400</v>
+        <v>33320</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/114/MTA-156375987/milklife_milklife_coklat_-_uht_teens_-1_pcs-tetra_slim_leaf_200ml-_full01_s44emxbn.jpg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/MTA-7895759/sorex_sorex_celana_dalam_hamil_motif_katun_lembut_maternity_panty_cd_1140_full02_j2ua28na.jpg</t>
         </is>
       </c>
       <c r="G12" t="n">
@@ -898,151 +897,151 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/clearance-milklife-uht-teens-tetra-slim-leaf-coklat-200-ml/ps--BLG-70029-08747?ds=BLG-70029-08747-00001&amp;source=SEARCH&amp;sid=e132f3cdc0f57c22&amp;metaData=SnHZRCX7NPLsJ+ExPEFNCxf/gWNGqtNIgQNID6HXdHW3VQ2WlzHp9deWrxqynfgSinxpZe4IAZruTtQd1TO7UejqrM/mjls6JQDzIHvTluMiB4zoBbkTKkiVxxU6hr74PdxTHKZBV9wukrN4w82/yWp5HoWHuYDNl07Gpt+tmXeDioWrdqW2jVDexSAU462NTDhvU2dGTHXFRrWe7cayKPgUkBrNSd1kvoEoL27Ax4FfyUcjpfQtbDHqJqFsTE07&amp;cnc=false&amp;pickupPointCode=PP-3527109&amp;pid1=BLG-70029-08747</t>
+          <t>https://www.blibli.com/p/sorex-celana-dalam-hamil-motif-katun-lembut-maternity-panty-cd-1140/ps--SOO-60051-00061?ds=SOO-60051-00061-00001&amp;source=SEARCH&amp;sid=6250e0eb050ab5a0&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC8ZIN0KweYTfTnX/ul7fF5HcTUF9bqmkuAK1tOmfkDJzJpxUsLAohHVwJa3vwtOUsujqrM/mjls6JQDzIHvTluMiB4zoBbkTKkiVxxU6hr74PdxTHKZBV9wukrN4w82/yWp5HoWHuYDNl07Gpt+tmXdtbUEB2KN2y84saGW8FURoFNpMZjfoNazsAekWU+LFfRtd5JisA+krezcArUVhBa3TrWgM/WffSFIKvZxBffSZ&amp;cnc=false&amp;pickupPointCode=PP-3126072&amp;pid1=SOO-60051-00061</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>INS-60055-00082</t>
+          <t>SOO-60051-00574</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Bliblimart</t>
+          <t>Fashion Wanita</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Indomilk</t>
+          <t>Sorex</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Indomilk Cokelat Susu UHT [115 mL]</t>
+          <t>Sorex Celana Dalam Wanita Midi Basic Comfort Chic Adem Lembut Pori-pori CD 1260</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>2600</v>
+        <v>24255</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/MTA-2487622/indomilk_indomilk_cokelat_susu_uht_-115_ml-_full06_eq5jfkm7.jpeg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/MTA-21977111/sorex_sorex_celana_dalam_wanita_midi_basic_comfort_chic_adem_lembut_pori-pori_cd_1260_full02_e9br0e3e.jpg</t>
         </is>
       </c>
       <c r="G13" t="n">
-        <v>4.9</v>
+        <v>5</v>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/indomilk-cokelat-susu-uht-115-ml/ps--INS-60055-00082?ds=INS-60055-00082-00001&amp;source=SEARCH&amp;sid=e132f3cdc0f57c22&amp;metaData=SnHZRCX7NPLsJ+ExPEFNCwR0bgev9saiJ9QpuPsgXPy3VQ2WlzHp9deWrxqynfgSmvX4tmylQG5Pvg43d5IsBbLBaB3tLseqCRU/10V6Qi4m/0gcuiAdTNyGqjLqLXjMVB0Z19F5S3OJm6xVPOQF+fYfYBdOaXUoSWEt7LUZrj8LXARBWNQVKjys2JWHCCuMwzUD/lqOnyWXlD/Zv/Ri6mB7LWEVRbLB5XRbQAog8mSC8ycDqzLGV84f5/SfYa6lUbjBPcmbjFwQFSuE8B89Lvv8mC0e9lRvXyQh+Na3LdQ=&amp;cnc=false&amp;pickupPointCode=PP-3043179&amp;pid1=INS-60055-00082</t>
+          <t>https://www.blibli.com/p/sorex-celana-dalam-wanita-midi-basic-comfort-chic-adem-lembut-pori-pori-cd-1260/ps--SOO-60051-00574?ds=SOO-60051-00574-00001&amp;source=SEARCH&amp;sid=6250e0eb050ab5a0&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC0rd1rndxbAlG8VCZRwhI4agIrFT0SP5wuYJuKSH3/MKJpxUsLAohHVwJa3vwtOUsujqrM/mjls6JQDzIHvTluMiB4zoBbkTKkiVxxU6hr74PdxTHKZBV9wukrN4w82/yWp5HoWHuYDNl07Gpt+tmXfO/kFtVj4porywlY2UWbf6VMqwppbx5Qk9+27gygWs9lk0gjRbIbx9mhzaC4fFgmtfyUcjpfQtbDHqJqFsTE07&amp;cnc=false&amp;pickupPointCode=PP-3126072&amp;pid1=SOO-60051-00574</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>BLD-60037-00015</t>
+          <t>SOO-60051-00042</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Bliblimart</t>
+          <t>Fashion Wanita</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Frisian Flag</t>
+          <t>Sorex</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Frisian Flag Low Fat French Vanilla Susu UHT [225 mL]</t>
+          <t>Sorex CD Basic Maxi Super Light Celana Dalam Wanita Extra Size Jumbo 1249</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>6500</v>
+        <v>37044</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/MTA-2663309/frisian_flag_frisian_flag_low_fat_french_vanilla_susu_uht_-225_ml-_full06_hevsxxnz.jpeg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/MTA-7886901/sorex_sorex_cd_basic_maxi_super_light_celana_dalam_wanita_extra_size_jumbo_1249_full02_g40b4t61.jpg</t>
         </is>
       </c>
       <c r="G14" t="n">
-        <v>4.9</v>
+        <v>5</v>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/frisian-flag-low-fat-french-vanilla-susu-uht-225-ml/ps--BLD-60037-00015?ds=BLD-60037-00015-00001&amp;source=SEARCH&amp;sid=e132f3cdc0f57c22&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC1R4AsY2zbEuPf0mEleNTFm3VQ2WlzHp9deWrxqynfgSqYpB9c1FKqQoXgFDUcveu1X6YqNL/N38iJlYkQlI2HD9cnB7A9Br96VNOoae/H1+BSFd02BuHmZWh0L7R6dhksB+tPNv9ITp+8ttAFmGt53nU4Dp3uhlwixflscAf8XVNd9Qdrb3QWYxenklePSJm24qiwzrO6nWnHsxgeryKb/ltUNk96VTdqdjG4caO5Q1wCaCWmOutPc0eIowrS/xtbSlp5iaPRa3auHKDapyNXA=&amp;cnc=false&amp;pickupPointCode=PP-3098866&amp;pid1=BLD-60037-00015</t>
+          <t>https://www.blibli.com/p/sorex-cd-basic-maxi-super-light-celana-dalam-wanita-extra-size-jumbo-1249/ps--SOO-60051-00042?ds=SOO-60051-00042-00001&amp;source=SEARCH&amp;sid=6250e0eb050ab5a0&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC/uzJZ4qiKCUsLXY6fa2mZsQHMYoO9/9ygcijfF65PUOJpxUsLAohHVwJa3vwtOUsujqrM/mjls6JQDzIHvTluMiB4zoBbkTKkiVxxU6hr74PdxTHKZBV9wukrN4w82/yWp5HoWHuYDNl07Gpt+tmXfO/kFtVj4porywlY2UWbf6VMqwppbx5Qk9+27gygWs9lk0gjRbIbx9mhzaC4fFgmtfyUcjpfQtbDHqJqFsTE07&amp;cnc=false&amp;pickupPointCode=PP-3126072&amp;pid1=SOO-60051-00042</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>BLB-60045-00045</t>
+          <t>SOO-60051-00427</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Bliblimart</t>
+          <t>Fashion Wanita</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Huki</t>
+          <t>Sorex</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Huki Botol Susu PP Baby Animal Orthodontic - Random [240 mL]</t>
+          <t>Sorex Young Miniset Anak Remaja Step 1 Freesize Tanpa Kawat Pita Mungil Miniset Y 1103</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>20000</v>
+        <v>30870</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/MTA-73185224/huki_huki_botol_susu_pp_baby_animal_orthodontic_-_random_-240_ml-_full11_r1paei7p.jpeg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/MTA-11560139/sorex_sorex_young_miniset_anak_remaja_step_1_freesize_tanpa_kawat_pita_mungil_miniset_y_1103_full01_m3k9nvkz.jpg</t>
         </is>
       </c>
       <c r="G15" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/huki-botol-susu-pp-baby-animal-orthodontic-random-240-ml/ps--BLB-60045-00045?ds=BLB-60045-00045-00001&amp;source=SEARCH&amp;sid=e132f3cdc0f57c22&amp;metaData=SnHZRCX7NPLsJ+ExPEFNCxzohPZzaxyiJv5ug5c6gt2T2r7fOYNS0fn24lYkspaB1VERKv4BBdBPFnhK63tfIejqrM/mjls6JQDzIHvTluMiB4zoBbkTKkiVxxU6hr74Axnpn5uUjYeSavSjwxFyeVCwq7vqJ42QPgBkY5BSoK0QGdv2rIvkdBs0xXb/7ciFIPAX4/+UO/JPduNR55DLnWF3+BJGgihk+Yk70VLJAfg3K1aYZAD0duLDi004fByjgbik78uUwj2VNiTmH/F8XDYolYQZzFnWMJuVJS4GZD0Gn6h/X6Ctr/9KCaAg44n9j+7L3Wik+RTA5iNCdr8f2A==&amp;cnc=false&amp;pickupPointCode=PP-3165865&amp;pid1=BLB-60045-00045</t>
+          <t>https://www.blibli.com/p/sorex-young-miniset-anak-remaja-step-1-freesize-tanpa-kawat-pita-mungil-miniset-y-1103/ps--SOO-60051-00427?ds=SOO-60051-00427-00002&amp;source=SEARCH&amp;sid=6250e0eb050ab5a0&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC+G4LZi2pi3YNLiDQiX+7EOacJbj2cXRya+Q0SCnBRoFJpxUsLAohHVwJa3vwtOUsujqrM/mjls6JQDzIHvTluMiB4zoBbkTKkiVxxU6hr74PdxTHKZBV9wukrN4w82/yWp5HoWHuYDNl07Gpt+tmXfO/kFtVj4porywlY2UWbf6VMqwppbx5Qk9+27gygWs9sZi4HFMNt1hNudy6hVQGo9fyUcjpfQtbDHqJqFsTE07&amp;cnc=false&amp;pickupPointCode=PP-3126072&amp;pid1=SOO-60051-00427</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>INS-60055-00209</t>
+          <t>SOO-60051-00274</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Bliblimart</t>
+          <t>Fashion Wanita</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Indomilk</t>
+          <t>Sorex</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Indomilk Full Cream Plain Susu UHT 115 mL</t>
+          <t>Sorex CD Basic Midi Katun Mix 1179</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>2600</v>
+        <v>26460</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/MTA-3950259/indomilk_indomilk_full_cream_plain_susu_uht_-115_ml-_full04_bdnw7yzd.jpeg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium//catalog-image/MTA-8385514/sorex_sorex_cd_basic_midi_katun_mix_1179_full01_f8nmyoy6.jpg</t>
         </is>
       </c>
       <c r="G16" t="n">
@@ -1050,151 +1049,151 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/indomilk-full-cream-plain-susu-uht-115-ml/ps--INS-60055-00209?ds=INS-60055-00209-00001&amp;source=SEARCH&amp;sid=e132f3cdc0f57c22&amp;metaData=SnHZRCX7NPLsJ+ExPEFNCwR0bgev9saiJ9QpuPsgXPy3VQ2WlzHp9deWrxqynfgSwwPzIYAGMqXEEIH06KVrrZbKIFVX5lKVfE28/P1rwwdP0HfjxNkfgWHG5INuEdtbni/RfXtjO+mLEBi1JvU4oOf9OamnFrvil6IltQoJVV7gVFzNUgTsVxnEJaAi206QylkZHer+F/DmhPZJvYm9VGEkj8u/5h4Kyn3dAqlMr+Xi4YSCsa/SsFeuwwC/3BZ9vavFjQW+Hi0U1g5VsfADeL+0KlWZP9TCw01G7E1sRkY=&amp;cnc=false&amp;pickupPointCode=PP-3043179&amp;pid1=INS-60055-00209</t>
+          <t>https://www.blibli.com/p/sorex-cd-basic-midi-katun-mix-1179/ps--SOO-60051-00274?ds=SOO-60051-00274-00001&amp;source=SEARCH&amp;sid=6250e0eb050ab5a0&amp;metaData=SnHZRCX7NPLsJ+ExPEFNCwR0bgev9saiJ9QpuPsgXPzIOwJf81+FzoG8lPia/LMVJpxUsLAohHVwJa3vwtOUsujqrM/mjls6JQDzIHvTluMiB4zoBbkTKkiVxxU6hr74PdxTHKZBV9wukrN4w82/yWp5HoWHuYDNl07Gpt+tmXfO/kFtVj4porywlY2UWbf6VMqwppbx5Qk9+27gygWs9lk0gjRbIbx9mhzaC4fFgmtfyUcjpfQtbDHqJqFsTE07&amp;cnc=false&amp;pickupPointCode=PP-3126072&amp;pid1=SOO-60051-00274</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>MEG-60041-00002</t>
+          <t>SOO-60051-00013</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Bliblimart</t>
+          <t>Fashion Wanita</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Greenfields</t>
+          <t>Sorex</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Medan - Greenfields UHT Fullcream Susu [1000 mL]</t>
+          <t>Sorex Basic Super Soft 1255 Celana Dalam Wanita - Multicolor</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>22000</v>
+        <v>22785</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium//103/MTA-12991980/greenfields_medan_-_greenfields_uht_fullcream_susu_-1000_ml-_full01_jvqzwe8i.jpg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/MTA-7709258/sorex_sorex_basic_super_soft_1255_celana_dalam_wanita_-__multicolor_full01_t4dg2gm7.jpg</t>
         </is>
       </c>
       <c r="G17" t="n">
-        <v>5</v>
+        <v>4.9</v>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/medan-greenfields-uht-fullcream-susu-1000-ml/ps--MEG-60041-00002?ds=MEG-60041-00002-00001&amp;source=SEARCH&amp;sid=e132f3cdc0f57c22&amp;metaData=SnHZRCX7NPLsJ+ExPEFNCzcTLm2yJwfE+vqixRWQ5q+T2r7fOYNS0fn24lYkspaBRE8oGmciCQ8xRUBc/m4bnVX6YqNL/N38iJlYkQlI2HD9cnB7A9Br96VNOoae/H1+BSFd02BuHmZWh0L7R6dhksB+tPNv9ITp+8ttAFmGt53nU4Dp3uhlwixflscAf8XVNd9Qdrb3QWYxenklePSJm24qiwzrO6nWnHsxgeryKb/ltUNk96VTdqdjG4caO5Q1EKRLV3Hac94zMayA3P2OPUaUYMkdIQYfNaoycLYqosk=&amp;cnc=false&amp;pickupPointCode=PP-3525989&amp;pid1=MEG-60041-00002</t>
+          <t>https://www.blibli.com/p/sorex-basic-super-soft-1255-celana-dalam-wanita-multicolor/ps--SOO-60051-00013?ds=SOO-60051-00013-00001&amp;source=SEARCH&amp;sid=6250e0eb050ab5a0&amp;metaData=SnHZRCX7NPLsJ+ExPEFNCzcTLm2yJwfE+vqixRWQ5q8xmBGsZhEvfPzU+A1f7vo+JpxUsLAohHVwJa3vwtOUsujqrM/mjls6JQDzIHvTluMiB4zoBbkTKkiVxxU6hr74PdxTHKZBV9wukrN4w82/yWp5HoWHuYDNl07Gpt+tmXfO/kFtVj4porywlY2UWbf6VMqwppbx5Qk9+27gygWs9lk0gjRbIbx9mhzaC4fFgmtfyUcjpfQtbDHqJqFsTE07&amp;cnc=false&amp;pickupPointCode=PP-3126072&amp;pid1=SOO-60051-00013</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>BLG-70029-09374</t>
+          <t>SOO-60051-00175</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Bliblimart</t>
+          <t>Fashion Wanita</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Greenfields</t>
+          <t>Sorex</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Clearance - Greenfields UHT Strawberry Minuman Susu [200 mL]</t>
+          <t>Sorex Bra Extra Comfort Busa Sedang Kawat Kait 3 Setara Cup B BH 3262</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>4500</v>
+        <v>55125</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/112/MTA-166078875/greenfields_greenfields_uht_strawberry_minuman_susu_-200_ml-_full04_zx2y0rx.jpg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/MTA-7994480/sorex_sorex_bra_extra_comfort_busa_sedang_kawat_kait_3_setara_cup_b_bh_3262_full03_bpk5yj9s.jpeg</t>
         </is>
       </c>
       <c r="G18" t="n">
-        <v>0</v>
+        <v>4.9</v>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/clearance-greenfields-uht-strawberry-minuman-susu-200-ml/ps--BLG-70029-09374?ds=BLG-70029-09374-00001&amp;source=SEARCH&amp;sid=e132f3cdc0f57c22&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC3dMFCi0+0h2Q7yp/RTOlfe3VQ2WlzHp9deWrxqynfgSXGwa1ZG0g99cMvoGAXvCEQSIEitAq/1WrQRC4F6yTsDlurVX7NrCB6MjjGzbuCOvw664EUevDp9eL6Ws+MzDLl0wE3gvXVJ3bf5C00nZu7gtJcVjQwK0YoIlqayUmPpM/rE1RDVspHjbMfc0GxnrrMcXor3TIJbXyW2l+BVCrAErvl0KBXJKdKcWce8lHB5y&amp;cnc=false&amp;pickupPointCode=PP-3526957&amp;pid1=BLG-70029-09374</t>
+          <t>https://www.blibli.com/p/sorex-bra-extra-comfort-busa-sedang-kawat-kait-3-setara-cup-b-bh-3262/ps--SOO-60051-00175?ds=SOO-60051-00175-00014&amp;source=SEARCH&amp;sid=6250e0eb050ab5a0&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC/HCzbecjA7sTaIoP2qZn9eYLh/3g9xopt0s/MYhR5faJpxUsLAohHVwJa3vwtOUsujqrM/mjls6JQDzIHvTluMiB4zoBbkTKkiVxxU6hr74PdxTHKZBV9wukrN4w82/yWp5HoWHuYDNl07Gpt+tmXfO/kFtVj4porywlY2UWbf6VMqwppbx5Qk9+27gygWs9sZi4HFMNt1hNudy6hVQGo9fyUcjpfQtbDHqJqFsTE07&amp;cnc=false&amp;pickupPointCode=PP-3126072&amp;pid1=SOO-60051-00175</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>LMS-60022-00338</t>
+          <t>SOO-60051-00295</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Kesehatan &amp; Kecantikan</t>
+          <t>Fashion Wanita</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>L-Men</t>
+          <t>Sorex</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Gym Starter Pack: L-Men Platinum Strawberry 800gr &amp; L-Men Isopower Creatine Stargizing 30 Sachet</t>
+          <t>Sorex Celana Dalam Wanita Basic Mini Super Soft Lembut Nyaman Dipakai CD 1257</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>365600</v>
+        <v>19992</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/101/MTA-155674721/l-men_gym_starter_pack_-_l-men_platinum_strawberry_800gr_-_l-men_isopower_creatine_stargizing_30_sachet_full07_cyixkg26.jpg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/MTA-18327672/sorex_sorex_celana_dalam_wanita_basic_mini_super_soft_lembut_nyaman_dipakai_cd_1257_full02_cqx8djmw.jpg</t>
         </is>
       </c>
       <c r="G19" t="n">
-        <v>4.8</v>
+        <v>4.9</v>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/gym-starter-pack-l-men-platinum-strawberry-800gr-l-men-isopower-creatine-stargizing-30-sachet/ps--LMS-60022-00338?ds=LMS-60022-00338-00001&amp;source=SEARCH&amp;sid=e132f3cdc0f57c22&amp;metaData=SnHZRCX7NPLsJ+ExPEFNCzL10t6deH8IJLci3UQaGCFiR8g8McAxsDs2Q1fRxwov+jueud2FI92c8YAiS/TajVX6YqNL/N38iJlYkQlI2HD9cnB7A9Br96VNOoae/H1+UvM5rYQ2b7sWjAIjInNGf9EzhaeZDpTR/fAyKgGVxs4Jb3XHBYDwr/rpsPgJumBr9pLkKEidQpCVEgJe2GcmIgb3zNcKWRrHOP3cRGuonLQ=&amp;cnc=false&amp;pickupPointCode=PP-3495578&amp;pid1=LMS-60022-00338</t>
+          <t>https://www.blibli.com/p/sorex-celana-dalam-wanita-basic-mini-super-soft-lembut-nyaman-dipakai-cd-1257/ps--SOO-60051-00295?ds=SOO-60051-00295-00001&amp;source=SEARCH&amp;sid=6250e0eb050ab5a0&amp;metaData=SnHZRCX7NPLsJ+ExPEFNCyyDdutSjnAKjW/qtRSWe1JSivqeb4HprTDVqcGV3PQCJpxUsLAohHVwJa3vwtOUsujqrM/mjls6JQDzIHvTluMiB4zoBbkTKkiVxxU6hr74PdxTHKZBV9wukrN4w82/yWp5HoWHuYDNl07Gpt+tmXfO/kFtVj4porywlY2UWbf6VMqwppbx5Qk9+27gygWs9lk0gjRbIbx9mhzaC4fFgmtfyUcjpfQtbDHqJqFsTE07&amp;cnc=false&amp;pickupPointCode=PP-3126072&amp;pid1=SOO-60051-00295</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>BLD-60037-00187</t>
+          <t>SOO-60051-00004</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Bliblimart</t>
+          <t>Fashion Wanita</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Frisian Flag</t>
+          <t>Sorex</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Frisian Flag Purefarm Full Cream Susu UHT 946 mL</t>
+          <t>Sorex Celana Dalam Wanita Basic Midi Soft &amp; Comfort CD 1228 Katun Mix Adem</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>18600</v>
+        <v>26754</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium//105/MTA-39783372/frisian_flag_frisian_flag_purefarm_full_cream_susu_uht_-946_ml-_full01_oum3b4t1.jpg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/MTA-7700289/sorex_sorex_celana_dalam_wanita_basic_midi_soft_-_comfort_cd_1228_katun_mix_adem_full02_nnq90z7s.jpg</t>
         </is>
       </c>
       <c r="G20" t="n">
@@ -1202,151 +1201,151 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/frisian-flag-purefarm-full-cream-susu-uht-946-ml/ps--BLD-60037-00187?ds=BLD-60037-00187-00001&amp;source=SEARCH&amp;sid=e132f3cdc0f57c22&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC83UCraFZ0P7NET872xC0whnh6wQ6PEr8y5kW/jpBoqa4jSPc0dx0L2nwfZhTbnE/rLBaB3tLseqCRU/10V6Qi4m/0gcuiAdTNyGqjLqLXjMVB0Z19F5S3OJm6xVPOQF+fYfYBdOaXUoSWEt7LUZrj8LXARBWNQVKjys2JWHCCuMwzUD/lqOnyWXlD/Zv/Ri6mB7LWEVRbLB5XRbQAog8mSC8ycDqzLGV84f5/SfYa6lKQVM5o2dZyqdFHEDP2wFPLs3aCsEU1E4Ung/d448uEI=&amp;cnc=false&amp;pickupPointCode=PP-3098866&amp;pid1=BLD-60037-00187</t>
+          <t>https://www.blibli.com/p/sorex-celana-dalam-wanita-basic-midi-soft-comfort-cd-1228-katun-mix-adem/ps--SOO-60051-00004?ds=SOO-60051-00004-00001&amp;source=SEARCH&amp;sid=6250e0eb050ab5a0&amp;metaData=SnHZRCX7NPLsJ+ExPEFNCwR0bgev9saiJ9QpuPsgXPy/kEEC5/YmxIZLZ3qqgiVyJpxUsLAohHVwJa3vwtOUsujqrM/mjls6JQDzIHvTluMiB4zoBbkTKkiVxxU6hr74PdxTHKZBV9wukrN4w82/yWp5HoWHuYDNl07Gpt+tmXfO/kFtVj4porywlY2UWbf6VMqwppbx5Qk9+27gygWs9lk0gjRbIbx9mhzaC4fFgmtfyUcjpfQtbDHqJqFsTE07&amp;cnc=false&amp;pickupPointCode=PP-3126072&amp;pid1=SOO-60051-00004</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>NUT-60023-00092</t>
+          <t>SOO-60051-00010</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Bliblimart</t>
+          <t>Fashion Wanita</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Hilo</t>
+          <t>Sorex</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>HiLo Gold Susu Tinggi Kalsium Rendah Lemak Chocolate [500 g ]</t>
+          <t>Sorex Cd Basic Bahan Super Soft 1251 Celana dalam Wanita</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>85100</v>
+        <v>23667</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium//catalog-image/MTA-1989097/hilo_hilo_gold_susu_tinggi_kalsium_rendah_lemak_chocolate_-500_g_-__full01_u6yh6qqj.jpg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/MTA-7708515/sorex_sorex_cd_basic_bahan_super_soft_1251_celana_dalam_wanita_full03_t1r1rwvf.jpg</t>
         </is>
       </c>
       <c r="G21" t="n">
-        <v>4.8</v>
+        <v>4.9</v>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/hilo-gold-susu-tinggi-kalsium-rendah-lemak-chocolate-500-g/ps--NUT-60023-00092?ds=NUT-60023-00092-00001&amp;source=SEARCH&amp;sid=e132f3cdc0f57c22&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC4jqhVUYBGnRHB2dDFMPniwmbE/LLJy7W3VwRB8pUx8xHDgDXETBrL/3N9/aupe551X6YqNL/N38iJlYkQlI2HD9cnB7A9Br96VNOoae/H1+BSFd02BuHmZWh0L7R6dhksB+tPNv9ITp+8ttAFmGt537CBlnldB1rbcOtYX5GcZpQng5UHb8zzKVhV9+Dw3QAKK1M+GoNdrP6ar75oze0NMAEuBGo/nw/sRN6/giFL7Lqsa6b+xuvla6E9/DzyQNRNsqkUK+CvLdAAXsjpTQQrPp5hlxWpxAbIaUqGBcGWhfBsu7/DiHhN3lQH6lziPodV/JRyOl9C1sMeomoWxMTTs=&amp;cnc=false&amp;pickupPointCode=PP-3495802&amp;pid1=NUT-60023-00092</t>
+          <t>https://www.blibli.com/p/sorex-cd-basic-bahan-super-soft-1251-celana-dalam-wanita/ps--SOO-60051-00010?ds=SOO-60051-00010-00001&amp;source=SEARCH&amp;sid=6250e0eb050ab5a0&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC6tKRkdMY5WBMzsytzOk73OhY4+eXFWJ8a6ITW30cbFkJpxUsLAohHVwJa3vwtOUsujqrM/mjls6JQDzIHvTluMiB4zoBbkTKkiVxxU6hr74PdxTHKZBV9wukrN4w82/yWp5HoWHuYDNl07Gpt+tmXfO/kFtVj4porywlY2UWbf6VMqwppbx5Qk9+27gygWs9lk0gjRbIbx9mhzaC4fFgmtfyUcjpfQtbDHqJqFsTE07&amp;cnc=false&amp;pickupPointCode=PP-3126072&amp;pid1=SOO-60051-00010</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>BLD-60037-00394</t>
+          <t>SOO-60051-00258</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Bliblimart</t>
+          <t>Fashion Wanita</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Frisian Flag</t>
+          <t>Sorex</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Frisian Flag Nutribrain Omega Susu Uht Chocolate [115 mL]</t>
+          <t>Sorex CD 1230 Basic Katun WARNA</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>2800</v>
+        <v>21900</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/106/MTA-156459093/frisian_flag_frisian_flag_nutribrain_omega_susu_uht_chocolate_-115_ml-_full01_xvbdwy0.jpg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/MTA-8247465/sorex_sorex_cd_1230_basic_katun_warna_full02_dcmpebfb.jpg</t>
         </is>
       </c>
       <c r="G22" t="n">
-        <v>4.3</v>
+        <v>4.8</v>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/frisian-flag-nutribrain-omega-susu-uht-chocolate-115-ml/ps--BLD-60037-00394?ds=BLD-60037-00394-00001&amp;source=SEARCH&amp;sid=e132f3cdc0f57c22&amp;metaData=SnHZRCX7NPLsJ+ExPEFNCxhotWbalOJK1bAKb4JrdH63VQ2WlzHp9deWrxqynfgSO1H2k8MmzxAQeKiypkJuPlesavfRnEsmWNUn9y9IGTPNbQv3e9jt8aL3d1v2xu9D3zP/3jXSVAsNO6CVkKiBbHhwvx3ifXg1BsOX37zBUHIopPuOXO3ZPFXx1Ozq+hxbn0t+Z31N/tG70rzxf062H4Scv7qvXlsLo00FBKrsBre0XBPM8Ib69hRyb0y0TLR/&amp;cnc=false&amp;pickupPointCode=PP-3098866&amp;pid1=BLD-60037-00394</t>
+          <t>https://www.blibli.com/p/sorex-cd-1230-basic-katun-warna/ps--SOO-60051-00258?ds=SOO-60051-00258-00002&amp;source=SEARCH&amp;sid=6250e0eb050ab5a0&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC+OZu5yoAs+ZwOIEQgV7goKIIGmm33viDj/+hYQaGlpdxFbcOmnv9bSync5a5kF4+lX6YqNL/N38iJlYkQlI2HD9cnB7A9Br96VNOoae/H1+BSFd02BuHmZWh0L7R6dhksB+tPNv9ITp+8ttAFmGt52x/tp/x6eG5ji3JFb8hWgxWH525tg6GPPr8PhUtYVf+Yhq+WjxonGWxb+TvCwQTPaDEC3cLXX0wtGQFaK7Z8yP&amp;cnc=false&amp;pickupPointCode=PP-3126072&amp;pid1=SOO-60051-00258</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>TEJ-70084-00247</t>
+          <t>SOO-60051-00079</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Bliblimart</t>
+          <t>Fashion Wanita</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Vidoran</t>
+          <t>Sorex</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>SMG/JOG/SOLO - Vidoran Xmart 3+ Madu Susu Formula 700 g</t>
+          <t>Sorex Bra Tanpa Kawat Super Soft Busa Sedang Setara Cup B 17238 BH Harian Simple Polos</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>51000</v>
+        <v>37240</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium//catalog-image/105/MTA-117803579/vidoran_smg-jog-solo_-_vidoran_xmart_3-_madu_susu_formula_700_g_full01_r0wttkjc.jpg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/MTA-18240855/sorex_sorex_bra_tanpa_kawat_super_soft_busa_sedang_setara_cup_b_17238_bh_harian_simple_polos_full02_t2k386dq.jpg</t>
         </is>
       </c>
       <c r="G23" t="n">
-        <v>5</v>
+        <v>4.8</v>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/smg-jog-solo-vidoran-xmart-3-madu-susu-formula-700-g/ps--TEJ-70084-00247?ds=TEJ-70084-00247-00001&amp;source=SEARCH&amp;sid=e132f3cdc0f57c22&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC/zjMYmgLdOqahjgDqbPvauT2r7fOYNS0fn24lYkspaB77cR3O357HYtLFjlWroZqeWk7L/WjZW4V3T1+QzDEpiZTqX+08YMFPt67oXduO/veDye5g4cJG51p5fjAlqNKr3Qa6Aw9nJN8ZS3vPJl9087KBj1oW91VVdgmsyeMwxA1ZBkU0NcX4uiXe/YPsHDKlaVTxNVKJtaXT+VmH890/Z50OgtOryTnW5cLdVxnS6XKKZohZrEj62hpwjPOPOeKefuNxBe1fmWzvRIc0H9ev6iqEzTFzwXsOb0sxDit2/B&amp;cnc=false&amp;pickupPointCode=PP-3528924&amp;pid1=TEJ-70084-00247</t>
+          <t>https://www.blibli.com/p/sorex-bra-tanpa-kawat-super-soft-busa-sedang-setara-cup-b-17238-bh-harian-simple-polos/ps--SOO-60051-00079?ds=SOO-60051-00079-00011&amp;source=SEARCH&amp;sid=6250e0eb050ab5a0&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC/uzJZ4qiKCUsLXY6fa2mZukJoT8NV2nfifVvZEWfKxkJpxUsLAohHVwJa3vwtOUsujqrM/mjls6JQDzIHvTluMiB4zoBbkTKkiVxxU6hr74PdxTHKZBV9wukrN4w82/yWp5HoWHuYDNl07Gpt+tmXfO/kFtVj4porywlY2UWbf6VMqwppbx5Qk9+27gygWs9sZi4HFMNt1hNudy6hVQGo9fyUcjpfQtbDHqJqFsTE07&amp;cnc=false&amp;pickupPointCode=PP-3126072&amp;pid1=SOO-60051-00079</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>LOI-36586-01266</t>
+          <t>SOO-60051-00467</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Home &amp; Living</t>
+          <t>Fashion Wanita</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>LocknLock</t>
+          <t>Sorex</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>LocknLock One Touch Clip Tumbler 550ML - LHC3249</t>
+          <t>Sorex Bra Tanpa Kawat Busa Kait 3 Setara Cup B Bra Harian Casual Comfort BH 65001</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>181000</v>
+        <v>52920</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium//92/MTA-20657304/locknlock_locknlock_one_touch_clip_tumbler_550ml_-_lhc3249_full02_m6cxf9vm.jpg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/MTA-12228968/sorex_sorex_bra_tanpa_kawat_busa_kait_3_setara_cup_b_bra_harian_casual_comfort_bh_65001_full02_br99daxr.jpeg</t>
         </is>
       </c>
       <c r="G24" t="n">
@@ -1354,166 +1353,166 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/locknlock-one-touch-clip-tumbler-550ml-lhc3249/ps--LOI-36586-01266?ds=LOI-36586-01266-00003&amp;source=SEARCH&amp;sid=e132f3cdc0f57c22&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC83UCraFZ0P7NET872xC0wh5LPrP51EEqEiLRjy53GKhWuEYT17AdwWUL3SlGLwkEuWk7L/WjZW4V3T1+QzDEpiZTqX+08YMFPt67oXduO/veDye5g4cJG51p5fjAlqNKhFRUDY7LArWqkV+AxOUq3VZ3JdAFGVbl5JSlY27jovfankehYe5gM2XTsam362ZdwNgGo3aFoz5nxXptjUARwtq+xgJseBgpvTygmxlBheFKxOnOrNxJdcBnW3+29tfvE+Y4uvtuoyjPRzfflxja6A=&amp;cnc=false&amp;pickupPointCode=PP-3009820&amp;pid1=LOI-36586-01266</t>
+          <t>https://www.blibli.com/p/sorex-bra-tanpa-kawat-busa-kait-3-setara-cup-b-bra-harian-casual-comfort-bh-65001/ps--SOO-60051-00467?ds=SOO-60051-00467-00002&amp;source=SEARCH&amp;sid=6250e0eb050ab5a0&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC+iQM9MJM8LcOV1edc2sOTJmjateuiD2bQM1xoGRlYR/5LByD0g7hF2jEY9iKzbkb1esavfRnEsmWNUn9y9IGTPNbQv3e9jt8aL3d1v2xu9D3zP/3jXSVAsNO6CVkKiBbHhwvx3ifXg1BsOX37zBUHLC06X8BZfWbuoyV1i+FIvCFi5ZGHXfeZdV+lqHHsOV+GmfylN82DRKT97iLHHfPs20XBPM8Ib69hRyb0y0TLR/&amp;cnc=false&amp;pickupPointCode=PP-3126072&amp;pid1=SOO-60051-00467</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>MIU-60036-00016</t>
+          <t>SOO-60051-00125</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Bliblimart</t>
+          <t>Fashion Wanita</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>MilkLife</t>
+          <t>Sorex</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>MilkLife Classic Choco UHT Kids Tetra Slim Leaf 115mL</t>
+          <t>Sorex Bra Extra Comfort Busa Tanpa Kawat Kait 2 Setara Cup B BH 9850</t>
         </is>
       </c>
       <c r="E25" t="n">
-        <v>2900</v>
+        <v>55125</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium//catalog-image/MTA-23409426/milklife_milklife_classic_cokelat_-_uht_kids_-1_pcs-_tetra_slim_leaf_115ml-_full01_retjowk1.jpeg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium//catalog-image/MTA-18247352/sorex_sorex_bra_extra_comfort_busa_tanpa_kawat_kait_2_setara_cup_b_bh_9850_full01_n9w2qvqq.jpg</t>
         </is>
       </c>
       <c r="G25" t="n">
-        <v>4.9</v>
+        <v>4.8</v>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/milklife-classic-choco-uht-kids-tetra-slim-leaf-115ml/ps--MIU-60036-00016?ds=MIU-60036-00016-00001&amp;source=SEARCH&amp;sid=e132f3cdc0f57c22&amp;metaData=SnHZRCX7NPLsJ+ExPEFNCwIcYjJhUkfzuki5iW9SKA+3VQ2WlzHp9deWrxqynfgSLfww3oC3M3hWNmwsypEKmJbKIFVX5lKVfE28/P1rwwdP0HfjxNkfgWHG5INuEdtbni/RfXtjO+mLEBi1JvU4oOf9OamnFrvil6IltQoJVV7gVFzNUgTsVxnEJaAi206QylkZHer+F/DmhPZJvYm9VGEkj8u/5h4Kyn3dAqlMr+Xi4YSCsa/SsFeuwwC/3BZ9vavFjQW+Hi0U1g5VsfADeL+0KlWZP9TCw01G7E1sRkY=&amp;cnc=false&amp;pickupPointCode=PP-3243836&amp;pid1=MIU-60036-00016</t>
+          <t>https://www.blibli.com/p/sorex-bra-extra-comfort-busa-tanpa-kawat-kait-2-setara-cup-b-bh-9850/ps--SOO-60051-00125?ds=SOO-60051-00125-00009&amp;source=SEARCH&amp;sid=6250e0eb050ab5a0&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC/HCzbecjA7sTaIoP2qZn9eYLh/3g9xopt0s/MYhR5faJpxUsLAohHVwJa3vwtOUsujqrM/mjls6JQDzIHvTluMiB4zoBbkTKkiVxxU6hr74PdxTHKZBV9wukrN4w82/yWp5HoWHuYDNl07Gpt+tmXfO/kFtVj4porywlY2UWbf6VMqwppbx5Qk9+27gygWs9sZi4HFMNt1hNudy6hVQGo9fyUcjpfQtbDHqJqFsTE07&amp;cnc=false&amp;pickupPointCode=PP-3126072&amp;pid1=SOO-60051-00125</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>BLG-70029-00111</t>
+          <t>SOO-60051-00090</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Bliblimart</t>
+          <t>Fashion Wanita</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>MilkLife</t>
+          <t>Sorex</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>MilkLife Stroberi Milkshake Susu UHT Kids [1 pcs/ Tetra Slim Leaf 125]</t>
+          <t>Bra Sorex Tanpa Kawat Busa Sedang Cup Setara Cup B Casual Comfort 65003 Basic</t>
         </is>
       </c>
       <c r="E26" t="n">
-        <v>2900</v>
+        <v>54880</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium//88/MTA-42240435/milklife_milklife_uht_strawberry_milkshake_-125_ml-_full01_e79qur2b.jpg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/MTA-18240575/sorex_bra_sorex_tanpa_kawat_busa_sedang_cup_setara_cup_b_casual_comfort_65003_basic_full02_jqezgsad.jpeg</t>
         </is>
       </c>
       <c r="G26" t="n">
-        <v>5</v>
+        <v>4.8</v>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/milklife-stroberi-milkshake-susu-uht-kids-1-pcs-tetra-slim-leaf-125/ps--BLG-70029-00111?ds=BLG-70029-00111-00001&amp;source=SEARCH&amp;sid=e132f3cdc0f57c22&amp;metaData=SnHZRCX7NPLsJ+ExPEFNCwIcYjJhUkfzuki5iW9SKA+3VQ2WlzHp9deWrxqynfgSeaqSka2vuLZuhqd7pSHzIFesavfRnEsmWNUn9y9IGTPNbQv3e9jt8aL3d1v2xu9D3zP/3jXSVAsNO6CVkKiBbHhwvx3ifXg1BsOX37zBUHIopPuOXO3ZPFXx1Ozq+hxbn0t+Z31N/tG70rzxf062H4Scv7qvXlsLo00FBKrsBreaNnpcWSO8NdJ4uY4f8r+nzG9GyVyKk94kpU7EioE4b7g1igoiRuGLR3dNi3eSKPU=&amp;cnc=false&amp;pickupPointCode=PP-3527470&amp;pid1=BLG-70029-00111</t>
+          <t>https://www.blibli.com/p/bra-sorex-tanpa-kawat-busa-sedang-cup-setara-cup-b-casual-comfort-65003-basic/ps--SOO-60051-00090?ds=SOO-60051-00090-00005&amp;source=SEARCH&amp;sid=6250e0eb050ab5a0&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC9AkQpPvNielOwWvOvbJVJWc8Qg5cJ1du71Plk4CIHX7JpxUsLAohHVwJa3vwtOUsujqrM/mjls6JQDzIHvTluMiB4zoBbkTKkiVxxU6hr74PdxTHKZBV9wukrN4w82/yWp5HoWHuYDNl07Gpt+tmXfO/kFtVj4porywlY2UWbf6VMqwppbx5Qk9+27gygWs9sZi4HFMNt1hNudy6hVQGo9fyUcjpfQtbDHqJqFsTE07&amp;cnc=false&amp;pickupPointCode=PP-3126072&amp;pid1=SOO-60051-00090</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>MIU-60036-00069</t>
+          <t>SOO-60051-00098</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Bliblimart</t>
+          <t>Ibu &amp; Anak</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>MilkLife</t>
+          <t>Sorex</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>MilkLife UHT Lactose Free [200 mL]</t>
+          <t>Sorex Bra Menyusui Busa Tipis Cup B Motif Bunga Cantik 8110 Kait 3</t>
         </is>
       </c>
       <c r="E27" t="n">
-        <v>4400</v>
+        <v>45570</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium//catalog-image/MTA-41391161/milklife_milklife_uht_lactose_free_-200_ml-_full01_ql8ywk8z.jpg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium//catalog-image/MTA-7932623/sorex_sorex_bh_menyusui_busa_tipis_motif_bunga_cantik_8110_kait_3_full02_rbxn2xa8.jpg</t>
         </is>
       </c>
       <c r="G27" t="n">
-        <v>4.9</v>
+        <v>4.8</v>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/milklife-uht-lactose-free-200-ml/ps--MIU-60036-00069?ds=MIU-60036-00069-00001&amp;source=SEARCH&amp;sid=e132f3cdc0f57c22&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC/yWWkfvbmGmkfSwUzmXNKO3VQ2WlzHp9deWrxqynfgSFhQAZzCJLQLk+plWA2r1mlX6YqNL/N38iJlYkQlI2HD9cnB7A9Br96VNOoae/H1+BSFd02BuHmZWh0L7R6dhksB+tPNv9ITp+8ttAFmGt53nU4Dp3uhlwixflscAf8XVNd9Qdrb3QWYxenklePSJm24qiwzrO6nWnHsxgeryKb/ltUNk96VTdqdjG4caO5Q1wCaCWmOutPc0eIowrS/xtbSlp5iaPRa3auHKDapyNXA=&amp;cnc=false&amp;pickupPointCode=PP-3243836&amp;pid1=MIU-60036-00069</t>
+          <t>https://www.blibli.com/p/sorex-bra-menyusui-busa-tipis-cup-b-motif-bunga-cantik-8110-kait-3/ps--SOO-60051-00098?ds=SOO-60051-00098-00006&amp;source=SEARCH&amp;sid=6250e0eb050ab5a0&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC3dMFCi0+0h2Q7yp/RTOlffhwMx40T52kBXuWAkJBYDIJpxUsLAohHVwJa3vwtOUsujqrM/mjls6JQDzIHvTluMiB4zoBbkTKkiVxxU6hr74PdxTHKZBV9wukrN4w82/yWp5HoWHuYDNl07Gpt+tmXdtbUEB2KN2y84saGW8FURoFNpMZjfoNazsAekWU+LFfRtd5JisA+krezcArUVhBa3RRAWlR/9fNhebCXAETnnd&amp;cnc=false&amp;pickupPointCode=PP-3126072&amp;pid1=SOO-60051-00098</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>TOT-70382-00006</t>
+          <t>SOO-60051-00356</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Ibu &amp; Anak</t>
+          <t>Fashion Wanita</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Tommee Tippee</t>
+          <t>Sorex</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>TommeeTippee Botol PP Close to Nature Black -  260ML/9oz  - Botol Susu Bayi</t>
+          <t>Sorex CD Wanita Melange Collection 15023 BH 11105, 11106 dan 11115</t>
         </is>
       </c>
       <c r="E28" t="n">
-        <v>107928</v>
+        <v>24990</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium//105/MTA-47575572/tommee-tippee_tommee-tippee_full01.jpg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium//catalog-image/MTA-10634356/sorex_sorex_cd_wanita_melange_collection_15023_bh_11105-_11106_dan_11115_full01_ftwsj520.jpg</t>
         </is>
       </c>
       <c r="G28" t="n">
-        <v>5</v>
+        <v>4.7</v>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/tommeetippee-botol-pp-close-to-nature-black-260ml-9oz-botol-susu-bayi/ps--TOT-70382-00006?ds=TOT-70382-00006-00001&amp;source=SEARCH&amp;sid=e132f3cdc0f57c22&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC0ry844Ce9aEHITmMYpiMq9gT1UYg0nHAvO+SFBeo4zuXqC6GJTmxkMPb5Wt+Q/hMFotyG7K9fuf6GhuhBg1qx5fpZP/HlAo0kBDTb857XQHO00wcIcM43S5kDh1UxrTh35uVJiiuCPRdlV4aliGvlC4/N0ykXdPBQ+Zmpzx07ptQYI2cttpewMJPj5goBPQRx15ZaBw7V58wFuGCPkAmWqPSV/DPGPfxgvN8/0Krqev&amp;cnc=false&amp;pickupPointCode=PP-3527181&amp;pid1=TOT-70382-00006</t>
+          <t>https://www.blibli.com/p/sorex-cd-wanita-melange-collection-15023-bh-11105-11106-dan-11115/ps--SOO-60051-00356?ds=SOO-60051-00356-00002&amp;source=SEARCH&amp;sid=6250e0eb050ab5a0&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC0rd1rndxbAlG8VCZRwhI4b+oLJqLy/XvDHMcpKt+HY6JpxUsLAohHVwJa3vwtOUsujqrM/mjls6JQDzIHvTluMiB4zoBbkTKkiVxxU6hr74PdxTHKZBV9wukrN4w82/yWp5HoWHuYDNl07Gpt+tmXfO/kFtVj4porywlY2UWbf6VMqwppbx5Qk9+27gygWs9lk0gjRbIbx9mhzaC4fFgmtfyUcjpfQtbDHqJqFsTE07&amp;cnc=false&amp;pickupPointCode=PP-3126072&amp;pid1=SOO-60051-00356</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>TOT-70382-00008</t>
+          <t>SOO-60051-00183</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1523,35 +1522,35 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Tommee Tippee</t>
+          <t>Sorex</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>TommeeTippee Botol PP Close to Nature Pink 260ML/9oz - Botol Susu Bayi</t>
+          <t>Sorex Corset ShapeUp Korset Celana Paha Highwaist Shapewear Stagen 13189</t>
         </is>
       </c>
       <c r="E29" t="n">
-        <v>107928</v>
+        <v>93100</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium//108/MTA-47575665/tommee-tippee_tommee-tippee_full01.jpg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/MTA-8072733/sorex_sorex_corset_shapeup_korset_celana_paha_highwaist_shapewear_stagen_13189_full01_j8iugqbd.jpg</t>
         </is>
       </c>
       <c r="G29" t="n">
-        <v>5</v>
+        <v>4.7</v>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/tommeetippee-botol-pp-close-to-nature-pink-260ml-9oz-botol-susu-bayi/ps--TOT-70382-00008?ds=TOT-70382-00008-00001&amp;source=SEARCH&amp;sid=e132f3cdc0f57c22&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC0ry844Ce9aEHITmMYpiMq9gT1UYg0nHAvO+SFBeo4zuvF4GJK6mx13yhfoPe2I6AOWk7L/WjZW4V3T1+QzDEpiZTqX+08YMFPt67oXduO/veDye5g4cJG51p5fjAlqNKr3Qa6Aw9nJN8ZS3vPJl9087KBj1oW91VVdgmsyeMwxAQdi2olXdtgt1P6+kbTziFbtEYHN8Z96N9EmgMub/2Ja79XCc5bYDgXVnw8KN9Bji&amp;cnc=false&amp;pickupPointCode=PP-3527181&amp;pid1=TOT-70382-00008</t>
+          <t>https://www.blibli.com/p/sorex-corset-shapeup-korset-celana-paha-highwaist-shapewear-stagen-13189/ps--SOO-60051-00183?ds=SOO-60051-00183-00002&amp;source=SEARCH&amp;sid=6250e0eb050ab5a0&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC0udwtGfjMBHkzcQHN9WHgcmbE/LLJy7W3VwRB8pUx8xJpxUsLAohHVwJa3vwtOUsujqrM/mjls6JQDzIHvTluMiB4zoBbkTKkiVxxU6hr74PdxTHKZBV9wukrN4w82/yWp5HoWHuYDNl07Gpt+tmXdtbUEB2KN2y84saGW8FURoFNpMZjfoNazsAekWU+LFfVvw+oDo6sSWOOV3QxYLnzVfyUcjpfQtbDHqJqFsTE07&amp;cnc=false&amp;pickupPointCode=PP-3126072&amp;pid1=SOO-60051-00183</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>TOT-70382-00009</t>
+          <t>SOO-60051-00157</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1561,446 +1560,446 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Tommee Tippee</t>
+          <t>Sorex</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>TommeeTippee Botol PP Close to Nature Lime Green-  260ML/9oz  - Botol Susu Bayi</t>
+          <t>Sorex Corset Shapewear Korset Tulang Reguler Size Stagen 1052 Pengecil Perut</t>
         </is>
       </c>
       <c r="E30" t="n">
-        <v>122918</v>
+        <v>78400</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium//111/MTA-47575965/tommee-tippee_tommee-tippee_full01.jpg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/MTA-7975883/sorex_sorex_corset_shapewear_korset_tulang_reguler_size_stagen_1052_pengecil_perut_full01_q5k3eby6.jpg</t>
         </is>
       </c>
       <c r="G30" t="n">
-        <v>5</v>
+        <v>4.7</v>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/tommeetippee-botol-pp-close-to-nature-lime-green-260ml-9oz-botol-susu-bayi/ps--TOT-70382-00009?ds=TOT-70382-00009-00001&amp;source=SEARCH&amp;sid=e132f3cdc0f57c22&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC2QNmx+r+f1ujpt2oEeckeC0lBlb77cMs6jcxr+f+IK39JvkEqCAqa4feXKpvDGvZla8f1JvScJ6DrHwqmhDSmJ38pLvQtrJkjvO7Vji06N5Y/z3GNGYn0VDwoIIPnDgZ5AnoLYwmKE1R7OS9+9VGfqViJT0I/qzo1dSRzxYbUZ/DGAybPeyfXm8q+SIgg++Ls1UV1sbzkIRtS1HuTjW8OB0cwAv5tbcj9Ui2cthtuZZ&amp;cnc=false&amp;pickupPointCode=PP-3527181&amp;pid1=TOT-70382-00009</t>
+          <t>https://www.blibli.com/p/sorex-corset-shapewear-korset-tulang-reguler-size-stagen-1052-pengecil-perut/ps--SOO-60051-00157?ds=SOO-60051-00157-00001&amp;source=SEARCH&amp;sid=6250e0eb050ab5a0&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC1v82AvnOYi0a9q7D8u1KCCX0LAHVJZ7EB+ox4oiZlNaJpxUsLAohHVwJa3vwtOUsujqrM/mjls6JQDzIHvTluMiB4zoBbkTKkiVxxU6hr74PdxTHKZBV9wukrN4w82/yWp5HoWHuYDNl07Gpt+tmXdtbUEB2KN2y84saGW8FURoFNpMZjfoNazsAekWU+LFfVvw+oDo6sSWOOV3QxYLnzVfyUcjpfQtbDHqJqFsTE07&amp;cnc=false&amp;pickupPointCode=PP-3126072&amp;pid1=SOO-60051-00157</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>PIB-70060-00154</t>
+          <t>LAB-70212-05594</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Ibu &amp; Anak</t>
+          <t>Fashion Wanita</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Pigeon</t>
+          <t>no brand</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Pigeon Botol PP Wide Neck with P-Plus Nipple Botol Susu [240 mL] PR010318</t>
+          <t>Sorex Busa Tipis Cantik Motif Kait Bh 3 Bunga Menyusui 8110, Ukuran Bra 40/90</t>
         </is>
       </c>
       <c r="E31" t="n">
-        <v>99600</v>
+        <v>35500</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium//catalog-image/99/MTA-118819143/pigeon_pigeon_botol_pp_wide_neck_with_p-plus_nipple_botol_susu_-240_ml-_pr010318_full05_h20sx2k.jpg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/109/MTA-165769470/brd-44261_sorex-busa-tipis-cantik-motif-kait-bh-3-bunga-menyusui-8110-ukuran-bra-40-90_full01-857c7e11.jpg</t>
         </is>
       </c>
       <c r="G31" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/pigeon-botol-pp-wide-neck-with-p-plus-nipple-botol-susu-240-ml-pr010318/ps--PIB-70060-00154?ds=PIB-70060-00154-00001&amp;source=SEARCH&amp;sid=e132f3cdc0f57c22&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC2XuNNHwI4Wu2llNpf1IcHxnh6wQ6PEr8y5kW/jpBoqadAnVTXMTPyuU5CGuMSVWXVesavfRnEsmWNUn9y9IGTPNbQv3e9jt8aL3d1v2xu9D3zP/3jXSVAsNO6CVkKiBbHhwvx3ifXg1BsOX37zBUHJdqJUNsHaqc/xrX/8eUT87D9X7JvQu62DvXKUCWSGFikKVlKV88zLDyNjH30/J/VI=&amp;cnc=false&amp;pickupPointCode=PP-3491245&amp;pid1=PIB-70060-00154</t>
+          <t>https://www.blibli.com/p/sorex-busa-tipis-cantik-motif-kait-bh-3-bunga-menyusui-8110-ukuran-bra-40-90/ps--LAB-70212-05594?ds=LAB-70212-05594-00003&amp;source=SEARCH&amp;sid=6250e0eb050ab5a0&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC7uWdf8oWYVqFa8kN7IOdiG/HAkxoVke7cxJ4LyInlLeCehKQbsgVGraUizdU4xFCnHOL7ft1r2B8la4jhSYbiSNDYUCs2SDfIC9YxZFA4sR5e7y1I67HStc8otBBiK5XJSts5Ttmig5MtQNiW9Bh+kRCVEuomQmWAa8P70g52bCaki4eOIxBkoZxlgI0gvu5v0lswRRcaDx8z50fOWMvOhM2TuCGo9wlT4OmaRfcPlvMg5yN2tby8UNstwdND2jMw==&amp;cnc=false&amp;pickupPointCode=PP-3499445&amp;pid1=LAB-70212-05594</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>TOT-70382-00003</t>
+          <t>SOO-60051-00497</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Ibu &amp; Anak</t>
+          <t>Fashion Wanita</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Tommee Tippee</t>
+          <t>Sorex</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>TommeeTippee Botol PP Close to Nature Clear 260ML/9oz- isi 2 - Botol Susu Bayi</t>
+          <t>Sorex Mystery Box Special Bra Cantik Kawat/Tanpa Kawat Setara cup B</t>
         </is>
       </c>
       <c r="E32" t="n">
-        <v>176328</v>
+        <v>58800</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium//101/MTA-47575235/tommee-tippee_tommee-tippee_full01.jpg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium//97/MTA-13765543/sorex_sorex_mystery_box_special_bra_cantik_kawat-tanpa_kawat__setara_cup_b_full03_h94hmgrl.jpg</t>
         </is>
       </c>
       <c r="G32" t="n">
-        <v>5</v>
+        <v>4.6</v>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/tommeetippee-botol-pp-close-to-nature-clear-260ml-9oz-isi-2-botol-susu-bayi/ps--TOT-70382-00003?ds=TOT-70382-00003-00001&amp;source=SEARCH&amp;sid=e132f3cdc0f57c22&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC1ifcoeXCfsl309abOwHy+UyRx2NB90AvgZAzR/Au2fsa6jWV42laeO3V9LtJs1QYOWk7L/WjZW4V3T1+QzDEpiZTqX+08YMFPt67oXduO/veDye5g4cJG51p5fjAlqNKr3Qa6Aw9nJN8ZS3vPJl9087KBj1oW91VVdgmsyeMwxAQdi2olXdtgt1P6+kbTziFbtEYHN8Z96N9EmgMub/2Ja79XCc5bYDgXVnw8KN9Bji&amp;cnc=false&amp;pickupPointCode=PP-3527181&amp;pid1=TOT-70382-00003</t>
+          <t>https://www.blibli.com/p/sorex-mystery-box-special-bra-cantik-kawat-tanpa-kawat-setara-cup-b/ps--SOO-60051-00497?ds=SOO-60051-00497-00002&amp;source=SEARCH&amp;sid=6250e0eb050ab5a0&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC0Io8iY7bS3QFgUrrRjl8b9l2MnZWZ1TwAwuODpbBDUVJpxUsLAohHVwJa3vwtOUsujqrM/mjls6JQDzIHvTluMiB4zoBbkTKkiVxxU6hr74PdxTHKZBV9wukrN4w82/yWp5HoWHuYDNl07Gpt+tmXfO/kFtVj4porywlY2UWbf6VMqwppbx5Qk9+27gygWs9sZi4HFMNt1hNudy6hVQGo9fyUcjpfQtbDHqJqFsTE07&amp;cnc=false&amp;pickupPointCode=PP-3126072&amp;pid1=SOO-60051-00497</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>TOT-70382-00019</t>
+          <t>SOO-60051-00280</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Ibu &amp; Anak</t>
+          <t>Fashion Wanita</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Tommee Tippee</t>
+          <t>Sorex</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>TommeeTippee Botol PP Close to Nature Blue 260ML/9oz - isi 2 - Botol Susu Bayi</t>
+          <t>Sorex Lingerie Lovely Series Baju Tidur Premium Satin Look Cute Ribbon Brukat Bunga BT 7002</t>
         </is>
       </c>
       <c r="E33" t="n">
-        <v>203920</v>
+        <v>102312</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium//104/MTA-47576803/tommee-tippee_tommee-tippee_full01.jpg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium//97/MTA-8395621/sorex_sorex_lingerie_baju_tidur_premium_satin_look_cute_ribbon_brukat_bunga_bt_7002_full01_pbu0j5i7.jpg</t>
         </is>
       </c>
       <c r="G33" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/tommeetippee-botol-pp-close-to-nature-blue-260ml-9oz-isi-2-botol-susu-bayi/ps--TOT-70382-00019?ds=TOT-70382-00019-00001&amp;source=SEARCH&amp;sid=e132f3cdc0f57c22&amp;metaData=SnHZRCX7NPLsJ+ExPEFNCxzohPZzaxyiJv5ug5c6gt1tsXYn3L1ksKYsCVRC7VEtRgjclo41Bv7m06q1VtnIFla8f1JvScJ6DrHwqmhDSmJ38pLvQtrJkjvO7Vji06N5Y/z3GNGYn0VDwoIIPnDgZ5AnoLYwmKE1R7OS9+9VGfqViJT0I/qzo1dSRzxYbUZ/DGAybPeyfXm8q+SIgg++Ls1UV1sbzkIRtS1HuTjW8OB0cwAv5tbcj9Ui2cthtuZZ&amp;cnc=false&amp;pickupPointCode=PP-3527181&amp;pid1=TOT-70382-00019</t>
+          <t>https://www.blibli.com/p/sorex-lingerie-lovely-series-baju-tidur-premium-satin-look-cute-ribbon-brukat-bunga-bt-7002/ps--SOO-60051-00280?ds=SOO-60051-00280-00003&amp;source=SEARCH&amp;sid=6250e0eb050ab5a0&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC0ry844Ce9aEHITmMYpiMq9e2UdUDLB5ofwWKbsz373iU+qNVzNAHCfEDldNFubAdFesavfRnEsmWNUn9y9IGTPNbQv3e9jt8aL3d1v2xu9D3zP/3jXSVAsNO6CVkKiBbHhwvx3ifXg1BsOX37zBUHLC06X8BZfWbuoyV1i+FIvCFi5ZGHXfeZdV+lqHHsOV+PA0N+dYDXaG8wXNJPvVud60XBPM8Ib69hRyb0y0TLR/&amp;cnc=false&amp;pickupPointCode=PP-3126072&amp;pid1=SOO-60051-00280</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>PIB-70060-00096</t>
+          <t>SOO-60051-01066</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Ibu &amp; Anak</t>
+          <t>Fashion Wanita</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Pigeon</t>
+          <t>Sorex</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Pigeon PR010807 PP Clear Streamline with S-Type Nipple Size M Botol Susu [250 mL]</t>
+          <t>Sorex Bra Tanpa Kawat Cup B Busa Sedang Cup 3/4 Nilon Bra Harian BH 33506</t>
         </is>
       </c>
       <c r="E34" t="n">
-        <v>53618</v>
+        <v>41200</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium//catalog-image/105/MTA-118811895/pigeon_pigeon_pr010807_pp_clear_streamline_with_s-type_nipple_size_m_botol_susu_-250_ml-_full11_cfbxgswr.jpg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/106/MTA-166158385/sorex_sorex_bra_tanpa_kawat_cup_b_busa_sedang_cup_3-4_nilon_bra_harian_bh_33506_full02_u8si6sir.jpg</t>
         </is>
       </c>
       <c r="G34" t="n">
-        <v>4.8</v>
+        <v>0</v>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/pigeon-pr010807-pp-clear-streamline-with-s-type-nipple-size-m-botol-susu-250-ml/ps--PIB-70060-00096?ds=PIB-70060-00096-00002&amp;source=SEARCH&amp;sid=e132f3cdc0f57c22&amp;metaData=SnHZRCX7NPLsJ+ExPEFNCxaO742P7KkmPAljo7+jfY/7bP+X+ATPnCC1i/iQNMrmJpxUsLAohHVwJa3vwtOUsujqrM/mjls6JQDzIHvTluMiB4zoBbkTKkiVxxU6hr74PdxTHKZBV9wukrN4w82/yWp5HoWHuYDNl07Gpt+tmXfUPfTcRHuI1P2DR2vMpEYmN4q/YrhOrAyjv307X3FLxrTAREenyKb84DVg8LJlYzA=&amp;cnc=false&amp;pickupPointCode=PP-3491245&amp;pid1=PIB-70060-00096</t>
+          <t>https://www.blibli.com/p/sorex-bra-tanpa-kawat-cup-b-busa-sedang-cup-3-4-nilon-bra-harian-bh-33506/ps--SOO-60051-01066?ds=SOO-60051-01066-00002&amp;source=SEARCH&amp;sid=6250e0eb050ab5a0&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC5nGzsCVntCT1sSfFwqgrxjG7ZKryzxMhLfm5+J6+v8bJpxUsLAohHVwJa3vwtOUsujqrM/mjls6JQDzIHvTluMiB4zoBbkTKkiVxxU6hr74PdxTHKZBV9wukrN4w82/yWp5HoWHuYDNl07Gpt+tmXfO/kFtVj4porywlY2UWbf6VMqwppbx5Qk9+27gygWs9sZi4HFMNt1hNudy6hVQGo9fyUcjpfQtbDHqJqFsTE07&amp;cnc=false&amp;pickupPointCode=PP-3126072&amp;pid1=SOO-60051-01066</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>PIB-70060-00065</t>
+          <t>SOO-60051-01064</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Ibu &amp; Anak</t>
+          <t>Fashion Wanita</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Pigeon</t>
+          <t>Sorex</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Pigeon PR010399 BTL PP Wide Neck W-P-PLUS Nipple Botol Susu - Purple [330 mL]</t>
+          <t>(PILIH WARNA) Sorex Celana Dalam Wanita Basic Midi Nara Super Soft CD OF 003</t>
         </is>
       </c>
       <c r="E35" t="n">
-        <v>103916</v>
+        <v>25800</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium//catalog-image/101/MTA-118801459/pigeon_pigeon_pr010399_btl_pp_wide_neck_w-p-plus_nipple_botol_susu_-_purple_-330_ml-_full05_84io0na.jpg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/94/MTA-166085102/sorex_-pilih_warna-_sorex_celana_dalam_wanita_basic_midi_nara_super_soft_cd_of_003_full04_kk9iitlq.jpg</t>
         </is>
       </c>
       <c r="G35" t="n">
-        <v>4.7</v>
+        <v>0</v>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/pigeon-pr010399-btl-pp-wide-neck-w-p-plus-nipple-botol-susu-purple-330-ml/ps--PIB-70060-00065?ds=PIB-70060-00065-00001&amp;source=SEARCH&amp;sid=e132f3cdc0f57c22&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC0ry844Ce9aEHITmMYpiMq+nXPZ3fvtXLkonE4D380C6U+qNVzNAHCfEDldNFubAdFesavfRnEsmWNUn9y9IGTPNbQv3e9jt8aL3d1v2xu9D3zP/3jXSVAsNO6CVkKiBbHhwvx3ifXg1BsOX37zBUHJdqJUNsHaqc/xrX/8eUT87D9X7JvQu62DvXKUCWSGFikKVlKV88zLDyNjH30/J/VI=&amp;cnc=false&amp;pickupPointCode=PP-3491245&amp;pid1=PIB-70060-00065</t>
+          <t>https://www.blibli.com/p/pilih-warna-sorex-celana-dalam-wanita-basic-midi-nara-super-soft-cd-of-003/ps--SOO-60051-01064?ds=SOO-60051-01064-00002&amp;source=SEARCH&amp;sid=6250e0eb050ab5a0&amp;metaData=SnHZRCX7NPLsJ+ExPEFNCzO4NENA+D3a2b160XD/ATBl2MnZWZ1TwAwuODpbBDUVJpxUsLAohHVwJa3vwtOUsujqrM/mjls6JQDzIHvTluMiB4zoBbkTKkiVxxU6hr74PdxTHKZBV9wukrN4w82/yWp5HoWHuYDNl07Gpt+tmXfO/kFtVj4porywlY2UWbf6VMqwppbx5Qk9+27gygWs9lk0gjRbIbx9mhzaC4fFgmtfyUcjpfQtbDHqJqFsTE07&amp;cnc=false&amp;pickupPointCode=PP-3126072&amp;pid1=SOO-60051-01064</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>PIB-70060-00256</t>
+          <t>SOO-60051-01063</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Ibu &amp; Anak</t>
+          <t>Fashion Wanita</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Pigeon</t>
+          <t>Sorex</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Pigeon PR010111 Wide Neck Botol Susu with P-Plus Nipple - White [160 mL]</t>
+          <t>(PILIH WARNA) Sorex Celana Dalam Wanita Basic Midi Comfort Yori Katun Mix CD OF 002</t>
         </is>
       </c>
       <c r="E36" t="n">
-        <v>157617</v>
+        <v>29400</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium//catalog-image/101/MTA-118844246/pigeon_pigeon-pr010111-wide-neck-botol-susu-with-p-plus-nipple---white--160-ml-_full03.jpg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/111/MTA-166084778/sorex_sorex_celana_dalam_wanita_basic_midi_comfort_yori_katun_mix_cd_of_002_full03_uugzz21e.jpg</t>
         </is>
       </c>
       <c r="G36" t="n">
-        <v>4.7</v>
+        <v>0</v>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/pigeon-pr010111-wide-neck-botol-susu-with-p-plus-nipple-white-160-ml/ps--PIB-70060-00256?ds=PIB-70060-00256-00001&amp;source=SEARCH&amp;sid=e132f3cdc0f57c22&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC9tiwxYVs41tNENObWAga5H6p8GGLNysbH/ekoSRyKYQU+qNVzNAHCfEDldNFubAdFesavfRnEsmWNUn9y9IGTPNbQv3e9jt8aL3d1v2xu9D3zP/3jXSVAsNO6CVkKiBbHhwvx3ifXg1BsOX37zBUHJdqJUNsHaqc/xrX/8eUT87D9X7JvQu62DvXKUCWSGFikKVlKV88zLDyNjH30/J/VI=&amp;cnc=false&amp;pickupPointCode=PP-3491245&amp;pid1=PIB-70060-00256</t>
+          <t>https://www.blibli.com/p/pilih-warna-sorex-celana-dalam-wanita-basic-midi-comfort-yori-katun-mix-cd-of-002/ps--SOO-60051-01063?ds=SOO-60051-01063-00018&amp;source=SEARCH&amp;sid=6250e0eb050ab5a0&amp;metaData=SnHZRCX7NPLsJ+ExPEFNCwIcYjJhUkfzuki5iW9SKA+X0LAHVJZ7EB+ox4oiZlNaJpxUsLAohHVwJa3vwtOUsujqrM/mjls6JQDzIHvTluMiB4zoBbkTKkiVxxU6hr74PdxTHKZBV9wukrN4w82/yWp5HoWHuYDNl07Gpt+tmXfO/kFtVj4porywlY2UWbf6VMqwppbx5Qk9+27gygWs9lk0gjRbIbx9mhzaC4fFgmtfyUcjpfQtbDHqJqFsTE07&amp;cnc=false&amp;pickupPointCode=PP-3126072&amp;pid1=SOO-60051-01063</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>SUB-70131-00001</t>
+          <t>LAB-70212-05592</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Bliblimart</t>
+          <t>Fashion Wanita</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>V-SOY</t>
+          <t>no brand</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>V-Soy Soya Bean Milk Multi-Grain 200 mL</t>
+          <t>Sorex Busa Tipis Cantik Motif Kait Bh 3 Bunga Menyusui 8110, Ukuran Bra 38/85</t>
         </is>
       </c>
       <c r="E37" t="n">
-        <v>7600</v>
+        <v>35500</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium//97/MTA-37181572/v-soy_v-soy-multi-grain-soya-bean-milk--200-ml-_full54.jpg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/116/MTA-165769469/brd-44261_sorex-busa-tipis-cantik-motif-kait-bh-3-bunga-menyusui-8110-ukuran-bra-38-85_full01-fb7fdff3.jpg</t>
         </is>
       </c>
       <c r="G37" t="n">
-        <v>4.9</v>
+        <v>0</v>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/v-soy-soya-bean-milk-multi-grain-200-ml/ps--SUB-70131-00001?ds=SUB-70131-00001-00001&amp;source=SEARCH&amp;sid=e132f3cdc0f57c22&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC3iBiFb6oLnHLQNEBDHZ7zi3VQ2WlzHp9deWrxqynfgSWu0SW4+dXt77eUDTP9Ij0lX6YqNL/N38iJlYkQlI2HD9cnB7A9Br96VNOoae/H1+BSFd02BuHmZWh0L7R6dhksB+tPNv9ITp+8ttAFmGt53nU4Dp3uhlwixflscAf8XVNd9Qdrb3QWYxenklePSJm2YIMI0lPmD6FoI5NoCioInltUNk96VTdqdjG4caO5Q1wCaCWmOutPc0eIowrS/xtVANmgzGmpkcTWih3zwHJGFy2lQHLum2Le2M2zPi58xKW3JybDOOru79yMazz2iAGV/JRyOl9C1sMeomoWxMTTs=&amp;cnc=false&amp;pickupPointCode=PP-3309290&amp;pid1=SUB-70131-00001</t>
+          <t>https://www.blibli.com/p/sorex-busa-tipis-cantik-motif-kait-bh-3-bunga-menyusui-8110-ukuran-bra-38-85/ps--LAB-70212-05592?ds=LAB-70212-05592-00001&amp;source=SEARCH&amp;sid=6250e0eb050ab5a0&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC7uWdf8oWYVqFa8kN7IOdiG/HAkxoVke7cxJ4LyInlLeCehKQbsgVGraUizdU4xFCnHOL7ft1r2B8la4jhSYbiSNDYUCs2SDfIC9YxZFA4sR5e7y1I67HStc8otBBiK5XJSts5Ttmig5MtQNiW9Bh+kRCVEuomQmWAa8P70g52bCaki4eOIxBkoZxlgI0gvu5v0lswRRcaDx8z50fOWMvOhM2TuCGo9wlT4OmaRfcPlvMg5yN2tby8UNstwdND2jMw==&amp;cnc=false&amp;pickupPointCode=PP-3499445&amp;pid1=LAB-70212-05592</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>MIU-60035-00479</t>
+          <t>BAG-70027-00459</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Bliblimart</t>
+          <t>Ibu &amp; Anak</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>MilkLife</t>
+          <t>Sorex</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>WHS - SMG/JOG/SOLO -MilkLife UHT Chocolate Milk - Susu Cokelat 1 liter</t>
+          <t>Handuk Bayi | Handuk Anak | Sorex Towel 100 X 50</t>
         </is>
       </c>
       <c r="E38" t="n">
-        <v>19000</v>
+        <v>69400</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/100/MTA-166162608/milklife_smg-jog-solo_-_milklife_uht_chocolate_milk_-_susu_cokelat_1_liter__full01_vu4ouru7.jpg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium//78/MTA-11021170/sorex_handuk_bayi_-_handuk_anak_-_sorex_towel_100_x_50_-_full01_3d2184d8.jpg</t>
         </is>
       </c>
       <c r="G38" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/whs-smg-jog-solo-milklife-uht-chocolate-milk-susu-cokelat-1-liter/ps--MIU-60035-00479?ds=MIU-60035-00479-00001&amp;source=SEARCH&amp;sid=e132f3cdc0f57c22&amp;metaData=SnHZRCX7NPLsJ+ExPEFNCyyDdutSjnAKjW/qtRSWe1KT2r7fOYNS0fn24lYkspaBKJn9h4w27QeeplXx/bodWejqrM/mjls6JQDzIHvTluMiB4zoBbkTKkiVxxU6hr74PdxTHKZBV9wukrN4w82/yWp5HoWHuYDNl07Gpt+tmXeDioWrdqW2jVDexSAU462NTDhvU2dGTHXFRrWe7cayKPgUkBrNSd1kvoEoL27Ax4FfyUcjpfQtbDHqJqFsTE07&amp;cnc=false&amp;pickupPointCode=PP-3528657&amp;pid1=MIU-60035-00479</t>
+          <t>https://www.blibli.com/p/handuk-bayi-handuk-anak-sorex-towel-100-x-50/ps--BAG-70027-00459?ds=BAG-70027-00459-00001&amp;source=SEARCH&amp;sid=6250e0eb050ab5a0&amp;metaData=SnHZRCX7NPLsJ+ExPEFNCwNduFYwfvFwnmds8RU/70OX0LAHVJZ7EB+ox4oiZlNaEg3X3jytsJx+M8M3Wz5HMejqrM/mjls6JQDzIHvTluMiB4zoBbkTKkiVxxU6hr74PdxTHKZBV9wukrN4w82/yWp5HoWHuYDNl07Gpt+tmXfUPfTcRHuI1P2DR2vMpEYmDdmyk291xKlcwhaoJiafSwI6rvWM2fME09xrH8SZaRY=&amp;cnc=false&amp;pickupPointCode=PP-3172350&amp;pid1=BAG-70027-00459</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>PIB-70060-00112</t>
+          <t>SOO-60051-01061</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Ibu &amp; Anak</t>
+          <t>Fashion Wanita</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Pigeon</t>
+          <t>Sorex</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Pigeon Training Toothbrush Lesson 2 Orange</t>
+          <t>Sorex Bra Tanpa Kawat Full Cup B Busa Sedang Kait 3 Nilon Mix Bra Harian BH 34235</t>
         </is>
       </c>
       <c r="E39" t="n">
-        <v>27823</v>
+        <v>85000</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium//catalog-image/109/MTA-118811998/pigeon_pigeon_full01.jpg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/105/MTA-165480746/sorex_sorex_bra_tanpa_kawat_full_cup_b_busa_sedang_kait_3_nilon_mix_bra_harian_bh_34235_full02_usrhnjca.jpg</t>
         </is>
       </c>
       <c r="G39" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/pigeon-training-toothbrush-lesson-2-orange/ps--PIB-70060-00112?ds=PIB-70060-00112-00001&amp;source=SEARCH&amp;sid=e132f3cdc0f57c22&amp;metaData=SnHZRCX7NPLsJ+ExPEFNCwXkXh0R7dL5+fNlrKiyDwx0O+Xum4AbLEfftyx0BpG8CehKQbsgVGraUizdU4xFCnHOL7ft1r2B8la4jhSYbiSNDYUCs2SDfIC9YxZFA4sR5e7y1I67HStc8otBBiK5XJSts5Ttmig5MtQNiW9Bh+kRCVEuomQmWAa8P70g52bCzk7fy2rvv+ow0YbqKM95HqQMXWaXOtSuMstJ6IABr+yVoV04qa0eYQjwc63Ch+ZJt30CNpx08CSls6cI1xwZCWWiZ0O2Mr8xqHu5eFiAfS8ZznBLAQ2nP1eCjEfaGKnbecIPcotNC9ds+ZQfRejTug==&amp;cnc=false&amp;pickupPointCode=PP-3491245&amp;pid1=PIB-70060-00112</t>
+          <t>https://www.blibli.com/p/sorex-bra-tanpa-kawat-full-cup-b-busa-sedang-kait-3-nilon-mix-bra-harian-bh-34235/ps--SOO-60051-01061?ds=SOO-60051-01061-00005&amp;source=SEARCH&amp;sid=6250e0eb050ab5a0&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC4jqhVUYBGnRHB2dDFMPniyT2r7fOYNS0fn24lYkspaBJpxUsLAohHVwJa3vwtOUsujqrM/mjls6JQDzIHvTluMiB4zoBbkTKkiVxxU6hr74PdxTHKZBV9wukrN4w82/yWp5HoWHuYDNl07Gpt+tmXfO/kFtVj4porywlY2UWbf6VMqwppbx5Qk9+27gygWs9sZi4HFMNt1hNudy6hVQGo9fyUcjpfQtbDHqJqFsTE07&amp;cnc=false&amp;pickupPointCode=PP-3126072&amp;pid1=SOO-60051-01061</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>PIB-70060-00111</t>
+          <t>SOO-60051-00825</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Ibu &amp; Anak</t>
+          <t>Fashion Wanita</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Pigeon</t>
+          <t>Sorex</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Pigeon Training Toothbrush Lesson 3 Pink</t>
+          <t>Sorex CD Seamless Cutting Midi Extra Size L-XL Anti Nyeplak Tanpa Jahitan EA 510</t>
         </is>
       </c>
       <c r="E40" t="n">
-        <v>44381</v>
+        <v>33000</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium//catalog-image/106/MTA-118811995/pigeon_pigeon_full01.jpg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/MTA-70468312/sorex_sorex_cd_seamless_cutting_midi_extra_size_jumbo_anti_nyeplak_tanpa_jahitan_ea_510_full01_tw5up5u7.jpg</t>
         </is>
       </c>
       <c r="G40" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/pigeon-training-toothbrush-lesson-3-pink/ps--PIB-70060-00111?ds=PIB-70060-00111-00001&amp;source=SEARCH&amp;sid=e132f3cdc0f57c22&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC/yWWkfvbmGmkfSwUzmXNKOo4B78dMCZh3/QzUsVUDMFCehKQbsgVGraUizdU4xFCnHOL7ft1r2B8la4jhSYbiSNDYUCs2SDfIC9YxZFA4sR5e7y1I67HStc8otBBiK5XJSts5Ttmig5MtQNiW9Bh+kRCVEuomQmWAa8P70g52bCzk7fy2rvv+ow0YbqKM95HqQMXWaXOtSuMstJ6IABr+yVoV04qa0eYQjwc63Ch+ZJt30CNpx08CSls6cI1xwZCWWiZ0O2Mr8xqHu5eFiAfS8ZznBLAQ2nP1eCjEfaGKnbecIPcotNC9ds+ZQfRejTug==&amp;cnc=false&amp;pickupPointCode=PP-3491245&amp;pid1=PIB-70060-00111</t>
+          <t>https://www.blibli.com/p/sorex-cd-seamless-cutting-midi-extra-size-l-xl-anti-nyeplak-tanpa-jahitan-ea-510/ps--SOO-60051-00825?ds=SOO-60051-00825-00011&amp;source=SEARCH&amp;sid=6250e0eb050ab5a0&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC8ZIN0KweYTfTnX/ul7fF5GT2r7fOYNS0fn24lYkspaBJpxUsLAohHVwJa3vwtOUsujqrM/mjls6JQDzIHvTluMiB4zoBbkTKkiVxxU6hr74PdxTHKZBV9wukrN4w82/yWp5HoWHuYDNl07Gpt+tmXfO/kFtVj4porywlY2UWbf6VMqwppbx5Qk9+27gygWs9lk0gjRbIbx9mhzaC4fFgmtfyUcjpfQtbDHqJqFsTE07&amp;cnc=false&amp;pickupPointCode=PP-3126072&amp;pid1=SOO-60051-00825</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>PIB-70060-00114</t>
+          <t>SOO-60051-01059</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Ibu &amp; Anak</t>
+          <t>Fashion Wanita</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Pigeon</t>
+          <t>Sorex</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Pigeon Training Toothbrush Lesson 3 Blue</t>
+          <t>Sorex Invisible Bra Busa Sedang Tanpa Kawat Kait 1 Nilon Seamless Cup B 3/4 BH 34239</t>
         </is>
       </c>
       <c r="E41" t="n">
-        <v>44381</v>
+        <v>71600</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium//catalog-image/94/MTA-118812008/pigeon_pigeon_full01.jpg</t>
+          <t>https://www.static-src.com/wcsstore/Indraprastha/images/catalog/medium/catalog-image/94/MTA-165474112/sorex_sorex_invisible_bra_busa_sedang_tanpa_kawat_kait_1_nilon_seamless_cup_b_3-4_bh_34239_full02_e7q9oqh8.jpg</t>
         </is>
       </c>
       <c r="G41" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>https://www.blibli.com/p/pigeon-training-toothbrush-lesson-3-blue/ps--PIB-70060-00114?ds=PIB-70060-00114-00001&amp;source=SEARCH&amp;sid=e132f3cdc0f57c22&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC/yWWkfvbmGmkfSwUzmXNKOo4B78dMCZh3/QzUsVUDMFCehKQbsgVGraUizdU4xFCnHOL7ft1r2B8la4jhSYbiSNDYUCs2SDfIC9YxZFA4sR5e7y1I67HStc8otBBiK5XJSts5Ttmig5MtQNiW9Bh+kRCVEuomQmWAa8P70g52bCzk7fy2rvv+ow0YbqKM95HqQMXWaXOtSuMstJ6IABr+yVoV04qa0eYQjwc63Ch+ZJt30CNpx08CSls6cI1xwZCWWiZ0O2Mr8xqHu5eFiAfS8ZznBLAQ2nP1eCjEfaGKnbecIPcotNC9ds+ZQfRejTug==&amp;cnc=false&amp;pickupPointCode=PP-3528888&amp;pid1=PIB-70060-00114</t>
+          <t>https://www.blibli.com/p/sorex-invisible-bra-busa-sedang-tanpa-kawat-kait-1-nilon-seamless-cup-b-3-4-bh-34239/ps--SOO-60051-01059?ds=SOO-60051-01059-00001&amp;source=SEARCH&amp;sid=6250e0eb050ab5a0&amp;metaData=SnHZRCX7NPLsJ+ExPEFNC6RXpYt557pWi7AhEmIfSHVnh6wQ6PEr8y5kW/jpBoqaJpxUsLAohHVwJa3vwtOUsujqrM/mjls6JQDzIHvTluMiB4zoBbkTKkiVxxU6hr74PdxTHKZBV9wukrN4w82/yWp5HoWHuYDNl07Gpt+tmXfO/kFtVj4porywlY2UWbf6VMqwppbx5Qk9+27gygWs9sZi4HFMNt1hNudy6hVQGo9fyUcjpfQtbDHqJqFsTE07&amp;cnc=false&amp;pickupPointCode=PP-3126072&amp;pid1=SOO-60051-01059</t>
         </is>
       </c>
     </row>

</xml_diff>